<commit_message>
updating platform version through excel
</commit_message>
<xml_diff>
--- a/src/test/resources/DataSet/NMCO_ONB.xlsx
+++ b/src/test/resources/DataSet/NMCO_ONB.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="TestData" sheetId="1" state="visible" r:id="rId2"/>
@@ -1223,10 +1223,10 @@
     <t xml:space="preserve">9.0.0</t>
   </si>
   <si>
+    <t xml:space="preserve">LENOVO_M10Plus_Android_10.0.0_2ba36</t>
+  </si>
+  <si>
     <t xml:space="preserve">SAMSUNG_GalaxyTabS6_Android_9.0.0_16c48</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LENOVO_M10Plus_Android_10.0.0_2ba36</t>
   </si>
   <si>
     <t xml:space="preserve">SAMSUNG_GalaxyTabS4_Android_10.0.0_2133b</t>
@@ -1341,10 +1341,10 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color rgb="FF6A8759"/>
-      <name val="JetBrains Mono"/>
-      <family val="3"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -1649,7 +1649,7 @@
   </sheetPr>
   <dimension ref="A1:AMJ248"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="0" topLeftCell="K1" activePane="topRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="M9" activeCellId="0" sqref="M9"/>
@@ -20475,12 +20475,12 @@
   </sheetPr>
   <dimension ref="A1:S13"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="D1" activeCellId="0" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I5" activeCellId="0" sqref="I5"/>
+      <selection pane="bottomRight" activeCell="I6" activeCellId="0" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -20720,7 +20720,7 @@
       <c r="H5" s="8" t="s">
         <v>396</v>
       </c>
-      <c r="I5" s="33" t="s">
+      <c r="I5" s="30" t="s">
         <v>397</v>
       </c>
       <c r="J5" s="8" t="s">
@@ -20747,7 +20747,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="44" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="44.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="8" t="s">
         <v>398</v>
       </c>
@@ -20772,7 +20772,7 @@
       <c r="H6" s="8" t="s">
         <v>399</v>
       </c>
-      <c r="I6" s="30" t="s">
+      <c r="I6" s="33" t="s">
         <v>400</v>
       </c>
       <c r="J6" s="8" t="s">
@@ -20811,7 +20811,7 @@
         <v>399</v>
       </c>
       <c r="I7" s="30" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="J7" s="8"/>
       <c r="K7" s="30"/>
@@ -20824,7 +20824,7 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="I8" s="0" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
adding test runner and testnd.xml file
</commit_message>
<xml_diff>
--- a/src/test/resources/DataSet/NMCO_ONB.xlsx
+++ b/src/test/resources/DataSet/NMCO_ONB.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2662" uniqueCount="403">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2676" uniqueCount="404">
   <si>
     <t xml:space="preserve">TestCaseName</t>
   </si>
@@ -1193,40 +1193,43 @@
     <t xml:space="preserve">bkx8w6zydrxh6kj7xxw5t4kr</t>
   </si>
   <si>
+    <t xml:space="preserve">9.0.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SAMSUNG_GalaxyTabS6_Android_9.0.0_16c48</t>
+  </si>
+  <si>
+    <t xml:space="preserve">uiautomator2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">app-debugOct11.apk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://device.pcloudy.com/appiumcloud/wd/hub</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Android_002</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.0.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SAMSUNG_GalaxyTabS5e_Android_10.0.0_cb1ca</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Android_003</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LENOVO_M10Plus_Android_10.0.0_2ba36</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Android_0003</t>
+  </si>
+  <si>
     <t xml:space="preserve">11.0.0</t>
   </si>
   <si>
     <t xml:space="preserve">SAMSUNG_GalaxyTabS6_Android_11.0.0_383e3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">uiautomator2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">app-debugOct11.apk</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://device.pcloudy.com/appiumcloud/wd/hub</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Android_002</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10.0.0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SAMSUNG_GalaxyTabS5e_Android_10.0.0_cb1ca</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Android_003</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9.0.0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LENOVO_M10Plus_Android_10.0.0_2ba36</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SAMSUNG_GalaxyTabS6_Android_9.0.0_16c48</t>
   </si>
   <si>
     <t xml:space="preserve">SAMSUNG_GalaxyTabS4_Android_10.0.0_2133b</t>
@@ -1243,7 +1246,7 @@
     <numFmt numFmtId="167" formatCode="@"/>
     <numFmt numFmtId="168" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
-  <fonts count="15">
+  <fonts count="14">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1340,12 +1343,6 @@
       <family val="0"/>
       <charset val="1"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -1429,7 +1426,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="34">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1559,10 +1556,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -20473,14 +20466,14 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:S13"/>
+  <dimension ref="A1:S15"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="D1" activeCellId="0" sqref="D1"/>
+      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I6" activeCellId="0" sqref="I6"/>
+      <selection pane="bottomRight" activeCell="I7" activeCellId="0" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -20684,8 +20677,8 @@
         <v>381</v>
       </c>
       <c r="N4" s="8"/>
-      <c r="O4" s="8" t="n">
-        <v>900</v>
+      <c r="O4" s="19" t="n">
+        <v>104</v>
       </c>
       <c r="P4" s="8" t="s">
         <v>394</v>
@@ -20695,7 +20688,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="44.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="44" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="8" t="s">
         <v>395</v>
       </c>
@@ -20736,8 +20729,8 @@
         <v>381</v>
       </c>
       <c r="N5" s="8"/>
-      <c r="O5" s="8" t="n">
-        <v>901</v>
+      <c r="O5" s="19" t="n">
+        <v>105</v>
       </c>
       <c r="P5" s="8" t="s">
         <v>394</v>
@@ -20770,10 +20763,10 @@
         <v>377</v>
       </c>
       <c r="H6" s="8" t="s">
+        <v>396</v>
+      </c>
+      <c r="I6" s="8" t="s">
         <v>399</v>
-      </c>
-      <c r="I6" s="33" t="s">
-        <v>400</v>
       </c>
       <c r="J6" s="8" t="s">
         <v>392</v>
@@ -20788,8 +20781,8 @@
         <v>381</v>
       </c>
       <c r="N6" s="8"/>
-      <c r="O6" s="8" t="n">
-        <v>902</v>
+      <c r="O6" s="19" t="n">
+        <v>106</v>
       </c>
       <c r="P6" s="8" t="s">
         <v>394</v>
@@ -20800,57 +20793,111 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="82.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="8"/>
-      <c r="B7" s="8"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="29"/>
-      <c r="F7" s="29"/>
-      <c r="G7" s="1"/>
+      <c r="A7" s="8" t="s">
+        <v>400</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>387</v>
+      </c>
+      <c r="E7" s="29" t="s">
+        <v>388</v>
+      </c>
+      <c r="F7" s="29" t="s">
+        <v>389</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>377</v>
+      </c>
       <c r="H7" s="8" t="s">
+        <v>401</v>
+      </c>
+      <c r="I7" s="30" t="s">
+        <v>402</v>
+      </c>
+      <c r="J7" s="8" t="s">
+        <v>392</v>
+      </c>
+      <c r="K7" s="31" t="s">
+        <v>393</v>
+      </c>
+      <c r="L7" s="24" t="s">
+        <v>380</v>
+      </c>
+      <c r="M7" s="11" t="s">
+        <v>381</v>
+      </c>
+      <c r="N7" s="8"/>
+      <c r="O7" s="19" t="n">
+        <v>106</v>
+      </c>
+      <c r="P7" s="8" t="s">
+        <v>394</v>
+      </c>
+      <c r="Q7" s="32" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="82.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="8"/>
+      <c r="B8" s="8"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="29"/>
+      <c r="F8" s="29"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="8"/>
+      <c r="I8" s="30" t="s">
+        <v>403</v>
+      </c>
+      <c r="J8" s="8"/>
+      <c r="K8" s="30"/>
+      <c r="L8" s="30"/>
+      <c r="M8" s="30"/>
+      <c r="N8" s="8"/>
+      <c r="O8" s="8"/>
+      <c r="P8" s="8"/>
+      <c r="Q8" s="32"/>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I9" s="0" t="s">
         <v>399</v>
       </c>
-      <c r="I7" s="30" t="s">
-        <v>401</v>
-      </c>
-      <c r="J7" s="8"/>
-      <c r="K7" s="30"/>
-      <c r="L7" s="30"/>
-      <c r="M7" s="30"/>
-      <c r="N7" s="8"/>
-      <c r="O7" s="8"/>
-      <c r="P7" s="8"/>
-      <c r="Q7" s="32"/>
-    </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I8" s="0" t="s">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I9" s="34" t="s">
+    </row>
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I10" s="33" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I11" s="33" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I12" s="33" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I13" s="33" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I14" s="33" t="s">
         <v>391</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I10" s="34" t="s">
-        <v>397</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I11" s="34" t="s">
-        <v>391</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I12" s="34" t="s">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="16.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="14" customFormat="false" ht="16.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="15" customFormat="false" ht="16.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="16" customFormat="false" ht="16.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="17" customFormat="false" ht="16.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="P2" r:id="rId1" display="http://127.0.0.1:4723/wd/hub"/>
@@ -20861,6 +20908,8 @@
     <hyperlink ref="P5" r:id="rId6" display="https://device.pcloudy.com/appiumcloud/wd/hub"/>
     <hyperlink ref="E6" r:id="rId7" display="sriganesh.d@i-exceed.com"/>
     <hyperlink ref="P6" r:id="rId8" display="https://device.pcloudy.com/appiumcloud/wd/hub"/>
+    <hyperlink ref="E7" r:id="rId9" display="sriganesh.d@i-exceed.com"/>
+    <hyperlink ref="P7" r:id="rId10" display="https://device.pcloudy.com/appiumcloud/wd/hub"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
updating  sonar fix code changes
</commit_message>
<xml_diff>
--- a/src/test/resources/DataSet/NMCO_ONB.xlsx
+++ b/src/test/resources/DataSet/NMCO_ONB.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2676" uniqueCount="404">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2677" uniqueCount="404">
   <si>
     <t xml:space="preserve">TestCaseName</t>
   </si>
@@ -1229,10 +1229,10 @@
     <t xml:space="preserve">11.0.0</t>
   </si>
   <si>
+    <t xml:space="preserve">SAMSUNG_GalaxyTabS4_Android_10.0.0_2133b</t>
+  </si>
+  <si>
     <t xml:space="preserve">SAMSUNG_GalaxyTabS6_Android_11.0.0_383e3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SAMSUNG_GalaxyTabS4_Android_10.0.0_2133b</t>
   </si>
 </sst>
 </file>
@@ -1246,7 +1246,7 @@
     <numFmt numFmtId="167" formatCode="@"/>
     <numFmt numFmtId="168" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
-  <fonts count="14">
+  <fonts count="15">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1343,6 +1343,12 @@
       <family val="0"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF6A8759"/>
+      <name val="JetBrains Mono"/>
+      <family val="3"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -1426,7 +1432,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="35">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1556,6 +1562,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -20466,14 +20476,14 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:S15"/>
+  <dimension ref="A1:S16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F5" activeCellId="0" sqref="F5"/>
+      <selection pane="bottomRight" activeCell="I7" activeCellId="0" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -20817,8 +20827,8 @@
       <c r="H7" s="8" t="s">
         <v>401</v>
       </c>
-      <c r="I7" s="30" t="s">
-        <v>402</v>
+      <c r="I7" s="33" t="s">
+        <v>391</v>
       </c>
       <c r="J7" s="8" t="s">
         <v>392</v>
@@ -20854,7 +20864,7 @@
       <c r="G8" s="1"/>
       <c r="H8" s="8"/>
       <c r="I8" s="30" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="J8" s="8"/>
       <c r="K8" s="30"/>
@@ -20865,39 +20875,60 @@
       <c r="P8" s="8"/>
       <c r="Q8" s="32"/>
     </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I9" s="0" t="s">
+    <row r="9" customFormat="false" ht="82.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="8"/>
+      <c r="B9" s="8"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="29"/>
+      <c r="F9" s="29"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="8"/>
+      <c r="I9" s="30" t="s">
+        <v>403</v>
+      </c>
+      <c r="J9" s="8"/>
+      <c r="K9" s="30"/>
+      <c r="L9" s="30"/>
+      <c r="M9" s="30"/>
+      <c r="N9" s="8"/>
+      <c r="O9" s="8"/>
+      <c r="P9" s="8"/>
+      <c r="Q9" s="32"/>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I10" s="0" t="s">
         <v>399</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I10" s="33" t="s">
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I11" s="34" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I12" s="34" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I13" s="34" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I14" s="34" t="s">
         <v>402</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I11" s="33" t="s">
-        <v>397</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I12" s="33" t="s">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I13" s="33" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I14" s="33" t="s">
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I15" s="34" t="s">
         <v>391</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="16.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="16" customFormat="false" ht="16.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="17" customFormat="false" ht="16.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="18" customFormat="false" ht="16.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="P2" r:id="rId1" display="http://127.0.0.1:4723/wd/hub"/>

</xml_diff>

<commit_message>
updating sonarqube major code change and bug fixes
</commit_message>
<xml_diff>
--- a/src/test/resources/DataSet/NMCO_ONB.xlsx
+++ b/src/test/resources/DataSet/NMCO_ONB.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2677" uniqueCount="404">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2677" uniqueCount="403">
   <si>
     <t xml:space="preserve">TestCaseName</t>
   </si>
@@ -1224,9 +1224,6 @@
   </si>
   <si>
     <t xml:space="preserve">Android_0003</t>
-  </si>
-  <si>
-    <t xml:space="preserve">11.0.0</t>
   </si>
   <si>
     <t xml:space="preserve">SAMSUNG_GalaxyTabS4_Android_10.0.0_2133b</t>
@@ -1246,7 +1243,7 @@
     <numFmt numFmtId="167" formatCode="@"/>
     <numFmt numFmtId="168" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
-  <fonts count="15">
+  <fonts count="14">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1343,12 +1340,6 @@
       <family val="0"/>
       <charset val="1"/>
     </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF6A8759"/>
-      <name val="JetBrains Mono"/>
-      <family val="3"/>
-    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -1432,7 +1423,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="34">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1562,10 +1553,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -20479,11 +20466,11 @@
   <dimension ref="A1:S16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="topRight" activeCell="H1" activeCellId="0" sqref="H1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I7" activeCellId="0" sqref="I7"/>
+      <selection pane="bottomRight" activeCell="O7" activeCellId="0" sqref="O7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -20646,7 +20633,7 @@
       </c>
       <c r="S3" s="28"/>
     </row>
-    <row r="4" customFormat="false" ht="44" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="44.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="8" t="s">
         <v>385</v>
       </c>
@@ -20825,9 +20812,9 @@
         <v>377</v>
       </c>
       <c r="H7" s="8" t="s">
-        <v>401</v>
-      </c>
-      <c r="I7" s="33" t="s">
+        <v>390</v>
+      </c>
+      <c r="I7" s="30" t="s">
         <v>391</v>
       </c>
       <c r="J7" s="8" t="s">
@@ -20844,7 +20831,7 @@
       </c>
       <c r="N7" s="8"/>
       <c r="O7" s="19" t="n">
-        <v>106</v>
+        <v>306</v>
       </c>
       <c r="P7" s="8" t="s">
         <v>394</v>
@@ -20864,7 +20851,7 @@
       <c r="G8" s="1"/>
       <c r="H8" s="8"/>
       <c r="I8" s="30" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="J8" s="8"/>
       <c r="K8" s="30"/>
@@ -20885,7 +20872,7 @@
       <c r="G9" s="1"/>
       <c r="H9" s="8"/>
       <c r="I9" s="30" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="J9" s="8"/>
       <c r="K9" s="30"/>
@@ -20902,27 +20889,27 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I11" s="34" t="s">
-        <v>403</v>
+      <c r="I11" s="33" t="s">
+        <v>402</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I12" s="34" t="s">
+      <c r="I12" s="33" t="s">
         <v>397</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I13" s="34" t="s">
-        <v>403</v>
+      <c r="I13" s="33" t="s">
+        <v>402</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I14" s="34" t="s">
-        <v>402</v>
+      <c r="I14" s="33" t="s">
+        <v>401</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I15" s="34" t="s">
+      <c r="I15" s="33" t="s">
         <v>391</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Pcloudy app upload code with dynamic url
</commit_message>
<xml_diff>
--- a/src/test/resources/DataSet/NMCO_ONB.xlsx
+++ b/src/test/resources/DataSet/NMCO_ONB.xlsx
@@ -10,6 +10,7 @@
   <sheets>
     <sheet name="TestData" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="device" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Sheet3" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2677" uniqueCount="403">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2691" uniqueCount="412">
   <si>
     <t xml:space="preserve">TestCaseName</t>
   </si>
@@ -1226,10 +1227,37 @@
     <t xml:space="preserve">Android_0003</t>
   </si>
   <si>
+    <t xml:space="preserve">SAMSUNG_GalaxyTabS6_Android_11.0.0_383e3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ios_01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ios</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13.3.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">APPLE_iPhoneXSMax_iOS_13.3.0_9049f</t>
+  </si>
+  <si>
+    <t xml:space="preserve">XCUITest</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://github.com/bitbar/test-samples/raw/master/apps/ios/bitbar-ios-sample.ipa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">com.bitbar.testdroid.BitbarIOSSample</t>
+  </si>
+  <si>
+    <t xml:space="preserve">com.iexceed.assistedonboardingapp.assistedonboarding.AssistedOnboardingActivity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">com.iexceed.assistedonboardingapp.automation</t>
+  </si>
+  <si>
     <t xml:space="preserve">SAMSUNG_GalaxyTabS4_Android_10.0.0_2133b</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SAMSUNG_GalaxyTabS6_Android_11.0.0_383e3</t>
   </si>
 </sst>
 </file>
@@ -1243,7 +1271,7 @@
     <numFmt numFmtId="167" formatCode="@"/>
     <numFmt numFmtId="168" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
-  <fonts count="14">
+  <fonts count="15">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1340,6 +1368,13 @@
       <family val="0"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF808080"/>
+      <name val="JetBrains Mono"/>
+      <family val="3"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -1423,7 +1458,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="37">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1556,6 +1591,18 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1582,11 +1629,11 @@
       <rgbColor rgb="FF800000"/>
       <rgbColor rgb="FF067D17"/>
       <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF6A8759"/>
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF008080"/>
       <rgbColor rgb="FFB4C7DC"/>
-      <rgbColor rgb="FF6A8759"/>
+      <rgbColor rgb="FF808080"/>
       <rgbColor rgb="FF9999FF"/>
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FFFFFFCC"/>
@@ -1640,9 +1687,9 @@
   <dimension ref="A1:AMJ248"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="0" topLeftCell="K1" activePane="topRight" state="frozen"/>
+      <pane xSplit="1" ySplit="0" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="M9" activeCellId="0" sqref="M9"/>
+      <selection pane="topRight" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -20466,11 +20513,11 @@
   <dimension ref="A1:S16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="H1" activeCellId="0" sqref="H1"/>
-      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="O7" activeCellId="0" sqref="O7"/>
+      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+      <selection pane="bottomRight" activeCell="A8" activeCellId="0" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -20815,7 +20862,7 @@
         <v>390</v>
       </c>
       <c r="I7" s="30" t="s">
-        <v>391</v>
+        <v>401</v>
       </c>
       <c r="J7" s="8" t="s">
         <v>392</v>
@@ -20842,25 +20889,54 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="82.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="8"/>
-      <c r="B8" s="8"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="29"/>
-      <c r="F8" s="29"/>
-      <c r="G8" s="1"/>
-      <c r="H8" s="8"/>
-      <c r="I8" s="30" t="s">
-        <v>401</v>
-      </c>
-      <c r="J8" s="8"/>
-      <c r="K8" s="30"/>
-      <c r="L8" s="30"/>
-      <c r="M8" s="30"/>
-      <c r="N8" s="8"/>
-      <c r="O8" s="8"/>
-      <c r="P8" s="8"/>
-      <c r="Q8" s="32"/>
+      <c r="A8" s="8" t="s">
+        <v>402</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="D8" s="33" t="s">
+        <v>403</v>
+      </c>
+      <c r="E8" s="29" t="s">
+        <v>388</v>
+      </c>
+      <c r="F8" s="29" t="s">
+        <v>389</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>377</v>
+      </c>
+      <c r="H8" s="33" t="s">
+        <v>404</v>
+      </c>
+      <c r="I8" s="8" t="s">
+        <v>405</v>
+      </c>
+      <c r="J8" s="30" t="s">
+        <v>406</v>
+      </c>
+      <c r="K8" s="30" t="s">
+        <v>407</v>
+      </c>
+      <c r="L8" s="1"/>
+      <c r="M8" s="8"/>
+      <c r="N8" s="34" t="s">
+        <v>408</v>
+      </c>
+      <c r="O8" s="1" t="n">
+        <v>500</v>
+      </c>
+      <c r="P8" s="8" t="s">
+        <v>394</v>
+      </c>
+      <c r="Q8" s="32" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="82.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="8"/>
@@ -20871,9 +20947,7 @@
       <c r="F9" s="29"/>
       <c r="G9" s="1"/>
       <c r="H9" s="8"/>
-      <c r="I9" s="30" t="s">
-        <v>402</v>
-      </c>
+      <c r="I9" s="30"/>
       <c r="J9" s="8"/>
       <c r="K9" s="30"/>
       <c r="L9" s="30"/>
@@ -20883,34 +20957,12 @@
       <c r="P9" s="8"/>
       <c r="Q9" s="32"/>
     </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I10" s="0" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I11" s="33" t="s">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I12" s="33" t="s">
-        <v>397</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I13" s="33" t="s">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I14" s="33" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I15" s="33" t="s">
-        <v>391</v>
+    <row r="10" customFormat="false" ht="55.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L10" s="35" t="s">
+        <v>409</v>
+      </c>
+      <c r="M10" s="35" t="s">
+        <v>410</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="16.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -20928,6 +20980,9 @@
     <hyperlink ref="P6" r:id="rId8" display="https://device.pcloudy.com/appiumcloud/wd/hub"/>
     <hyperlink ref="E7" r:id="rId9" display="sriganesh.d@i-exceed.com"/>
     <hyperlink ref="P7" r:id="rId10" display="https://device.pcloudy.com/appiumcloud/wd/hub"/>
+    <hyperlink ref="E8" r:id="rId11" display="sriganesh.d@i-exceed.com"/>
+    <hyperlink ref="K8" r:id="rId12" display="https://github.com/bitbar/test-samples/raw/master/apps/ios/bitbar-ios-sample.ipa"/>
+    <hyperlink ref="P8" r:id="rId13" display="https://device.pcloudy.com/appiumcloud/wd/hub"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -20937,4 +20992,66 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="B4:B11"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="91" zoomScaleNormal="91" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="9.14"/>
+  </cols>
+  <sheetData>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B4" s="0" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B5" s="36" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B6" s="36" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B7" s="36" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B8" s="36" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B9" s="36" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B11" s="36" t="s">
+        <v>411</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
updaing home page definition to passing ios dynamic URL
</commit_message>
<xml_diff>
--- a/src/test/resources/DataSet/NMCO_ONB.xlsx
+++ b/src/test/resources/DataSet/NMCO_ONB.xlsx
@@ -1230,10 +1230,10 @@
     <t xml:space="preserve">ios</t>
   </si>
   <si>
-    <t xml:space="preserve">13.5.1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">APPLE_iPhone7plus_iOS_13.5.1_b1cc7</t>
+    <t xml:space="preserve">14.3.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">APPLE_iPhoneXS_iOS_14.3.0_33b29</t>
   </si>
   <si>
     <t xml:space="preserve">XCUITest</t>
@@ -20499,7 +20499,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="D1" activeCellId="0" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F8" activeCellId="0" sqref="F8"/>
+      <selection pane="bottomRight" activeCell="G7" activeCellId="0" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
updating old feature file
</commit_message>
<xml_diff>
--- a/src/test/resources/DataSet/NMCO_ONB.xlsx
+++ b/src/test/resources/DataSet/NMCO_ONB.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2690" uniqueCount="411">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2695" uniqueCount="414">
   <si>
     <t xml:space="preserve">TestCaseName</t>
   </si>
@@ -1230,31 +1230,40 @@
     <t xml:space="preserve">ios</t>
   </si>
   <si>
+    <t xml:space="preserve">13.1.3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">APPLE_iPhone7_iOS_13.1.3_316f0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">XCUITest</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://readuser:Re@d@1234@artifactory.appzillon.com/artifactory/iOS-ipa/ao/automated/AUTOMATIONDebug-1.0.0-20-11-2021-22%3A37/AUTOMATIONDebug-1.0.0-20-11-2021-22%3A37.ipa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LENOVO_M10Plus_Android_10.0.0_2ba36</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SAMSUNG_GalaxyTabS6_Android_11.0.0_383e3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SAMSUNG_GalaxyTabS5e_Android_10.0.0_cb1ca</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SAMSUNG_GalaxyTabS4_Android_10.0.0_2133b</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SAMSUNG_GalaxyTabS6_Android_9.0.0_16c48</t>
+  </si>
+  <si>
+    <t xml:space="preserve">APPLE_iPhoneXR_iOS_14.5.0_b3558</t>
+  </si>
+  <si>
+    <t xml:space="preserve">APPLE_iPhoneSE_iOS_13.5.1_c982c</t>
+  </si>
+  <si>
     <t xml:space="preserve">13.5.1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">APPLE_iPhoneSE_iOS_13.5.1_c982c</t>
-  </si>
-  <si>
-    <t xml:space="preserve">XCUITest</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://readuser:Re@d@1234@artifactory.appzillon.com/artifactory/iOS-ipa/ao/automated/AUTOMATIONDebug-1.0.0-20-11-2021-22%3A37/AUTOMATIONDebug-1.0.0-20-11-2021-22%3A37.ipa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LENOVO_M10Plus_Android_10.0.0_2ba36</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SAMSUNG_GalaxyTabS6_Android_11.0.0_383e3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SAMSUNG_GalaxyTabS5e_Android_10.0.0_cb1ca</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SAMSUNG_GalaxyTabS4_Android_10.0.0_2133b</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SAMSUNG_GalaxyTabS6_Android_9.0.0_16c48</t>
   </si>
 </sst>
 </file>
@@ -1268,7 +1277,7 @@
     <numFmt numFmtId="167" formatCode="@"/>
     <numFmt numFmtId="168" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
-  <fonts count="14">
+  <fonts count="15">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1357,6 +1366,12 @@
       <name val="JetBrains Mono"/>
       <family val="3"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
@@ -1448,7 +1463,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="37">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1585,7 +1600,15 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -20499,7 +20522,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="D1" activeCellId="0" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F8" activeCellId="0" sqref="F8"/>
+      <selection pane="bottomRight" activeCell="G8" activeCellId="0" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -20895,7 +20918,7 @@
       <c r="H8" s="32" t="s">
         <v>402</v>
       </c>
-      <c r="I8" s="11" t="s">
+      <c r="I8" s="33" t="s">
         <v>403</v>
       </c>
       <c r="J8" s="30" t="s">
@@ -20906,7 +20929,7 @@
       </c>
       <c r="L8" s="1"/>
       <c r="M8" s="8"/>
-      <c r="N8" s="33"/>
+      <c r="N8" s="34"/>
       <c r="O8" s="1" t="n">
         <v>500</v>
       </c>
@@ -20952,10 +20975,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B4:B13"/>
+  <dimension ref="B4:F19"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="91" zoomScaleNormal="91" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
+      <selection pane="topLeft" activeCell="B18" activeCellId="0" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -20969,27 +20992,27 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="34" t="s">
+      <c r="B5" s="35" t="s">
         <v>407</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="34" t="s">
+      <c r="B6" s="35" t="s">
         <v>408</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="34" t="s">
+      <c r="B7" s="35" t="s">
         <v>407</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="34" t="s">
+      <c r="B8" s="35" t="s">
         <v>409</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="34" t="s">
+      <c r="B9" s="35" t="s">
         <v>410</v>
       </c>
     </row>
@@ -20999,13 +21022,34 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="34" t="s">
+      <c r="B11" s="35" t="s">
         <v>409</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="34" t="s">
+      <c r="B13" s="35" t="s">
         <v>391</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B17" s="0" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B18" s="0" t="s">
+        <v>403</v>
+      </c>
+      <c r="F18" s="0" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B19" s="36" t="s">
+        <v>412</v>
+      </c>
+      <c r="F19" s="36" t="s">
+        <v>413</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updating excel and legal entity feature file
</commit_message>
<xml_diff>
--- a/src/test/resources/DataSet/NMCO_ONB.xlsx
+++ b/src/test/resources/DataSet/NMCO_ONB.xlsx
@@ -1197,30 +1197,33 @@
     <t xml:space="preserve">11.0.0</t>
   </si>
   <si>
+    <t xml:space="preserve">SAMSUNG_GalaxyTabS6_Android_11.0.0_383e3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">uiautomator2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Automation-1-0-0-24-11-2021.apk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://device.pcloudy.com/appiumcloud/wd/hub</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Android_002</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9.0.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SAMSUNG_GalaxyTabS3_Android_9.0.0_77658</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Android_003</t>
+  </si>
+  <si>
     <t xml:space="preserve">SAMSUNG_GalaxyTabS5e_Android_11.0.0_cb1ca</t>
   </si>
   <si>
-    <t xml:space="preserve">uiautomator2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Automation-1-0-0-24-11-2021.apk</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://device.pcloudy.com/appiumcloud/wd/hub</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Android_002</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9.0.0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SAMSUNG_GalaxyTabS3_Android_9.0.0_77658</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Android_003</t>
-  </si>
-  <si>
     <t xml:space="preserve">Android_0003</t>
   </si>
   <si>
@@ -1243,9 +1246,6 @@
   </si>
   <si>
     <t xml:space="preserve">LENOVO_M10Plus_Android_10.0.0_2ba36</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SAMSUNG_GalaxyTabS6_Android_11.0.0_383e3</t>
   </si>
   <si>
     <t xml:space="preserve">SAMSUNG_GalaxyTabS5e_Android_10.0.0_cb1ca</t>
@@ -1277,7 +1277,7 @@
     <numFmt numFmtId="167" formatCode="@"/>
     <numFmt numFmtId="168" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
-  <fonts count="15">
+  <fonts count="16">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1366,6 +1366,12 @@
       <name val="JetBrains Mono"/>
       <family val="3"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF6A8759"/>
+      <name val="JetBrains Mono"/>
+      <family val="3"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1463,7 +1469,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="38">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1584,7 +1590,7 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1592,15 +1598,19 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1608,7 +1618,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -20522,7 +20532,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="D1" activeCellId="0" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G8" activeCellId="0" sqref="G8"/>
+      <selection pane="bottomRight" activeCell="G4" activeCellId="0" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -20685,7 +20695,7 @@
       </c>
       <c r="S3" s="28"/>
     </row>
-    <row r="4" customFormat="false" ht="44" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="44.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="8" t="s">
         <v>385</v>
       </c>
@@ -20762,7 +20772,7 @@
       <c r="H5" s="8" t="s">
         <v>396</v>
       </c>
-      <c r="I5" s="30" t="s">
+      <c r="I5" s="32" t="s">
         <v>397</v>
       </c>
       <c r="J5" s="8" t="s">
@@ -20814,8 +20824,8 @@
       <c r="H6" s="8" t="s">
         <v>390</v>
       </c>
-      <c r="I6" s="30" t="s">
-        <v>391</v>
+      <c r="I6" s="32" t="s">
+        <v>399</v>
       </c>
       <c r="J6" s="8" t="s">
         <v>392</v>
@@ -20843,7 +20853,7 @@
     </row>
     <row r="7" customFormat="false" ht="82.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="8" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="B7" s="8" t="s">
         <v>44</v>
@@ -20866,8 +20876,8 @@
       <c r="H7" s="8" t="s">
         <v>390</v>
       </c>
-      <c r="I7" s="30" t="s">
-        <v>391</v>
+      <c r="I7" s="32" t="s">
+        <v>399</v>
       </c>
       <c r="J7" s="8" t="s">
         <v>392</v>
@@ -20895,7 +20905,7 @@
     </row>
     <row r="8" customFormat="false" ht="82.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="8" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="B8" s="8" t="s">
         <v>44</v>
@@ -20903,8 +20913,8 @@
       <c r="C8" s="1" t="s">
         <v>386</v>
       </c>
-      <c r="D8" s="32" t="s">
-        <v>401</v>
+      <c r="D8" s="33" t="s">
+        <v>402</v>
       </c>
       <c r="E8" s="29" t="s">
         <v>388</v>
@@ -20915,21 +20925,21 @@
       <c r="G8" s="1" t="s">
         <v>377</v>
       </c>
-      <c r="H8" s="32" t="s">
-        <v>402</v>
-      </c>
-      <c r="I8" s="33" t="s">
+      <c r="H8" s="33" t="s">
         <v>403</v>
       </c>
-      <c r="J8" s="30" t="s">
+      <c r="I8" s="34" t="s">
         <v>404</v>
       </c>
+      <c r="J8" s="32" t="s">
+        <v>405</v>
+      </c>
       <c r="K8" s="11" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="L8" s="1"/>
       <c r="M8" s="8"/>
-      <c r="N8" s="34"/>
+      <c r="N8" s="35"/>
       <c r="O8" s="1" t="n">
         <v>500</v>
       </c>
@@ -20978,7 +20988,7 @@
   <dimension ref="B4:F19"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="91" zoomScaleNormal="91" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B18" activeCellId="0" sqref="B18"/>
+      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -20988,31 +20998,31 @@
   <sheetData>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="0" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="35" t="s">
-        <v>407</v>
+      <c r="B5" s="36" t="s">
+        <v>391</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="35" t="s">
+      <c r="B6" s="36" t="s">
         <v>408</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="35" t="s">
-        <v>407</v>
+      <c r="B7" s="36" t="s">
+        <v>391</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="35" t="s">
+      <c r="B8" s="36" t="s">
         <v>409</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="35" t="s">
+      <c r="B9" s="36" t="s">
         <v>410</v>
       </c>
     </row>
@@ -21022,13 +21032,13 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="35" t="s">
+      <c r="B11" s="36" t="s">
         <v>409</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="35" t="s">
-        <v>391</v>
+      <c r="B13" s="36" t="s">
+        <v>399</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -21038,17 +21048,17 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="0" t="s">
+        <v>404</v>
+      </c>
+      <c r="F18" s="0" t="s">
         <v>403</v>
       </c>
-      <c r="F18" s="0" t="s">
-        <v>402</v>
-      </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="36" t="s">
+      <c r="B19" s="37" t="s">
         <v>412</v>
       </c>
-      <c r="F19" s="36" t="s">
+      <c r="F19" s="37" t="s">
         <v>413</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update ios device in excel
</commit_message>
<xml_diff>
--- a/src/test/resources/DataSet/NMCO_ONB.xlsx
+++ b/src/test/resources/DataSet/NMCO_ONB.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2696" uniqueCount="415">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2696" uniqueCount="416">
   <si>
     <t xml:space="preserve">TestCaseName</t>
   </si>
@@ -1233,40 +1233,43 @@
     <t xml:space="preserve">ios</t>
   </si>
   <si>
+    <t xml:space="preserve">13.3.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">APPLE_iPhoneX_iOS_13.3.1_90703</t>
+  </si>
+  <si>
+    <t xml:space="preserve">XCUITest</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://readuser:Re@d@1234@artifactory.appzillon.com/artifactory/iOS-ipa/ao/automated/AUTOMATIONDebug-1.0.0-20-11-2021-22%3A37/AUTOMATIONDebug-1.0.0-20-11-2021-22%3A37.ipa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LENOVO_M10Plus_Android_10.0.0_2ba36</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SAMSUNG_GalaxyTabS5e_Android_10.0.0_cb1ca</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SAMSUNG_GalaxyTabS4_Android_10.0.0_2133b</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SAMSUNG_GalaxyTabS6_Android_9.0.0_16c48</t>
+  </si>
+  <si>
+    <t xml:space="preserve">APPLE_iPhoneXR_iOS_14.5.0_b3558</t>
+  </si>
+  <si>
+    <t xml:space="preserve">APPLE_iPhone7_iOS_13.1.3_316f0</t>
+  </si>
+  <si>
     <t xml:space="preserve">13.1.3</t>
   </si>
   <si>
-    <t xml:space="preserve">APPLE_iPhone7_iOS_13.1.3_316f0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">XCUITest</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://readuser:Re@d@1234@artifactory.appzillon.com/artifactory/iOS-ipa/ao/automated/AUTOMATIONDebug-1.0.0-20-11-2021-22%3A37/AUTOMATIONDebug-1.0.0-20-11-2021-22%3A37.ipa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LENOVO_M10Plus_Android_10.0.0_2ba36</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SAMSUNG_GalaxyTabS5e_Android_10.0.0_cb1ca</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SAMSUNG_GalaxyTabS4_Android_10.0.0_2133b</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SAMSUNG_GalaxyTabS6_Android_9.0.0_16c48</t>
-  </si>
-  <si>
-    <t xml:space="preserve">APPLE_iPhoneXR_iOS_14.5.0_b3558</t>
-  </si>
-  <si>
     <t xml:space="preserve">APPLE_iPhoneSE_iOS_13.5.1_c982c</t>
   </si>
   <si>
     <t xml:space="preserve">13.5.1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">APPLE_iPhoneX_iOS_13.3.1_90703</t>
   </si>
 </sst>
 </file>
@@ -20525,7 +20528,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="D1" activeCellId="0" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I4" activeCellId="0" sqref="I4"/>
+      <selection pane="bottomRight" activeCell="G8" activeCellId="0" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -20981,7 +20984,7 @@
   <dimension ref="B4:F20"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="91" zoomScaleNormal="91" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
+      <selection pane="topLeft" activeCell="B20" activeCellId="0" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -21041,23 +21044,23 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="0" t="s">
-        <v>404</v>
+        <v>412</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>403</v>
+        <v>413</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="36" t="s">
-        <v>412</v>
+        <v>414</v>
       </c>
       <c r="F19" s="36" t="s">
-        <v>413</v>
+        <v>415</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="0" t="s">
-        <v>414</v>
+        <v>404</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updating legalentity feature file with gesture scenario
</commit_message>
<xml_diff>
--- a/src/test/resources/DataSet/NMCO_ONB.xlsx
+++ b/src/test/resources/DataSet/NMCO_ONB.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2698" uniqueCount="419">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2699" uniqueCount="420">
   <si>
     <t xml:space="preserve">TestCaseName</t>
   </si>
@@ -1261,6 +1261,9 @@
   </si>
   <si>
     <t xml:space="preserve">SAMSUNG_GalaxyM02_Android_11.0.0_51323</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SAMSUNG_GalaxyM01_Android_11.0.0_7425f</t>
   </si>
   <si>
     <t xml:space="preserve">APPLE_iPhoneXR_iOS_14.5.0_b3558</t>
@@ -20547,7 +20550,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="D1" activeCellId="0" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J7" activeCellId="0" sqref="J7"/>
+      <selection pane="bottomRight" activeCell="I4" activeCellId="0" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -21003,7 +21006,7 @@
   <dimension ref="B4:F24"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="91" zoomScaleNormal="91" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B23" activeCellId="0" sqref="B23"/>
+      <selection pane="topLeft" activeCell="B16" activeCellId="0" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -21061,28 +21064,32 @@
         <v>412</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B15" s="0" t="s">
+        <v>413</v>
+      </c>
+    </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="0" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="0" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="37" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="F22" s="37" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -21092,7 +21099,7 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="0" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updating excel according to jenkins
</commit_message>
<xml_diff>
--- a/src/test/resources/DataSet/NMCO_ONB.xlsx
+++ b/src/test/resources/DataSet/NMCO_ONB.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2711" uniqueCount="426">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2711" uniqueCount="425">
   <si>
     <t xml:space="preserve">TestCaseName</t>
   </si>
@@ -1209,7 +1209,7 @@
     <t xml:space="preserve">11.0.0</t>
   </si>
   <si>
-    <t xml:space="preserve">SAMSUNG_GalaxyM12_Android_11.0.0_df6a7</t>
+    <t xml:space="preserve">SAMSUNG_GalaxyM02_Android_11.0.0_51323</t>
   </si>
   <si>
     <t xml:space="preserve">uiautomator2</t>
@@ -1276,9 +1276,6 @@
   </si>
   <si>
     <t xml:space="preserve">SAMSUNG_GalaxyTabS3_Android_9.0.0_77658</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SAMSUNG_GalaxyM02_Android_11.0.0_51323</t>
   </si>
   <si>
     <t xml:space="preserve">SAMSUNG_GalaxyM01_Android_11.0.0_7425f</t>
@@ -1404,10 +1401,10 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color rgb="FF6A8759"/>
-      <name val="JetBrains Mono"/>
-      <family val="3"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -1416,10 +1413,10 @@
       <family val="3"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
+      <sz val="12"/>
+      <color rgb="FF6A8759"/>
+      <name val="JetBrains Mono"/>
+      <family val="3"/>
     </font>
     <font>
       <sz val="12"/>
@@ -1648,16 +1645,16 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -20614,7 +20611,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="G1" activeCellId="0" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I7" activeCellId="0" sqref="I7"/>
+      <selection pane="bottomRight" activeCell="H4" activeCellId="0" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -20777,7 +20774,7 @@
       </c>
       <c r="S3" s="28"/>
     </row>
-    <row r="4" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="46.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="8" t="s">
         <v>389</v>
       </c>
@@ -20854,7 +20851,7 @@
       <c r="H5" s="8" t="s">
         <v>394</v>
       </c>
-      <c r="I5" s="30" t="s">
+      <c r="I5" s="34" t="s">
         <v>401</v>
       </c>
       <c r="J5" s="8" t="s">
@@ -20906,7 +20903,7 @@
       <c r="H6" s="8" t="s">
         <v>394</v>
       </c>
-      <c r="I6" s="30" t="s">
+      <c r="I6" s="34" t="s">
         <v>404</v>
       </c>
       <c r="J6" s="8" t="s">
@@ -20958,7 +20955,7 @@
       <c r="H7" s="8" t="s">
         <v>394</v>
       </c>
-      <c r="I7" s="34" t="s">
+      <c r="I7" s="35" t="s">
         <v>401</v>
       </c>
       <c r="J7" s="8" t="s">
@@ -20995,7 +20992,7 @@
       <c r="C8" s="1" t="s">
         <v>390</v>
       </c>
-      <c r="D8" s="35" t="s">
+      <c r="D8" s="36" t="s">
         <v>408</v>
       </c>
       <c r="E8" s="29" t="s">
@@ -21007,13 +21004,13 @@
       <c r="G8" s="1" t="s">
         <v>381</v>
       </c>
-      <c r="H8" s="35" t="s">
+      <c r="H8" s="36" t="s">
         <v>409</v>
       </c>
-      <c r="I8" s="36" t="s">
+      <c r="I8" s="30" t="s">
         <v>410</v>
       </c>
-      <c r="J8" s="34" t="s">
+      <c r="J8" s="35" t="s">
         <v>411</v>
       </c>
       <c r="K8" s="11" t="s">
@@ -21070,7 +21067,7 @@
   <dimension ref="B4:F24"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="91" zoomScaleNormal="91" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
+      <selection pane="topLeft" activeCell="B14" activeCellId="0" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -21125,35 +21122,35 @@
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="0" t="s">
-        <v>418</v>
+        <v>395</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="0" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="0" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="0" t="s">
+        <v>420</v>
+      </c>
+      <c r="F21" s="0" t="s">
         <v>421</v>
-      </c>
-      <c r="F21" s="0" t="s">
-        <v>422</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="39" t="s">
+        <v>422</v>
+      </c>
+      <c r="F22" s="39" t="s">
         <v>423</v>
-      </c>
-      <c r="F22" s="39" t="s">
-        <v>424</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -21163,7 +21160,7 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="0" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updating excel according to jenkins job trigger
</commit_message>
<xml_diff>
--- a/src/test/resources/DataSet/NMCO_ONB.xlsx
+++ b/src/test/resources/DataSet/NMCO_ONB.xlsx
@@ -1209,79 +1209,79 @@
     <t xml:space="preserve">11.0.0</t>
   </si>
   <si>
+    <t xml:space="preserve">SAMSUNG_GalaxyTabS6_Android_11.0.0_383e3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">uiautomator2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Automation-1-0-5-6-12-2021.apk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">com.iexceed.assistedonboardingapp.assistedonboarding.AssistedOnboardingActivity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://device.pcloudy.com/appiumcloud/wd/hub</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Android_002</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SAMSUNG_GalaxyTabS5e_Android_11.0.0_cb1ca</t>
+  </si>
+  <si>
+    <t xml:space="preserve">com.iexceed.assistedonboardingapp.qa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Android_003</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Android_0003</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Automation-1-0-0-24-11-2021.apk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IOS_001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ios</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13.3.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">APPLE_iPhoneX_iOS_13.3.1_90703</t>
+  </si>
+  <si>
+    <t xml:space="preserve">XCUITest</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://readuser:Re@d@1234@artifactory.appzillon.com/artifactory/iOS-ipa/ao/automated/AUTOMATIONDebug-1.0.0-20-11-2021-22%3A37/AUTOMATIONDebug-1.0.0-20-11-2021-22%3A37.ipa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LENOVO_M10Plus_Android_10.0.0_2ba36</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SAMSUNG_GalaxyTabS5e_Android_10.0.0_cb1ca</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SAMSUNG_GalaxyTabS4_Android_10.0.0_2133b</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SAMSUNG_GalaxyTabS6_Android_9.0.0_16c48</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SAMSUNG_GalaxyTabS3_Android_9.0.0_77658</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SAMSUNG_GalaxyM02_Android_11.0.0_51323</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SAMSUNG_GalaxyM01_Android_11.0.0_7425f</t>
+  </si>
+  <si>
     <t xml:space="preserve">SAMSUNG_GalaxyM12_Android_11.0.0_df6a7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">uiautomator2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Automation-1-0-5-6-12-2021.apk</t>
-  </si>
-  <si>
-    <t xml:space="preserve">com.iexceed.assistedonboardingapp.assistedonboarding.AssistedOnboardingActivity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://device.pcloudy.com/appiumcloud/wd/hub</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Android_002</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SAMSUNG_GalaxyTabS5e_Android_11.0.0_cb1ca</t>
-  </si>
-  <si>
-    <t xml:space="preserve">com.iexceed.assistedonboardingapp.qa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Android_003</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SAMSUNG_GalaxyTabS6_Android_11.0.0_383e3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Android_0003</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Automation-1-0-0-24-11-2021.apk</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IOS_001</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ios</t>
-  </si>
-  <si>
-    <t xml:space="preserve">13.3.1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">APPLE_iPhoneX_iOS_13.3.1_90703</t>
-  </si>
-  <si>
-    <t xml:space="preserve">XCUITest</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://readuser:Re@d@1234@artifactory.appzillon.com/artifactory/iOS-ipa/ao/automated/AUTOMATIONDebug-1.0.0-20-11-2021-22%3A37/AUTOMATIONDebug-1.0.0-20-11-2021-22%3A37.ipa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LENOVO_M10Plus_Android_10.0.0_2ba36</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SAMSUNG_GalaxyTabS5e_Android_10.0.0_cb1ca</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SAMSUNG_GalaxyTabS4_Android_10.0.0_2133b</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SAMSUNG_GalaxyTabS6_Android_9.0.0_16c48</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SAMSUNG_GalaxyTabS3_Android_9.0.0_77658</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SAMSUNG_GalaxyM02_Android_11.0.0_51323</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SAMSUNG_GalaxyM01_Android_11.0.0_7425f</t>
   </si>
   <si>
     <t xml:space="preserve">APPLE_iPhoneXR_iOS_14.5.0_b3558</t>
@@ -1404,10 +1404,10 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
+      <sz val="12"/>
+      <color rgb="FF6A8759"/>
+      <name val="JetBrains Mono"/>
+      <family val="3"/>
     </font>
     <font>
       <sz val="12"/>
@@ -20753,7 +20753,7 @@
       </c>
       <c r="S3" s="28"/>
     </row>
-    <row r="4" customFormat="false" ht="46.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="8" t="s">
         <v>389</v>
       </c>
@@ -20883,7 +20883,7 @@
         <v>394</v>
       </c>
       <c r="I6" s="32" t="s">
-        <v>404</v>
+        <v>395</v>
       </c>
       <c r="J6" s="8" t="s">
         <v>396</v>
@@ -20911,7 +20911,7 @@
     </row>
     <row r="7" customFormat="false" ht="82.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="8" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="B7" s="8" t="s">
         <v>44</v>
@@ -20941,7 +20941,7 @@
         <v>396</v>
       </c>
       <c r="K7" s="8" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="L7" s="24" t="s">
         <v>384</v>
@@ -20963,7 +20963,7 @@
     </row>
     <row r="8" customFormat="false" ht="82.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="8" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B8" s="8" t="s">
         <v>44</v>
@@ -20972,7 +20972,7 @@
         <v>390</v>
       </c>
       <c r="D8" s="33" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="E8" s="29" t="s">
         <v>392</v>
@@ -20984,16 +20984,16 @@
         <v>381</v>
       </c>
       <c r="H8" s="33" t="s">
+        <v>408</v>
+      </c>
+      <c r="I8" s="8" t="s">
         <v>409</v>
       </c>
-      <c r="I8" s="8" t="s">
+      <c r="J8" s="32" t="s">
         <v>410</v>
       </c>
-      <c r="J8" s="32" t="s">
+      <c r="K8" s="11" t="s">
         <v>411</v>
-      </c>
-      <c r="K8" s="11" t="s">
-        <v>412</v>
       </c>
       <c r="L8" s="1"/>
       <c r="M8" s="8"/>
@@ -21046,7 +21046,7 @@
   <dimension ref="B4:F27"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="91" zoomScaleNormal="91" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B16" activeCellId="0" sqref="B16"/>
+      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -21056,42 +21056,42 @@
   <sheetData>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="0" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="35" t="s">
-        <v>404</v>
+        <v>395</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="35" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="35" t="s">
-        <v>404</v>
+        <v>395</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="35" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="35" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="0" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="35" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -21101,17 +21101,17 @@
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="0" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="0" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="0" t="s">
-        <v>395</v>
+        <v>419</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -21141,7 +21141,7 @@
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="0" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
updating project with jekins job trigger with one URL
</commit_message>
<xml_diff>
--- a/src/test/resources/DataSet/NMCO_ONB.xlsx
+++ b/src/test/resources/DataSet/NMCO_ONB.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2712" uniqueCount="426">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2713" uniqueCount="427">
   <si>
     <t xml:space="preserve">TestCaseName</t>
   </si>
@@ -1135,6 +1135,9 @@
   </si>
   <si>
     <t xml:space="preserve">automationName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">applicationURL</t>
   </si>
   <si>
     <t xml:space="preserve">applicationName</t>
@@ -1313,7 +1316,7 @@
     <numFmt numFmtId="167" formatCode="@"/>
     <numFmt numFmtId="168" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
-  <fonts count="15">
+  <fonts count="14">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1405,12 +1408,6 @@
     </font>
     <font>
       <sz val="12"/>
-      <color rgb="FF6A8759"/>
-      <name val="JetBrains Mono"/>
-      <family val="3"/>
-    </font>
-    <font>
-      <sz val="12"/>
       <color rgb="FF808080"/>
       <name val="JetBrains Mono"/>
       <family val="3"/>
@@ -1499,7 +1496,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="36">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1620,7 +1617,7 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1628,15 +1625,11 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -20583,14 +20576,14 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:S16"/>
+  <dimension ref="A1:T9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="G1" activeCellId="0" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H4" activeCellId="0" sqref="H4"/>
+      <selection pane="bottomRight" activeCell="K7" activeCellId="0" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -20604,12 +20597,12 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="9.17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="18.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="9.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="14.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="19.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="26.35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="14" style="0" width="9.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="29.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="17" style="0" width="9.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="11" style="0" width="14.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="19.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="26.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="15" style="0" width="9.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="29.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="18" style="0" width="9.17"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -20658,375 +20651,382 @@
       <c r="O1" s="4" t="s">
         <v>375</v>
       </c>
-      <c r="P1" s="18" t="s">
+      <c r="P1" s="4" t="s">
         <v>376</v>
       </c>
-      <c r="Q1" s="4" t="s">
+      <c r="Q1" s="18" t="s">
         <v>377</v>
+      </c>
+      <c r="R1" s="4" t="s">
+        <v>378</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="19" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="B2" s="20" t="s">
         <v>44</v>
       </c>
       <c r="C2" s="20" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="D2" s="20" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="E2" s="21"/>
       <c r="F2" s="21"/>
       <c r="G2" s="20" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="H2" s="20"/>
       <c r="I2" s="20" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="J2" s="22" t="s">
-        <v>383</v>
-      </c>
-      <c r="K2" s="23"/>
-      <c r="L2" s="24" t="s">
         <v>384</v>
       </c>
-      <c r="M2" s="11" t="s">
+      <c r="K2" s="22"/>
+      <c r="L2" s="23"/>
+      <c r="M2" s="24" t="s">
         <v>385</v>
       </c>
-      <c r="N2" s="23"/>
-      <c r="O2" s="22" t="n">
+      <c r="N2" s="11" t="s">
+        <v>386</v>
+      </c>
+      <c r="O2" s="23"/>
+      <c r="P2" s="22" t="n">
         <v>500</v>
       </c>
-      <c r="P2" s="25" t="s">
-        <v>386</v>
-      </c>
-      <c r="Q2" s="22" t="n">
+      <c r="Q2" s="25" t="s">
+        <v>387</v>
+      </c>
+      <c r="R2" s="22" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="19" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="B3" s="19" t="s">
         <v>44</v>
       </c>
       <c r="C3" s="19" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="D3" s="19" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="E3" s="19"/>
       <c r="F3" s="19"/>
       <c r="G3" s="19" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="H3" s="26"/>
       <c r="I3" s="26" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="J3" s="26" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="K3" s="26"/>
-      <c r="L3" s="24" t="s">
-        <v>384</v>
-      </c>
-      <c r="M3" s="11" t="s">
+      <c r="L3" s="26"/>
+      <c r="M3" s="24" t="s">
         <v>385</v>
       </c>
-      <c r="N3" s="19"/>
-      <c r="O3" s="19" t="n">
+      <c r="N3" s="11" t="s">
+        <v>386</v>
+      </c>
+      <c r="O3" s="19"/>
+      <c r="P3" s="19" t="n">
         <v>103</v>
       </c>
-      <c r="P3" s="26" t="s">
-        <v>386</v>
-      </c>
-      <c r="Q3" s="27" t="n">
+      <c r="Q3" s="26" t="s">
+        <v>387</v>
+      </c>
+      <c r="R3" s="27" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="S3" s="28"/>
+      <c r="T3" s="28"/>
     </row>
     <row r="4" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="8" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="B4" s="8" t="s">
         <v>44</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="E4" s="29" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="F4" s="29" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="H4" s="8" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="I4" s="30" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="J4" s="8" t="s">
-        <v>396</v>
-      </c>
-      <c r="K4" s="11" t="s">
         <v>397</v>
       </c>
-      <c r="L4" s="24" t="s">
+      <c r="K4" s="8"/>
+      <c r="L4" s="11" t="s">
         <v>398</v>
       </c>
-      <c r="M4" s="11" t="s">
-        <v>385</v>
-      </c>
-      <c r="N4" s="8"/>
-      <c r="O4" s="19" t="n">
+      <c r="M4" s="24" t="s">
+        <v>399</v>
+      </c>
+      <c r="N4" s="11" t="s">
+        <v>386</v>
+      </c>
+      <c r="O4" s="8"/>
+      <c r="P4" s="19" t="n">
         <v>306</v>
       </c>
-      <c r="P4" s="8" t="s">
-        <v>399</v>
-      </c>
-      <c r="Q4" s="31" t="n">
+      <c r="Q4" s="8" t="s">
+        <v>400</v>
+      </c>
+      <c r="R4" s="31" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="8" t="s">
+        <v>401</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>391</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>392</v>
+      </c>
+      <c r="E5" s="29" t="s">
+        <v>393</v>
+      </c>
+      <c r="F5" s="29" t="s">
+        <v>394</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>382</v>
+      </c>
+      <c r="H5" s="8" t="s">
+        <v>395</v>
+      </c>
+      <c r="I5" s="30" t="s">
+        <v>402</v>
+      </c>
+      <c r="J5" s="8" t="s">
+        <v>397</v>
+      </c>
+      <c r="K5" s="8"/>
+      <c r="L5" s="11" t="s">
+        <v>398</v>
+      </c>
+      <c r="M5" s="24" t="s">
+        <v>399</v>
+      </c>
+      <c r="N5" s="11" t="s">
+        <v>403</v>
+      </c>
+      <c r="O5" s="8"/>
+      <c r="P5" s="19" t="n">
+        <v>105</v>
+      </c>
+      <c r="Q5" s="8" t="s">
         <v>400</v>
       </c>
-      <c r="B5" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>390</v>
-      </c>
-      <c r="D5" s="8" t="s">
-        <v>391</v>
-      </c>
-      <c r="E5" s="29" t="s">
-        <v>392</v>
-      </c>
-      <c r="F5" s="29" t="s">
-        <v>393</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>381</v>
-      </c>
-      <c r="H5" s="8" t="s">
-        <v>394</v>
-      </c>
-      <c r="I5" s="32" t="s">
-        <v>401</v>
-      </c>
-      <c r="J5" s="8" t="s">
-        <v>396</v>
-      </c>
-      <c r="K5" s="11" t="s">
-        <v>397</v>
-      </c>
-      <c r="L5" s="24" t="s">
-        <v>398</v>
-      </c>
-      <c r="M5" s="11" t="s">
-        <v>402</v>
-      </c>
-      <c r="N5" s="8"/>
-      <c r="O5" s="19" t="n">
-        <v>105</v>
-      </c>
-      <c r="P5" s="8" t="s">
-        <v>399</v>
-      </c>
-      <c r="Q5" s="31" t="n">
+      <c r="R5" s="31" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="8" t="s">
+        <v>404</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>391</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>392</v>
+      </c>
+      <c r="E6" s="29" t="s">
+        <v>393</v>
+      </c>
+      <c r="F6" s="29" t="s">
+        <v>394</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>382</v>
+      </c>
+      <c r="H6" s="8" t="s">
+        <v>395</v>
+      </c>
+      <c r="I6" s="30" t="s">
+        <v>396</v>
+      </c>
+      <c r="J6" s="8" t="s">
+        <v>397</v>
+      </c>
+      <c r="K6" s="8"/>
+      <c r="L6" s="11" t="s">
+        <v>398</v>
+      </c>
+      <c r="M6" s="24" t="s">
+        <v>399</v>
+      </c>
+      <c r="N6" s="11" t="s">
         <v>403</v>
       </c>
-      <c r="B6" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>390</v>
-      </c>
-      <c r="D6" s="8" t="s">
-        <v>391</v>
-      </c>
-      <c r="E6" s="29" t="s">
-        <v>392</v>
-      </c>
-      <c r="F6" s="29" t="s">
-        <v>393</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>381</v>
-      </c>
-      <c r="H6" s="8" t="s">
-        <v>394</v>
-      </c>
-      <c r="I6" s="32" t="s">
-        <v>395</v>
-      </c>
-      <c r="J6" s="8" t="s">
-        <v>396</v>
-      </c>
-      <c r="K6" s="11" t="s">
-        <v>397</v>
-      </c>
-      <c r="L6" s="24" t="s">
-        <v>398</v>
-      </c>
-      <c r="M6" s="11" t="s">
-        <v>402</v>
-      </c>
-      <c r="N6" s="8"/>
-      <c r="O6" s="19" t="n">
+      <c r="O6" s="8"/>
+      <c r="P6" s="19" t="n">
         <v>106</v>
       </c>
-      <c r="P6" s="8" t="s">
-        <v>399</v>
-      </c>
-      <c r="Q6" s="31" t="n">
+      <c r="Q6" s="8" t="s">
+        <v>400</v>
+      </c>
+      <c r="R6" s="31" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="82.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="8" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="B7" s="8" t="s">
         <v>44</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="E7" s="29" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="F7" s="29" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="H7" s="8" t="s">
-        <v>394</v>
-      </c>
-      <c r="I7" s="32" t="s">
-        <v>401</v>
+        <v>395</v>
+      </c>
+      <c r="I7" s="30" t="s">
+        <v>402</v>
       </c>
       <c r="J7" s="8" t="s">
-        <v>396</v>
-      </c>
-      <c r="K7" s="8" t="s">
-        <v>405</v>
-      </c>
-      <c r="L7" s="24" t="s">
-        <v>384</v>
-      </c>
-      <c r="M7" s="11" t="s">
+        <v>397</v>
+      </c>
+      <c r="K7" s="8"/>
+      <c r="L7" s="8" t="s">
+        <v>406</v>
+      </c>
+      <c r="M7" s="24" t="s">
         <v>385</v>
       </c>
-      <c r="N7" s="8"/>
-      <c r="O7" s="19" t="n">
+      <c r="N7" s="11" t="s">
+        <v>386</v>
+      </c>
+      <c r="O7" s="8"/>
+      <c r="P7" s="19" t="n">
         <v>306</v>
       </c>
-      <c r="P7" s="8" t="s">
-        <v>399</v>
-      </c>
-      <c r="Q7" s="31" t="n">
+      <c r="Q7" s="8" t="s">
+        <v>400</v>
+      </c>
+      <c r="R7" s="31" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="82.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="8" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="B8" s="8" t="s">
         <v>44</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>390</v>
-      </c>
-      <c r="D8" s="33" t="s">
-        <v>407</v>
+        <v>391</v>
+      </c>
+      <c r="D8" s="32" t="s">
+        <v>408</v>
       </c>
       <c r="E8" s="29" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="F8" s="29" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>381</v>
-      </c>
-      <c r="H8" s="33" t="s">
-        <v>408</v>
+        <v>382</v>
+      </c>
+      <c r="H8" s="32" t="s">
+        <v>409</v>
       </c>
       <c r="I8" s="8" t="s">
-        <v>409</v>
-      </c>
-      <c r="J8" s="32" t="s">
         <v>410</v>
       </c>
-      <c r="K8" s="11" t="s">
+      <c r="J8" s="30" t="s">
         <v>411</v>
       </c>
-      <c r="L8" s="1"/>
-      <c r="M8" s="8"/>
-      <c r="N8" s="34"/>
-      <c r="O8" s="1" t="n">
+      <c r="K8" s="30"/>
+      <c r="L8" s="11" t="s">
+        <v>412</v>
+      </c>
+      <c r="M8" s="1"/>
+      <c r="N8" s="8"/>
+      <c r="O8" s="33"/>
+      <c r="P8" s="1" t="n">
         <v>500</v>
       </c>
-      <c r="P8" s="8" t="s">
-        <v>399</v>
-      </c>
-      <c r="Q8" s="31" t="n">
+      <c r="Q8" s="8" t="s">
+        <v>400</v>
+      </c>
+      <c r="R8" s="31" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="82.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="16" customFormat="false" ht="16.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="17" customFormat="false" ht="16.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="18" customFormat="false" ht="16.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="P2" r:id="rId1" display="http://127.0.0.1:4723/wd/hub"/>
-    <hyperlink ref="P3" r:id="rId2" display="http://127.0.0.1:4723/wd/hub"/>
+    <hyperlink ref="Q2" r:id="rId1" display="http://127.0.0.1:4723/wd/hub"/>
+    <hyperlink ref="Q3" r:id="rId2" display="http://127.0.0.1:4723/wd/hub"/>
     <hyperlink ref="E4" r:id="rId3" display="sriganesh.d@i-exceed.com"/>
-    <hyperlink ref="P4" r:id="rId4" display="https://device.pcloudy.com/appiumcloud/wd/hub"/>
+    <hyperlink ref="Q4" r:id="rId4" display="https://device.pcloudy.com/appiumcloud/wd/hub"/>
     <hyperlink ref="E5" r:id="rId5" display="sriganesh.d@i-exceed.com"/>
-    <hyperlink ref="P5" r:id="rId6" display="https://device.pcloudy.com/appiumcloud/wd/hub"/>
+    <hyperlink ref="Q5" r:id="rId6" display="https://device.pcloudy.com/appiumcloud/wd/hub"/>
     <hyperlink ref="E6" r:id="rId7" display="sriganesh.d@i-exceed.com"/>
-    <hyperlink ref="P6" r:id="rId8" display="https://device.pcloudy.com/appiumcloud/wd/hub"/>
+    <hyperlink ref="Q6" r:id="rId8" display="https://device.pcloudy.com/appiumcloud/wd/hub"/>
     <hyperlink ref="E7" r:id="rId9" display="sriganesh.d@i-exceed.com"/>
-    <hyperlink ref="P7" r:id="rId10" display="https://device.pcloudy.com/appiumcloud/wd/hub"/>
+    <hyperlink ref="Q7" r:id="rId10" display="https://device.pcloudy.com/appiumcloud/wd/hub"/>
     <hyperlink ref="E8" r:id="rId11" display="sriganesh.d@i-exceed.com"/>
-    <hyperlink ref="P8" r:id="rId12" display="https://device.pcloudy.com/appiumcloud/wd/hub"/>
+    <hyperlink ref="Q8" r:id="rId12" display="https://device.pcloudy.com/appiumcloud/wd/hub"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -21056,62 +21056,62 @@
   <sheetData>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="0" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="35" t="s">
-        <v>395</v>
+      <c r="B5" s="34" t="s">
+        <v>396</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="35" t="s">
-        <v>413</v>
+      <c r="B6" s="34" t="s">
+        <v>414</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="35" t="s">
-        <v>395</v>
+      <c r="B7" s="34" t="s">
+        <v>396</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="35" t="s">
-        <v>414</v>
+      <c r="B8" s="34" t="s">
+        <v>415</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="35" t="s">
-        <v>415</v>
+      <c r="B9" s="34" t="s">
+        <v>416</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="0" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="35" t="s">
-        <v>414</v>
+      <c r="B11" s="34" t="s">
+        <v>415</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="35" t="s">
-        <v>401</v>
+      <c r="B13" s="34" t="s">
+        <v>402</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="0" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="0" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="0" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -21120,33 +21120,33 @@
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="0" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="0" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="36" t="s">
-        <v>423</v>
-      </c>
-      <c r="F25" s="36" t="s">
+      <c r="B25" s="35" t="s">
         <v>424</v>
+      </c>
+      <c r="F25" s="35" t="s">
+        <v>425</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="0" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="0" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updating pcloudy connection class
</commit_message>
<xml_diff>
--- a/src/test/resources/DataSet/NMCO_ONB.xlsx
+++ b/src/test/resources/DataSet/NMCO_ONB.xlsx
@@ -20621,11 +20621,11 @@
   <dimension ref="A1:T9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="G8" activeCellId="0" sqref="G8"/>
+      <selection pane="topRight" activeCell="G1" activeCellId="0" sqref="G1"/>
+      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="J4" activeCellId="0" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
updating excel and test runner2
</commit_message>
<xml_diff>
--- a/src/test/resources/DataSet/NMCO_ONB.xlsx
+++ b/src/test/resources/DataSet/NMCO_ONB.xlsx
@@ -1212,7 +1212,7 @@
     <t xml:space="preserve">11.0.0</t>
   </si>
   <si>
-    <t xml:space="preserve">SAMSUNG_GalaxyTabS5e_Android_11.0.0_cb1ca</t>
+    <t xml:space="preserve">SAMSUNG_GalaxyTabS6_Android_11.0.0_383e3</t>
   </si>
   <si>
     <t xml:space="preserve">uiautomator2</t>
@@ -1258,10 +1258,10 @@
     <t xml:space="preserve">Android_003</t>
   </si>
   <si>
-    <t xml:space="preserve">SAMSUNG_GalaxyTabS6_Android_11.0.0_383e3</t>
-  </si>
-  <si>
     <t xml:space="preserve">Android_0003</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SAMSUNG_GalaxyTabS5e_Android_11.0.0_cb1ca</t>
   </si>
   <si>
     <t xml:space="preserve">IOS_001</t>
@@ -1332,7 +1332,7 @@
     <numFmt numFmtId="167" formatCode="@"/>
     <numFmt numFmtId="168" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
-  <fonts count="15">
+  <fonts count="16">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1421,6 +1421,12 @@
       <name val="JetBrains Mono"/>
       <family val="3"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF6A8759"/>
+      <name val="JetBrains Mono"/>
+      <family val="3"/>
     </font>
     <font>
       <sz val="12"/>
@@ -1519,7 +1525,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="37">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1640,6 +1646,10 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1652,7 +1662,7 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -20602,11 +20612,11 @@
   <dimension ref="A1:T9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="G6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="G1" activeCellId="0" sqref="G1"/>
-      <selection pane="bottomLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="I8" activeCellId="0" sqref="I8"/>
+      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="H4" activeCellId="0" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -20800,7 +20810,7 @@
       <c r="H4" s="8" t="s">
         <v>395</v>
       </c>
-      <c r="I4" s="8" t="s">
+      <c r="I4" s="30" t="s">
         <v>396</v>
       </c>
       <c r="J4" s="8" t="s">
@@ -20825,7 +20835,7 @@
       <c r="Q4" s="8" t="s">
         <v>401</v>
       </c>
-      <c r="R4" s="30" t="n">
+      <c r="R4" s="31" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -20855,7 +20865,7 @@
       <c r="H5" s="8" t="s">
         <v>395</v>
       </c>
-      <c r="I5" s="31" t="s">
+      <c r="I5" s="32" t="s">
         <v>403</v>
       </c>
       <c r="J5" s="8" t="s">
@@ -20880,7 +20890,7 @@
       <c r="Q5" s="8" t="s">
         <v>401</v>
       </c>
-      <c r="R5" s="30" t="n">
+      <c r="R5" s="31" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -20910,8 +20920,8 @@
       <c r="H6" s="8" t="s">
         <v>395</v>
       </c>
-      <c r="I6" s="31" t="s">
-        <v>405</v>
+      <c r="I6" s="32" t="s">
+        <v>396</v>
       </c>
       <c r="J6" s="8" t="s">
         <v>397</v>
@@ -20933,14 +20943,14 @@
       <c r="Q6" s="8" t="s">
         <v>401</v>
       </c>
-      <c r="R6" s="30" t="n">
+      <c r="R6" s="31" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="82.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="8" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="B7" s="8" t="s">
         <v>44</v>
@@ -20963,8 +20973,8 @@
       <c r="H7" s="8" t="s">
         <v>395</v>
       </c>
-      <c r="I7" s="31" t="s">
-        <v>396</v>
+      <c r="I7" s="32" t="s">
+        <v>406</v>
       </c>
       <c r="J7" s="8" t="s">
         <v>397</v>
@@ -20986,7 +20996,7 @@
       <c r="Q7" s="8" t="s">
         <v>401</v>
       </c>
-      <c r="R7" s="30" t="n">
+      <c r="R7" s="31" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -21001,7 +21011,7 @@
       <c r="C8" s="1" t="s">
         <v>391</v>
       </c>
-      <c r="D8" s="32" t="s">
+      <c r="D8" s="33" t="s">
         <v>408</v>
       </c>
       <c r="E8" s="29" t="s">
@@ -21013,29 +21023,29 @@
       <c r="G8" s="1" t="s">
         <v>382</v>
       </c>
-      <c r="H8" s="32" t="s">
+      <c r="H8" s="33" t="s">
         <v>409</v>
       </c>
       <c r="I8" s="8" t="s">
         <v>410</v>
       </c>
-      <c r="J8" s="31" t="s">
+      <c r="J8" s="32" t="s">
         <v>411</v>
       </c>
-      <c r="K8" s="31" t="s">
+      <c r="K8" s="32" t="s">
         <v>412</v>
       </c>
       <c r="L8" s="11"/>
       <c r="M8" s="1"/>
       <c r="N8" s="8"/>
-      <c r="O8" s="33"/>
+      <c r="O8" s="34"/>
       <c r="P8" s="1" t="n">
         <v>500</v>
       </c>
       <c r="Q8" s="8" t="s">
         <v>401</v>
       </c>
-      <c r="R8" s="30" t="n">
+      <c r="R8" s="31" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -21074,7 +21084,7 @@
   <dimension ref="B4:F27"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="91" zoomScaleNormal="91" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B24" activeCellId="0" sqref="B24"/>
+      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -21088,27 +21098,27 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="34" t="s">
-        <v>405</v>
+      <c r="B5" s="35" t="s">
+        <v>396</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="34" t="s">
+      <c r="B6" s="35" t="s">
         <v>414</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="34" t="s">
-        <v>405</v>
+      <c r="B7" s="35" t="s">
+        <v>396</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="34" t="s">
+      <c r="B8" s="35" t="s">
         <v>415</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="34" t="s">
+      <c r="B9" s="35" t="s">
         <v>416</v>
       </c>
     </row>
@@ -21118,13 +21128,13 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="34" t="s">
+      <c r="B11" s="35" t="s">
         <v>415</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="34" t="s">
-        <v>396</v>
+      <c r="B13" s="35" t="s">
+        <v>406</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -21160,10 +21170,10 @@
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="35" t="s">
+      <c r="B25" s="36" t="s">
         <v>410</v>
       </c>
-      <c r="F25" s="35" t="s">
+      <c r="F25" s="36" t="s">
         <v>409</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updating android url version 1.0.7
</commit_message>
<xml_diff>
--- a/src/test/resources/DataSet/NMCO_ONB.xlsx
+++ b/src/test/resources/DataSet/NMCO_ONB.xlsx
@@ -1221,26 +1221,7 @@
     <t xml:space="preserve">http://readuser:Re@d@1234@20.80.0.230:8082/artifactory/android-apk/ao/manual/qaRelease-1.0.5-06-12-2021-19:31.apk</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF067D17"/>
-        <rFont val="JetBrains Mono"/>
-        <family val="3"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Automation-1-0-6-13-12-2021</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF067D17"/>
-        <rFont val="JetBrains Mono"/>
-        <family val="3"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">.apk</t>
-    </r>
+    <t xml:space="preserve">Automation-1-0-7-21-12-2021.apk</t>
   </si>
   <si>
     <t xml:space="preserve">com.iexceed.assistedonboardingapp.assistedonboarding.AssistedOnboardingActivity</t>
@@ -1528,7 +1509,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="39">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1650,6 +1631,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -20619,11 +20604,11 @@
   <dimension ref="A1:T9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="G4" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G4" activeCellId="0" sqref="G4"/>
+      <selection pane="topRight" activeCell="G1" activeCellId="0" sqref="G1"/>
+      <selection pane="bottomLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="bottomRight" activeCell="I5" activeCellId="0" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -20792,7 +20777,7 @@
       </c>
       <c r="T3" s="29"/>
     </row>
-    <row r="4" customFormat="false" ht="109.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="108.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="8" t="s">
         <v>390</v>
       </c>
@@ -20826,7 +20811,7 @@
       <c r="K4" s="8" t="s">
         <v>398</v>
       </c>
-      <c r="L4" s="11" t="s">
+      <c r="L4" s="31" t="s">
         <v>399</v>
       </c>
       <c r="M4" s="25" t="s">
@@ -20842,7 +20827,7 @@
       <c r="Q4" s="8" t="s">
         <v>401</v>
       </c>
-      <c r="R4" s="31" t="n">
+      <c r="R4" s="32" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -20881,7 +20866,7 @@
       <c r="K5" s="8" t="s">
         <v>398</v>
       </c>
-      <c r="L5" s="11" t="s">
+      <c r="L5" s="31" t="s">
         <v>399</v>
       </c>
       <c r="M5" s="25" t="s">
@@ -20897,7 +20882,7 @@
       <c r="Q5" s="8" t="s">
         <v>401</v>
       </c>
-      <c r="R5" s="31" t="n">
+      <c r="R5" s="32" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -20927,14 +20912,14 @@
       <c r="H6" s="8" t="s">
         <v>395</v>
       </c>
-      <c r="I6" s="32" t="s">
+      <c r="I6" s="33" t="s">
         <v>406</v>
       </c>
       <c r="J6" s="8" t="s">
         <v>397</v>
       </c>
       <c r="K6" s="8"/>
-      <c r="L6" s="11" t="s">
+      <c r="L6" s="31" t="s">
         <v>399</v>
       </c>
       <c r="M6" s="25" t="s">
@@ -20950,7 +20935,7 @@
       <c r="Q6" s="8" t="s">
         <v>401</v>
       </c>
-      <c r="R6" s="31" t="n">
+      <c r="R6" s="32" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -20980,14 +20965,14 @@
       <c r="H7" s="8" t="s">
         <v>395</v>
       </c>
-      <c r="I7" s="32" t="s">
+      <c r="I7" s="33" t="s">
         <v>406</v>
       </c>
       <c r="J7" s="8" t="s">
         <v>397</v>
       </c>
       <c r="K7" s="8"/>
-      <c r="L7" s="11" t="s">
+      <c r="L7" s="31" t="s">
         <v>399</v>
       </c>
       <c r="M7" s="25" t="s">
@@ -21003,7 +20988,7 @@
       <c r="Q7" s="8" t="s">
         <v>401</v>
       </c>
-      <c r="R7" s="31" t="n">
+      <c r="R7" s="32" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -21018,7 +21003,7 @@
       <c r="C8" s="1" t="s">
         <v>391</v>
       </c>
-      <c r="D8" s="33" t="s">
+      <c r="D8" s="34" t="s">
         <v>409</v>
       </c>
       <c r="E8" s="30" t="s">
@@ -21030,29 +21015,29 @@
       <c r="G8" s="1" t="s">
         <v>382</v>
       </c>
-      <c r="H8" s="33" t="s">
+      <c r="H8" s="34" t="s">
         <v>410</v>
       </c>
       <c r="I8" s="8" t="s">
         <v>411</v>
       </c>
-      <c r="J8" s="32" t="s">
+      <c r="J8" s="33" t="s">
         <v>412</v>
       </c>
-      <c r="K8" s="32" t="s">
+      <c r="K8" s="33" t="s">
         <v>413</v>
       </c>
       <c r="L8" s="11"/>
       <c r="M8" s="1"/>
       <c r="N8" s="8"/>
-      <c r="O8" s="34"/>
+      <c r="O8" s="35"/>
       <c r="P8" s="1" t="n">
         <v>500</v>
       </c>
       <c r="Q8" s="8" t="s">
         <v>401</v>
       </c>
-      <c r="R8" s="31" t="n">
+      <c r="R8" s="32" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -21076,19 +21061,19 @@
       <c r="F9" s="30" t="s">
         <v>394</v>
       </c>
-      <c r="G9" s="33" t="s">
+      <c r="G9" s="34" t="s">
         <v>382</v>
       </c>
-      <c r="H9" s="33" t="s">
+      <c r="H9" s="34" t="s">
         <v>415</v>
       </c>
       <c r="I9" s="8" t="s">
         <v>416</v>
       </c>
-      <c r="J9" s="32" t="s">
+      <c r="J9" s="33" t="s">
         <v>412</v>
       </c>
-      <c r="K9" s="35" t="s">
+      <c r="K9" s="36" t="s">
         <v>413</v>
       </c>
       <c r="P9" s="1" t="n">
@@ -21097,7 +21082,7 @@
       <c r="Q9" s="8" t="s">
         <v>401</v>
       </c>
-      <c r="R9" s="31" t="n">
+      <c r="R9" s="32" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -21151,27 +21136,27 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="36" t="s">
+      <c r="B5" s="37" t="s">
         <v>406</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="36" t="s">
+      <c r="B6" s="37" t="s">
         <v>418</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="36" t="s">
+      <c r="B7" s="37" t="s">
         <v>406</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="36" t="s">
+      <c r="B8" s="37" t="s">
         <v>419</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="36" t="s">
+      <c r="B9" s="37" t="s">
         <v>420</v>
       </c>
     </row>
@@ -21181,12 +21166,12 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="36" t="s">
+      <c r="B11" s="37" t="s">
         <v>419</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="36" t="s">
+      <c r="B13" s="37" t="s">
         <v>396</v>
       </c>
     </row>
@@ -21223,10 +21208,10 @@
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="37" t="s">
+      <c r="B25" s="38" t="s">
         <v>411</v>
       </c>
-      <c r="F25" s="37" t="s">
+      <c r="F25" s="38" t="s">
         <v>410</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updating ios step def for updating dynamic url in excel for each build
</commit_message>
<xml_diff>
--- a/src/test/resources/DataSet/NMCO_ONB.xlsx
+++ b/src/test/resources/DataSet/NMCO_ONB.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2737" uniqueCount="433">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2731" uniqueCount="432">
   <si>
     <t xml:space="preserve">TestCaseName</t>
   </si>
@@ -1224,6 +1224,9 @@
     <t xml:space="preserve">http://readuser:Re@d@1234@20.80.0.230:8082/artifactory/android-apk/ao/manual/qaRelease-1.0.5-06-12-2021-19:31.apk</t>
   </si>
   <si>
+    <t xml:space="preserve">https://readuser:Re@d@1234@artifactory.appzillon.com/artifactory/android-apk/ao/manual/qaRelease-1.0.7-21-12-2021-15:37.apk</t>
+  </si>
+  <si>
     <t xml:space="preserve">Automation-1-0-7-21-12-2021.apk</t>
   </si>
   <si>
@@ -1315,12 +1318,6 @@
   </si>
   <si>
     <t xml:space="preserve">APPLE_iPhoneX_iOS_14.0.0_1b718</t>
-  </si>
-  <si>
-    <t>di</t>
-  </si>
-  <si>
-    <t>https://readuser:Re@d@1234@artifactory.appzillon.com/artifactory/android-apk/ao/manual/qaRelease-1.0.7-21-12-2021-15:37.apk</t>
   </si>
 </sst>
 </file>
@@ -1334,7 +1331,7 @@
     <numFmt numFmtId="167" formatCode="@"/>
     <numFmt numFmtId="168" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
-  <fonts count="17">
+  <fonts count="13">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1397,13 +1394,6 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="13.5"/>
-      <color rgb="FF000000"/>
-      <name val="JetBrains Mono"/>
-      <family val="3"/>
-      <charset val="1"/>
-    </font>
-    <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="JetBrains Mono"/>
@@ -1425,27 +1415,8 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="12"/>
       <color rgb="FF067D17"/>
-      <name val="JetBrains Mono"/>
-      <family val="3"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF067D17"/>
-      <name val="JetBrains Mono"/>
-      <family val="3"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF808080"/>
       <name val="JetBrains Mono"/>
       <family val="3"/>
       <charset val="1"/>
@@ -1533,7 +1504,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="36">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1622,15 +1593,7 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1638,11 +1601,11 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1654,15 +1617,11 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1670,11 +1629,7 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1682,15 +1637,11 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1720,11 +1671,11 @@
       <rgbColor rgb="FF800000"/>
       <rgbColor rgb="FF067D17"/>
       <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FF6A8759"/>
+      <rgbColor rgb="FF808000"/>
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF008080"/>
       <rgbColor rgb="FFB4C7DC"/>
-      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF6A8759"/>
       <rgbColor rgb="FF9999FF"/>
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FFFFFFCC"/>
@@ -1785,56 +1736,56 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" customWidth="true" hidden="false" style="1" width="32.3" collapsed="true" outlineLevel="0"/>
-    <col min="2" max="2" customWidth="true" hidden="false" style="1" width="12.85" collapsed="true" outlineLevel="0"/>
-    <col min="3" max="3" customWidth="true" hidden="false" style="1" width="4.43" collapsed="true" outlineLevel="0"/>
-    <col min="4" max="4" customWidth="true" hidden="false" style="1" width="7.83" collapsed="true" outlineLevel="0"/>
-    <col min="5" max="6" customWidth="true" hidden="false" style="1" width="11.9" collapsed="true" outlineLevel="0"/>
-    <col min="7" max="8" customWidth="true" hidden="false" style="1" width="15.54" collapsed="true" outlineLevel="0"/>
-    <col min="9" max="9" customWidth="true" hidden="false" style="1" width="17.31" collapsed="true" outlineLevel="0"/>
-    <col min="10" max="10" customWidth="true" hidden="false" style="1" width="16.2" collapsed="true" outlineLevel="0"/>
-    <col min="11" max="11" customWidth="true" hidden="false" style="2" width="22.49" collapsed="true" outlineLevel="0"/>
-    <col min="12" max="12" customWidth="true" hidden="false" style="1" width="22.49" collapsed="true" outlineLevel="0"/>
-    <col min="13" max="13" customWidth="true" hidden="false" style="1" width="17.86" collapsed="true" outlineLevel="0"/>
-    <col min="14" max="14" customWidth="true" hidden="false" style="1" width="16.2" collapsed="true" outlineLevel="0"/>
-    <col min="15" max="15" customWidth="true" hidden="false" style="1" width="15.21" collapsed="true" outlineLevel="0"/>
-    <col min="16" max="16" customWidth="true" hidden="false" style="1" width="13.78" collapsed="true" outlineLevel="0"/>
-    <col min="17" max="17" customWidth="true" hidden="false" style="1" width="13.56" collapsed="true" outlineLevel="0"/>
-    <col min="18" max="18" customWidth="true" hidden="false" style="1" width="24.43" collapsed="true" outlineLevel="0"/>
-    <col min="19" max="19" customWidth="true" hidden="false" style="1" width="20.28" collapsed="true" outlineLevel="0"/>
-    <col min="20" max="20" customWidth="true" hidden="false" style="1" width="14.11" collapsed="true" outlineLevel="0"/>
-    <col min="21" max="21" customWidth="true" hidden="false" style="2" width="19.51" collapsed="true" outlineLevel="0"/>
-    <col min="22" max="22" customWidth="true" hidden="false" style="2" width="21.17" collapsed="true" outlineLevel="0"/>
-    <col min="23" max="23" customWidth="true" hidden="false" style="1" width="14.99" collapsed="true" outlineLevel="0"/>
-    <col min="24" max="25" customWidth="true" hidden="false" style="1" width="19.51" collapsed="true" outlineLevel="0"/>
-    <col min="26" max="26" customWidth="true" hidden="false" style="1" width="24.36" collapsed="true" outlineLevel="0"/>
-    <col min="27" max="27" customWidth="true" hidden="false" style="1" width="14.11" collapsed="true" outlineLevel="0"/>
-    <col min="28" max="28" customWidth="true" hidden="false" style="1" width="18.85" collapsed="true" outlineLevel="0"/>
-    <col min="29" max="29" customWidth="true" hidden="false" style="1" width="19.95" collapsed="true" outlineLevel="0"/>
-    <col min="30" max="31" customWidth="true" hidden="false" style="1" width="21.04" collapsed="true" outlineLevel="0"/>
-    <col min="32" max="32" customWidth="true" hidden="false" style="1" width="22.49" collapsed="true" outlineLevel="0"/>
-    <col min="33" max="33" customWidth="true" hidden="false" style="1" width="20.94" collapsed="true" outlineLevel="0"/>
-    <col min="34" max="34" customWidth="true" hidden="false" style="1" width="20.28" collapsed="true" outlineLevel="0"/>
-    <col min="35" max="35" customWidth="true" hidden="false" style="1" width="21.04" collapsed="true" outlineLevel="0"/>
-    <col min="36" max="37" customWidth="true" hidden="false" style="1" width="19.4" collapsed="true" outlineLevel="0"/>
-    <col min="38" max="38" customWidth="true" hidden="false" style="1" width="18.3" collapsed="true" outlineLevel="0"/>
-    <col min="39" max="39" customWidth="true" hidden="false" style="1" width="19.95" collapsed="true" outlineLevel="0"/>
-    <col min="40" max="40" customWidth="true" hidden="false" style="2" width="20.84" collapsed="true" outlineLevel="0"/>
-    <col min="41" max="41" customWidth="true" hidden="false" style="3" width="32.74" collapsed="true" outlineLevel="0"/>
-    <col min="42" max="42" customWidth="true" hidden="false" style="1" width="22.04" collapsed="true" outlineLevel="0"/>
-    <col min="43" max="43" customWidth="true" hidden="false" style="1" width="8.57" collapsed="true" outlineLevel="0"/>
-    <col min="44" max="44" customWidth="true" hidden="false" style="1" width="20.94" collapsed="true" outlineLevel="0"/>
-    <col min="45" max="45" customWidth="true" hidden="false" style="1" width="15.11" collapsed="true" outlineLevel="0"/>
-    <col min="46" max="46" customWidth="true" hidden="false" style="1" width="19.18" collapsed="true" outlineLevel="0"/>
-    <col min="47" max="47" customWidth="true" hidden="false" style="1" width="16.74" collapsed="true" outlineLevel="0"/>
-    <col min="48" max="48" customWidth="true" hidden="false" style="3" width="14.0" collapsed="true" outlineLevel="0"/>
-    <col min="49" max="49" customWidth="true" hidden="false" style="3" width="16.11" collapsed="true" outlineLevel="0"/>
-    <col min="50" max="50" customWidth="true" hidden="false" style="1" width="12.35" collapsed="true" outlineLevel="0"/>
-    <col min="51" max="52" customWidth="true" hidden="false" style="1" width="17.64" collapsed="true" outlineLevel="0"/>
-    <col min="53" max="53" customWidth="true" hidden="false" style="1" width="18.08" collapsed="true" outlineLevel="0"/>
-    <col min="54" max="54" customWidth="true" hidden="false" style="2" width="18.08" collapsed="true" outlineLevel="0"/>
-    <col min="55" max="990" customWidth="true" hidden="false" style="1" width="8.57" collapsed="true" outlineLevel="0"/>
-    <col min="991" max="1025" customWidth="true" hidden="false" style="0" width="9.14" collapsed="true" outlineLevel="0"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="32.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="12.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="4.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="7.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="1" width="11.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="1" width="15.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="17.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="16.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="2" width="22.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="22.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="17.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="16.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="15.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="13.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="13.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="24.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="1" width="20.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="1" width="14.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="2" width="19.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="2" width="21.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="1" width="14.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="24" style="1" width="19.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="1" width="24.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="1" width="14.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="1" width="18.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="1" width="19.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="30" style="1" width="21.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="32" style="1" width="22.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="33" style="1" width="20.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="34" min="34" style="1" width="20.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="35" min="35" style="1" width="21.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="37" min="36" style="1" width="19.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="38" min="38" style="1" width="18.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="39" min="39" style="1" width="19.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="40" min="40" style="2" width="20.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="41" min="41" style="3" width="32.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="42" min="42" style="1" width="22.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="43" min="43" style="1" width="8.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="44" min="44" style="1" width="20.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="45" min="45" style="1" width="15.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="46" min="46" style="1" width="19.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="47" min="47" style="1" width="16.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="48" min="48" style="3" width="14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="49" min="49" style="3" width="16.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="50" min="50" style="1" width="12.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="52" min="51" style="1" width="17.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="53" min="53" style="1" width="18.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="54" min="54" style="2" width="18.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="990" min="55" style="1" width="8.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="991" style="0" width="9.14"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -20636,31 +20587,31 @@
   <dimension ref="A1:U9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="topRight" activeCell="F1" activeCellId="0" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A6" activeCellId="0" sqref="A6"/>
+      <selection pane="bottomRight" activeCell="L10" activeCellId="0" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" customWidth="true" hidden="false" style="17" width="12.57" collapsed="true" outlineLevel="0"/>
-    <col min="2" max="2" customWidth="true" hidden="false" style="17" width="5.18" collapsed="true" outlineLevel="0"/>
-    <col min="3" max="4" customWidth="true" hidden="false" style="17" width="9.17" collapsed="true" outlineLevel="0"/>
-    <col min="5" max="5" customWidth="true" hidden="false" style="17" width="19.4" collapsed="true" outlineLevel="0"/>
-    <col min="6" max="6" customWidth="true" hidden="false" style="17" width="20.5" collapsed="true" outlineLevel="0"/>
-    <col min="7" max="7" customWidth="true" hidden="false" style="17" width="15.11" collapsed="true" outlineLevel="0"/>
-    <col min="8" max="8" customWidth="true" hidden="false" style="17" width="9.17" collapsed="true" outlineLevel="0"/>
-    <col min="9" max="9" customWidth="true" hidden="false" style="17" width="18.85" collapsed="true" outlineLevel="0"/>
-    <col min="10" max="10" customWidth="true" hidden="false" style="17" width="9.17" collapsed="true" outlineLevel="0"/>
-    <col min="11" max="11" customWidth="true" hidden="false" style="17" width="17.86" collapsed="true" outlineLevel="0"/>
-    <col min="12" max="13" customWidth="true" hidden="false" style="17" width="14.87" collapsed="true" outlineLevel="0"/>
-    <col min="14" max="14" customWidth="true" hidden="false" style="17" width="19.18" collapsed="true" outlineLevel="0"/>
-    <col min="15" max="15" customWidth="true" hidden="false" style="17" width="26.35" collapsed="true" outlineLevel="0"/>
-    <col min="16" max="17" customWidth="true" hidden="false" style="17" width="9.17" collapsed="true" outlineLevel="0"/>
-    <col min="18" max="18" customWidth="true" hidden="false" style="17" width="29.45" collapsed="true" outlineLevel="0"/>
-    <col min="19" max="1025" customWidth="true" hidden="false" style="17" width="9.17" collapsed="true" outlineLevel="0"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="17" width="12.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="17" width="5.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="17" width="9.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="17" width="19.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="17" width="20.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="17" width="15.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="17" width="9.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="17" width="18.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="17" width="9.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="17" width="17.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="12" style="17" width="14.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="17" width="19.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="17" width="26.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="16" style="17" width="9.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="17" width="29.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="19" style="17" width="9.17"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -20735,35 +20686,28 @@
       <c r="D2" s="21" t="s">
         <v>382</v>
       </c>
-      <c r="E2"/>
-      <c r="F2"/>
       <c r="G2" s="21" t="s">
         <v>383</v>
       </c>
-      <c r="H2"/>
       <c r="I2" s="21" t="s">
         <v>384</v>
       </c>
-      <c r="J2" s="23" t="s">
+      <c r="J2" s="22" t="s">
         <v>385</v>
       </c>
-      <c r="K2"/>
-      <c r="L2"/>
-      <c r="M2"/>
-      <c r="N2" s="25" t="s">
+      <c r="N2" s="23" t="s">
         <v>386</v>
       </c>
       <c r="O2" s="11" t="s">
         <v>387</v>
       </c>
-      <c r="P2"/>
-      <c r="Q2" s="23" t="n">
+      <c r="Q2" s="22" t="n">
         <v>500</v>
       </c>
-      <c r="R2" s="26" t="s">
+      <c r="R2" s="24" t="s">
         <v>388</v>
       </c>
-      <c r="S2" s="23" t="n">
+      <c r="S2" s="22" t="n">
         <v>0</v>
       </c>
     </row>
@@ -20780,39 +20724,32 @@
       <c r="D3" s="20" t="s">
         <v>382</v>
       </c>
-      <c r="E3"/>
-      <c r="F3"/>
       <c r="G3" s="20" t="s">
         <v>383</v>
       </c>
-      <c r="H3"/>
-      <c r="I3" s="27" t="s">
+      <c r="I3" s="25" t="s">
         <v>390</v>
       </c>
-      <c r="J3" s="27" t="s">
+      <c r="J3" s="25" t="s">
         <v>385</v>
       </c>
-      <c r="K3"/>
-      <c r="L3"/>
-      <c r="M3"/>
-      <c r="N3" s="25" t="s">
+      <c r="N3" s="23" t="s">
         <v>386</v>
       </c>
       <c r="O3" s="11" t="s">
         <v>387</v>
       </c>
-      <c r="P3"/>
       <c r="Q3" s="20" t="n">
         <v>103</v>
       </c>
-      <c r="R3" s="27" t="s">
+      <c r="R3" s="25" t="s">
         <v>388</v>
       </c>
-      <c r="S3" s="28" t="b">
+      <c r="S3" s="26" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="U3" s="29"/>
+      <c r="U3" s="27"/>
     </row>
     <row r="4" customFormat="false" ht="108.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="8" t="s">
@@ -20827,10 +20764,10 @@
       <c r="D4" s="8" t="s">
         <v>393</v>
       </c>
-      <c r="E4" s="30" t="s">
+      <c r="E4" s="28" t="s">
         <v>394</v>
       </c>
-      <c r="F4" s="30" t="s">
+      <c r="F4" s="28" t="s">
         <v>395</v>
       </c>
       <c r="G4" s="1" t="s">
@@ -20839,7 +20776,7 @@
       <c r="H4" s="8" t="s">
         <v>396</v>
       </c>
-      <c r="I4" s="31" t="s">
+      <c r="I4" s="8" t="s">
         <v>397</v>
       </c>
       <c r="J4" s="8" t="s">
@@ -20848,33 +20785,32 @@
       <c r="K4" s="8" t="s">
         <v>399</v>
       </c>
-      <c r="L4" t="s">
-        <v>432</v>
-      </c>
-      <c r="M4" s="32" t="s">
+      <c r="L4" s="17" t="s">
         <v>400</v>
       </c>
-      <c r="N4" s="25" t="s">
+      <c r="M4" s="29" t="s">
         <v>401</v>
+      </c>
+      <c r="N4" s="23" t="s">
+        <v>402</v>
       </c>
       <c r="O4" s="11" t="s">
         <v>387</v>
       </c>
-      <c r="P4"/>
       <c r="Q4" s="20" t="n">
         <v>306</v>
       </c>
       <c r="R4" s="8" t="s">
-        <v>402</v>
-      </c>
-      <c r="S4" s="33" t="b">
+        <v>403</v>
+      </c>
+      <c r="S4" s="30" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="108.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="8" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="B5" s="8" t="s">
         <v>44</v>
@@ -20885,20 +20821,20 @@
       <c r="D5" s="8" t="s">
         <v>393</v>
       </c>
-      <c r="E5" s="30" t="s">
+      <c r="E5" s="28" t="s">
         <v>394</v>
       </c>
-      <c r="F5" s="30" t="s">
+      <c r="F5" s="28" t="s">
         <v>395</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>383</v>
       </c>
       <c r="H5" s="8" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="I5" s="8" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="J5" s="8" t="s">
         <v>398</v>
@@ -20906,31 +20842,29 @@
       <c r="K5" s="8" t="s">
         <v>399</v>
       </c>
-      <c r="L5"/>
-      <c r="M5" s="32" t="s">
-        <v>400</v>
-      </c>
-      <c r="N5" s="25" t="s">
+      <c r="M5" s="29" t="s">
         <v>401</v>
+      </c>
+      <c r="N5" s="23" t="s">
+        <v>402</v>
       </c>
       <c r="O5" s="11" t="s">
         <v>387</v>
       </c>
-      <c r="P5"/>
       <c r="Q5" s="20" t="n">
         <v>307</v>
       </c>
       <c r="R5" s="8" t="s">
-        <v>402</v>
-      </c>
-      <c r="S5" s="33" t="b">
+        <v>403</v>
+      </c>
+      <c r="S5" s="30" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="102.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="8" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="B6" s="8" t="s">
         <v>44</v>
@@ -20941,10 +20875,10 @@
       <c r="D6" s="8" t="s">
         <v>393</v>
       </c>
-      <c r="E6" s="30" t="s">
+      <c r="E6" s="28" t="s">
         <v>394</v>
       </c>
-      <c r="F6" s="30" t="s">
+      <c r="F6" s="28" t="s">
         <v>395</v>
       </c>
       <c r="G6" s="1" t="s">
@@ -20953,40 +20887,38 @@
       <c r="H6" s="8" t="s">
         <v>396</v>
       </c>
-      <c r="I6" s="31" t="s">
+      <c r="I6" s="8" t="s">
         <v>397</v>
       </c>
       <c r="J6" s="8" t="s">
         <v>398</v>
       </c>
-      <c r="K6"/>
-      <c r="L6" s="34" t="s">
-        <v>407</v>
-      </c>
-      <c r="M6" s="32" t="s">
-        <v>400</v>
-      </c>
-      <c r="N6" s="25" t="s">
+      <c r="L6" s="11" t="s">
+        <v>408</v>
+      </c>
+      <c r="M6" s="29" t="s">
         <v>401</v>
+      </c>
+      <c r="N6" s="23" t="s">
+        <v>402</v>
       </c>
       <c r="O6" s="11" t="s">
         <v>387</v>
       </c>
-      <c r="P6"/>
       <c r="Q6" s="20" t="n">
         <v>106</v>
       </c>
       <c r="R6" s="8" t="s">
-        <v>402</v>
-      </c>
-      <c r="S6" s="33" t="b">
+        <v>403</v>
+      </c>
+      <c r="S6" s="30" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="82.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="8" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="B7" s="8" t="s">
         <v>44</v>
@@ -20997,10 +20929,10 @@
       <c r="D7" s="8" t="s">
         <v>393</v>
       </c>
-      <c r="E7" s="30" t="s">
+      <c r="E7" s="28" t="s">
         <v>394</v>
       </c>
-      <c r="F7" s="30" t="s">
+      <c r="F7" s="28" t="s">
         <v>395</v>
       </c>
       <c r="G7" s="1" t="s">
@@ -21009,38 +20941,35 @@
       <c r="H7" s="8" t="s">
         <v>396</v>
       </c>
-      <c r="I7" s="35" t="s">
-        <v>409</v>
+      <c r="I7" s="31" t="s">
+        <v>410</v>
       </c>
       <c r="J7" s="8" t="s">
         <v>398</v>
       </c>
-      <c r="K7"/>
-      <c r="L7"/>
-      <c r="M7" s="32" t="s">
-        <v>400</v>
-      </c>
-      <c r="N7" s="25" t="s">
+      <c r="M7" s="29" t="s">
+        <v>401</v>
+      </c>
+      <c r="N7" s="23" t="s">
         <v>386</v>
       </c>
       <c r="O7" s="11" t="s">
         <v>387</v>
       </c>
-      <c r="P7"/>
       <c r="Q7" s="20" t="n">
         <v>306</v>
       </c>
       <c r="R7" s="8" t="s">
-        <v>402</v>
-      </c>
-      <c r="S7" s="33" t="b">
+        <v>403</v>
+      </c>
+      <c r="S7" s="30" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="106.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="8" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="B8" s="8" t="s">
         <v>44</v>
@@ -21048,49 +20977,44 @@
       <c r="C8" s="1" t="s">
         <v>392</v>
       </c>
-      <c r="D8" s="36" t="s">
-        <v>411</v>
-      </c>
-      <c r="E8" s="30" t="s">
+      <c r="D8" s="32" t="s">
+        <v>412</v>
+      </c>
+      <c r="E8" s="28" t="s">
         <v>394</v>
       </c>
-      <c r="F8" s="30" t="s">
+      <c r="F8" s="28" t="s">
         <v>395</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>383</v>
       </c>
-      <c r="H8" s="36" t="s">
-        <v>412</v>
-      </c>
-      <c r="I8" s="31" t="s">
+      <c r="H8" s="32" t="s">
         <v>413</v>
       </c>
-      <c r="J8" s="35" t="s">
+      <c r="I8" s="8" t="s">
         <v>414</v>
       </c>
-      <c r="K8" s="35" t="s">
+      <c r="J8" s="31" t="s">
         <v>415</v>
       </c>
-      <c r="L8"/>
-      <c r="M8"/>
-      <c r="N8"/>
-      <c r="O8"/>
-      <c r="P8"/>
+      <c r="K8" s="31" t="s">
+        <v>416</v>
+      </c>
       <c r="Q8" s="1" t="n">
         <v>500</v>
       </c>
       <c r="R8" s="8" t="s">
-        <v>402</v>
-      </c>
-      <c r="S8" s="33" t="b">
+        <v>403</v>
+      </c>
+      <c r="S8" s="30" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="82.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="17" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="B9" s="17" t="s">
         <v>44</v>
@@ -21099,41 +21023,36 @@
         <v>392</v>
       </c>
       <c r="D9" s="17" t="s">
-        <v>411</v>
-      </c>
-      <c r="E9" s="30" t="s">
+        <v>412</v>
+      </c>
+      <c r="E9" s="28" t="s">
         <v>394</v>
       </c>
-      <c r="F9" s="30" t="s">
+      <c r="F9" s="28" t="s">
         <v>395</v>
       </c>
-      <c r="G9" s="36" t="s">
+      <c r="G9" s="32" t="s">
         <v>383</v>
       </c>
-      <c r="H9" s="36" t="s">
-        <v>417</v>
+      <c r="H9" s="32" t="s">
+        <v>418</v>
       </c>
       <c r="I9" s="8" t="s">
-        <v>418</v>
-      </c>
-      <c r="J9" s="35" t="s">
-        <v>414</v>
-      </c>
-      <c r="K9" s="38" t="s">
+        <v>419</v>
+      </c>
+      <c r="J9" s="31" t="s">
         <v>415</v>
       </c>
-      <c r="L9"/>
-      <c r="M9"/>
-      <c r="N9"/>
-      <c r="O9"/>
-      <c r="P9"/>
+      <c r="K9" s="33" t="s">
+        <v>416</v>
+      </c>
       <c r="Q9" s="1" t="n">
         <v>501</v>
       </c>
       <c r="R9" s="8" t="s">
-        <v>402</v>
-      </c>
-      <c r="S9" s="33" t="b">
+        <v>403</v>
+      </c>
+      <c r="S9" s="30" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -21178,7 +21097,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1025" customWidth="true" hidden="false" style="0" width="9.14" collapsed="true" outlineLevel="0"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="9.14"/>
   </cols>
   <sheetData>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -21187,58 +21106,58 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="39" t="s">
-        <v>409</v>
+      <c r="B5" s="34" t="s">
+        <v>410</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="39" t="s">
-        <v>419</v>
+      <c r="B6" s="34" t="s">
+        <v>420</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="39" t="s">
-        <v>409</v>
+      <c r="B7" s="34" t="s">
+        <v>410</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="39" t="s">
-        <v>420</v>
+      <c r="B8" s="34" t="s">
+        <v>421</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="39" t="s">
-        <v>421</v>
+      <c r="B9" s="34" t="s">
+        <v>422</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="0" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="39" t="s">
-        <v>420</v>
+      <c r="B11" s="34" t="s">
+        <v>421</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="39" t="s">
-        <v>422</v>
+      <c r="B13" s="34" t="s">
+        <v>423</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="0" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="0" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="0" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -21247,38 +21166,38 @@
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="0" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="0" t="s">
+        <v>414</v>
+      </c>
+      <c r="F24" s="0" t="s">
         <v>413</v>
       </c>
-      <c r="F24" s="0" t="s">
-        <v>412</v>
-      </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="40" t="s">
-        <v>427</v>
-      </c>
-      <c r="F25" s="40" t="s">
+      <c r="B25" s="35" t="s">
         <v>428</v>
+      </c>
+      <c r="F25" s="35" t="s">
+        <v>429</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="0" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="0" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="0" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updating pom file and feature files
</commit_message>
<xml_diff>
--- a/src/test/resources/DataSet/NMCO_ONB.xlsx
+++ b/src/test/resources/DataSet/NMCO_ONB.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2734" uniqueCount="434">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2777" uniqueCount="434">
   <si>
     <t xml:space="preserve">TestCaseName</t>
   </si>
@@ -1323,7 +1323,7 @@
     <t xml:space="preserve">APPLE_iPhoneX_iOS_14.0.0_1b718</t>
   </si>
   <si>
-    <t>https://readuser:Re@d@1234@artifactory.appzillon.com/artifactory/android-apk/ao/manual/qaRelease-1.0.7-21-12-2021-15:37.apk</t>
+    <t>https://artifactory.appzillon.com/artifactory/android-apk/ao/manual/qaRelease-1.0.7-21-12-2021-15:37.apk</t>
   </si>
 </sst>
 </file>
@@ -1337,7 +1337,7 @@
     <numFmt numFmtId="167" formatCode="@"/>
     <numFmt numFmtId="168" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
-  <fonts count="14">
+  <fonts count="13">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1427,12 +1427,6 @@
       <family val="3"/>
       <charset val="1"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -1516,7 +1510,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="36">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1647,10 +1641,6 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -20603,11 +20593,11 @@
   <dimension ref="A1:U9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="F6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B6" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="F1" activeCellId="0" sqref="F1"/>
+      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="I8" activeCellId="0" sqref="I8"/>
+      <selection pane="bottomRight" activeCell="A7" activeCellId="0" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -20897,7 +20887,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="46.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="108.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="8" t="s">
         <v>408</v>
       </c>
@@ -20928,7 +20918,9 @@
       <c r="J6" s="8" t="s">
         <v>398</v>
       </c>
-      <c r="K6"/>
+      <c r="K6" s="8" t="s">
+        <v>399</v>
+      </c>
       <c r="L6" s="11" t="s">
         <v>409</v>
       </c>
@@ -20984,8 +20976,12 @@
       <c r="J7" s="8" t="s">
         <v>398</v>
       </c>
-      <c r="K7"/>
-      <c r="L7"/>
+      <c r="K7" s="8" t="s">
+        <v>399</v>
+      </c>
+      <c r="L7" t="s">
+        <v>433</v>
+      </c>
       <c r="M7" s="29" t="s">
         <v>401</v>
       </c>
@@ -21032,7 +21028,7 @@
       <c r="H8" s="32" t="s">
         <v>414</v>
       </c>
-      <c r="I8" s="33" t="s">
+      <c r="I8" s="8" t="s">
         <v>415</v>
       </c>
       <c r="J8" s="31" t="s">
@@ -21088,7 +21084,7 @@
       <c r="J9" s="31" t="s">
         <v>416</v>
       </c>
-      <c r="K9" s="34" t="s">
+      <c r="K9" s="33" t="s">
         <v>417</v>
       </c>
       <c r="L9"/>
@@ -21158,27 +21154,27 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="35" t="s">
+      <c r="B5" s="34" t="s">
         <v>411</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="35" t="s">
+      <c r="B6" s="34" t="s">
         <v>421</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="35" t="s">
+      <c r="B7" s="34" t="s">
         <v>411</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="35" t="s">
+      <c r="B8" s="34" t="s">
         <v>422</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="35" t="s">
+      <c r="B9" s="34" t="s">
         <v>423</v>
       </c>
     </row>
@@ -21188,12 +21184,12 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="35" t="s">
+      <c r="B11" s="34" t="s">
         <v>422</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="35" t="s">
+      <c r="B13" s="34" t="s">
         <v>424</v>
       </c>
     </row>
@@ -21230,10 +21226,10 @@
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="36" t="s">
+      <c r="B25" s="35" t="s">
         <v>415</v>
       </c>
-      <c r="F25" s="36" t="s">
+      <c r="F25" s="35" t="s">
         <v>414</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updating pom file with sonar version
</commit_message>
<xml_diff>
--- a/src/test/resources/DataSet/NMCO_ONB.xlsx
+++ b/src/test/resources/DataSet/NMCO_ONB.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2735" uniqueCount="434">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2796" uniqueCount="436">
   <si>
     <t xml:space="preserve">TestCaseName</t>
   </si>
@@ -1257,33 +1257,36 @@
     <t xml:space="preserve">Android_0003</t>
   </si>
   <si>
+    <t xml:space="preserve">10.0.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IOS_001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ios</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13.3.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">APPLE_iPhoneSE_iOS_13.5.1_c982c</t>
+  </si>
+  <si>
+    <t xml:space="preserve">XCUITest</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://readuser:Re@d@1234@artifactory.appzillon.com/artifactory/iOS-ipa/ao/automated/AUTOMATIONDebug-1.0.0-13-12-2021-13%3A29/AUTOMATIONDebug-1.0.0-13-12-2021-13%3A29.ipa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IOS_02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">APPLE_iPhoneXS_iOS_14.1.0_21d51</t>
+  </si>
+  <si>
     <t xml:space="preserve">SAMSUNG_GalaxyTabS6_Android_11.0.0_383e3</t>
   </si>
   <si>
-    <t xml:space="preserve">IOS_001</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ios</t>
-  </si>
-  <si>
-    <t xml:space="preserve">13.3.1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">APPLE_iPhoneSE_iOS_13.5.1_c982c</t>
-  </si>
-  <si>
-    <t xml:space="preserve">XCUITest</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://readuser:Re@d@1234@artifactory.appzillon.com/artifactory/iOS-ipa/ao/automated/AUTOMATIONDebug-1.0.0-13-12-2021-13%3A29/AUTOMATIONDebug-1.0.0-13-12-2021-13%3A29.ipa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IOS_02</t>
-  </si>
-  <si>
-    <t xml:space="preserve">APPLE_iPhoneXS_iOS_14.1.0_21d51</t>
-  </si>
-  <si>
     <t xml:space="preserve">SAMSUNG_GalaxyTabS5e_Android_10.0.0_cb1ca</t>
   </si>
   <si>
@@ -1324,6 +1327,9 @@
   </si>
   <si>
     <t xml:space="preserve">APPLE_iPhone7plus_iOS_13.3.1_ce483</t>
+  </si>
+  <si>
+    <t>https://artifactory.appzillon.com/artifactory/android-apk/ao/manual/qaRelease-1.0.7-21-12-2021-15:37.apk</t>
   </si>
 </sst>
 </file>
@@ -1641,7 +1647,7 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1649,7 +1655,7 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1752,56 +1758,56 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="32.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="12.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="4.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="7.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="1" width="11.9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="1" width="15.54"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="17.31"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="16.2"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="2" width="22.49"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="22.49"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="17.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="16.2"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="15.21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="13.78"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="13.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="24.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="1" width="20.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="1" width="14.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="2" width="19.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="2" width="21.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="1" width="14.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="24" style="1" width="19.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="1" width="24.36"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="1" width="14.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="1" width="18.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="1" width="19.95"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="30" style="1" width="21.04"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="32" style="1" width="22.49"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="33" style="1" width="20.94"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="34" min="34" style="1" width="20.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="35" min="35" style="1" width="21.04"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="37" min="36" style="1" width="19.4"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="38" min="38" style="1" width="18.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="39" min="39" style="1" width="19.95"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="40" min="40" style="2" width="20.84"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="41" min="41" style="3" width="32.74"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="42" min="42" style="1" width="22.04"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="43" min="43" style="1" width="8.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="44" min="44" style="1" width="20.94"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="45" min="45" style="1" width="15.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="46" min="46" style="1" width="19.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="47" min="47" style="1" width="16.74"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="48" min="48" style="3" width="14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="49" min="49" style="3" width="16.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="50" min="50" style="1" width="12.35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="52" min="51" style="1" width="17.64"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="53" min="53" style="1" width="18.08"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="54" min="54" style="2" width="18.08"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="990" min="55" style="1" width="8.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="991" style="0" width="9.14"/>
+    <col min="1" max="1" customWidth="true" hidden="false" style="1" width="32.3" collapsed="true" outlineLevel="0"/>
+    <col min="2" max="2" customWidth="true" hidden="false" style="1" width="12.85" collapsed="true" outlineLevel="0"/>
+    <col min="3" max="3" customWidth="true" hidden="false" style="1" width="4.43" collapsed="true" outlineLevel="0"/>
+    <col min="4" max="4" customWidth="true" hidden="false" style="1" width="7.83" collapsed="true" outlineLevel="0"/>
+    <col min="5" max="6" customWidth="true" hidden="false" style="1" width="11.9" collapsed="true" outlineLevel="0"/>
+    <col min="7" max="8" customWidth="true" hidden="false" style="1" width="15.54" collapsed="true" outlineLevel="0"/>
+    <col min="9" max="9" customWidth="true" hidden="false" style="1" width="17.31" collapsed="true" outlineLevel="0"/>
+    <col min="10" max="10" customWidth="true" hidden="false" style="1" width="16.2" collapsed="true" outlineLevel="0"/>
+    <col min="11" max="11" customWidth="true" hidden="false" style="2" width="22.49" collapsed="true" outlineLevel="0"/>
+    <col min="12" max="12" customWidth="true" hidden="false" style="1" width="22.49" collapsed="true" outlineLevel="0"/>
+    <col min="13" max="13" customWidth="true" hidden="false" style="1" width="17.86" collapsed="true" outlineLevel="0"/>
+    <col min="14" max="14" customWidth="true" hidden="false" style="1" width="16.2" collapsed="true" outlineLevel="0"/>
+    <col min="15" max="15" customWidth="true" hidden="false" style="1" width="15.21" collapsed="true" outlineLevel="0"/>
+    <col min="16" max="16" customWidth="true" hidden="false" style="1" width="13.78" collapsed="true" outlineLevel="0"/>
+    <col min="17" max="17" customWidth="true" hidden="false" style="1" width="13.56" collapsed="true" outlineLevel="0"/>
+    <col min="18" max="18" customWidth="true" hidden="false" style="1" width="24.43" collapsed="true" outlineLevel="0"/>
+    <col min="19" max="19" customWidth="true" hidden="false" style="1" width="20.28" collapsed="true" outlineLevel="0"/>
+    <col min="20" max="20" customWidth="true" hidden="false" style="1" width="14.11" collapsed="true" outlineLevel="0"/>
+    <col min="21" max="21" customWidth="true" hidden="false" style="2" width="19.51" collapsed="true" outlineLevel="0"/>
+    <col min="22" max="22" customWidth="true" hidden="false" style="2" width="21.17" collapsed="true" outlineLevel="0"/>
+    <col min="23" max="23" customWidth="true" hidden="false" style="1" width="14.99" collapsed="true" outlineLevel="0"/>
+    <col min="24" max="25" customWidth="true" hidden="false" style="1" width="19.51" collapsed="true" outlineLevel="0"/>
+    <col min="26" max="26" customWidth="true" hidden="false" style="1" width="24.36" collapsed="true" outlineLevel="0"/>
+    <col min="27" max="27" customWidth="true" hidden="false" style="1" width="14.11" collapsed="true" outlineLevel="0"/>
+    <col min="28" max="28" customWidth="true" hidden="false" style="1" width="18.85" collapsed="true" outlineLevel="0"/>
+    <col min="29" max="29" customWidth="true" hidden="false" style="1" width="19.95" collapsed="true" outlineLevel="0"/>
+    <col min="30" max="31" customWidth="true" hidden="false" style="1" width="21.04" collapsed="true" outlineLevel="0"/>
+    <col min="32" max="32" customWidth="true" hidden="false" style="1" width="22.49" collapsed="true" outlineLevel="0"/>
+    <col min="33" max="33" customWidth="true" hidden="false" style="1" width="20.94" collapsed="true" outlineLevel="0"/>
+    <col min="34" max="34" customWidth="true" hidden="false" style="1" width="20.28" collapsed="true" outlineLevel="0"/>
+    <col min="35" max="35" customWidth="true" hidden="false" style="1" width="21.04" collapsed="true" outlineLevel="0"/>
+    <col min="36" max="37" customWidth="true" hidden="false" style="1" width="19.4" collapsed="true" outlineLevel="0"/>
+    <col min="38" max="38" customWidth="true" hidden="false" style="1" width="18.3" collapsed="true" outlineLevel="0"/>
+    <col min="39" max="39" customWidth="true" hidden="false" style="1" width="19.95" collapsed="true" outlineLevel="0"/>
+    <col min="40" max="40" customWidth="true" hidden="false" style="2" width="20.84" collapsed="true" outlineLevel="0"/>
+    <col min="41" max="41" customWidth="true" hidden="false" style="3" width="32.74" collapsed="true" outlineLevel="0"/>
+    <col min="42" max="42" customWidth="true" hidden="false" style="1" width="22.04" collapsed="true" outlineLevel="0"/>
+    <col min="43" max="43" customWidth="true" hidden="false" style="1" width="8.57" collapsed="true" outlineLevel="0"/>
+    <col min="44" max="44" customWidth="true" hidden="false" style="1" width="20.94" collapsed="true" outlineLevel="0"/>
+    <col min="45" max="45" customWidth="true" hidden="false" style="1" width="15.11" collapsed="true" outlineLevel="0"/>
+    <col min="46" max="46" customWidth="true" hidden="false" style="1" width="19.18" collapsed="true" outlineLevel="0"/>
+    <col min="47" max="47" customWidth="true" hidden="false" style="1" width="16.74" collapsed="true" outlineLevel="0"/>
+    <col min="48" max="48" customWidth="true" hidden="false" style="3" width="14.0" collapsed="true" outlineLevel="0"/>
+    <col min="49" max="49" customWidth="true" hidden="false" style="3" width="16.11" collapsed="true" outlineLevel="0"/>
+    <col min="50" max="50" customWidth="true" hidden="false" style="1" width="12.35" collapsed="true" outlineLevel="0"/>
+    <col min="51" max="52" customWidth="true" hidden="false" style="1" width="17.64" collapsed="true" outlineLevel="0"/>
+    <col min="53" max="53" customWidth="true" hidden="false" style="1" width="18.08" collapsed="true" outlineLevel="0"/>
+    <col min="54" max="54" customWidth="true" hidden="false" style="2" width="18.08" collapsed="true" outlineLevel="0"/>
+    <col min="55" max="990" customWidth="true" hidden="false" style="1" width="8.57" collapsed="true" outlineLevel="0"/>
+    <col min="991" max="1025" customWidth="true" hidden="false" style="0" width="9.14" collapsed="true" outlineLevel="0"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -20603,31 +20609,31 @@
   <dimension ref="A1:U9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="I8" activeCellId="0" sqref="I8"/>
+      <selection pane="bottomLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+      <selection pane="bottomRight" activeCell="F7" activeCellId="0" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="17" width="12.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="17" width="5.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="17" width="9.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="17" width="19.4"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="17" width="20.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="17" width="15.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="17" width="9.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="17" width="18.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="17" width="9.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="17" width="17.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="12" style="17" width="14.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="17" width="19.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="17" width="26.35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="16" style="17" width="9.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="17" width="29.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="19" style="17" width="9.17"/>
+    <col min="1" max="1" customWidth="true" hidden="false" style="17" width="12.57" collapsed="true" outlineLevel="0"/>
+    <col min="2" max="2" customWidth="true" hidden="false" style="17" width="5.18" collapsed="true" outlineLevel="0"/>
+    <col min="3" max="4" customWidth="true" hidden="false" style="17" width="9.17" collapsed="true" outlineLevel="0"/>
+    <col min="5" max="5" customWidth="true" hidden="false" style="17" width="19.4" collapsed="true" outlineLevel="0"/>
+    <col min="6" max="6" customWidth="true" hidden="false" style="17" width="20.5" collapsed="true" outlineLevel="0"/>
+    <col min="7" max="7" customWidth="true" hidden="false" style="17" width="15.11" collapsed="true" outlineLevel="0"/>
+    <col min="8" max="8" customWidth="true" hidden="false" style="17" width="9.17" collapsed="true" outlineLevel="0"/>
+    <col min="9" max="9" customWidth="true" hidden="false" style="17" width="18.85" collapsed="true" outlineLevel="0"/>
+    <col min="10" max="10" customWidth="true" hidden="false" style="17" width="9.17" collapsed="true" outlineLevel="0"/>
+    <col min="11" max="11" customWidth="true" hidden="false" style="17" width="17.86" collapsed="true" outlineLevel="0"/>
+    <col min="12" max="13" customWidth="true" hidden="false" style="17" width="14.87" collapsed="true" outlineLevel="0"/>
+    <col min="14" max="14" customWidth="true" hidden="false" style="17" width="19.18" collapsed="true" outlineLevel="0"/>
+    <col min="15" max="15" customWidth="true" hidden="false" style="17" width="26.35" collapsed="true" outlineLevel="0"/>
+    <col min="16" max="17" customWidth="true" hidden="false" style="17" width="9.17" collapsed="true" outlineLevel="0"/>
+    <col min="18" max="18" customWidth="true" hidden="false" style="17" width="29.45" collapsed="true" outlineLevel="0"/>
+    <col min="19" max="1025" customWidth="true" hidden="false" style="17" width="9.17" collapsed="true" outlineLevel="0"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -20702,21 +20708,28 @@
       <c r="D2" s="21" t="s">
         <v>382</v>
       </c>
+      <c r="E2"/>
+      <c r="F2"/>
       <c r="G2" s="21" t="s">
         <v>383</v>
       </c>
+      <c r="H2"/>
       <c r="I2" s="21" t="s">
         <v>384</v>
       </c>
       <c r="J2" s="22" t="s">
         <v>385</v>
       </c>
+      <c r="K2"/>
+      <c r="L2"/>
+      <c r="M2"/>
       <c r="N2" s="23" t="s">
         <v>386</v>
       </c>
       <c r="O2" s="11" t="s">
         <v>387</v>
       </c>
+      <c r="P2"/>
       <c r="Q2" s="22" t="n">
         <v>500</v>
       </c>
@@ -20740,28 +20753,35 @@
       <c r="D3" s="20" t="s">
         <v>382</v>
       </c>
+      <c r="E3"/>
+      <c r="F3"/>
       <c r="G3" s="20" t="s">
         <v>383</v>
       </c>
+      <c r="H3"/>
       <c r="I3" s="25" t="s">
         <v>390</v>
       </c>
       <c r="J3" s="25" t="s">
         <v>385</v>
       </c>
+      <c r="K3"/>
+      <c r="L3"/>
+      <c r="M3"/>
       <c r="N3" s="23" t="s">
         <v>386</v>
       </c>
       <c r="O3" s="11" t="s">
         <v>387</v>
       </c>
+      <c r="P3"/>
       <c r="Q3" s="20" t="n">
         <v>103</v>
       </c>
       <c r="R3" s="25" t="s">
         <v>388</v>
       </c>
-      <c r="S3" s="26" t="n">
+      <c r="S3" s="26" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -20813,13 +20833,14 @@
       <c r="O4" s="11" t="s">
         <v>387</v>
       </c>
+      <c r="P4"/>
       <c r="Q4" s="20" t="n">
         <v>306</v>
       </c>
       <c r="R4" s="8" t="s">
         <v>403</v>
       </c>
-      <c r="S4" s="30" t="n">
+      <c r="S4" s="30" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -20870,13 +20891,14 @@
       <c r="O5" s="11" t="s">
         <v>387</v>
       </c>
+      <c r="P5"/>
       <c r="Q5" s="20" t="n">
         <v>307</v>
       </c>
       <c r="R5" s="8" t="s">
         <v>403</v>
       </c>
-      <c r="S5" s="30" t="n">
+      <c r="S5" s="30" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -20927,13 +20949,14 @@
       <c r="O6" s="11" t="s">
         <v>387</v>
       </c>
+      <c r="P6"/>
       <c r="Q6" s="20" t="n">
         <v>106</v>
       </c>
       <c r="R6" s="8" t="s">
         <v>403</v>
       </c>
-      <c r="S6" s="30" t="n">
+      <c r="S6" s="30" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -20961,10 +20984,10 @@
         <v>383</v>
       </c>
       <c r="H7" s="8" t="s">
-        <v>396</v>
+        <v>411</v>
       </c>
       <c r="I7" s="31" t="s">
-        <v>411</v>
+        <v>397</v>
       </c>
       <c r="J7" s="8" t="s">
         <v>398</v>
@@ -20972,6 +20995,9 @@
       <c r="K7" s="8" t="s">
         <v>399</v>
       </c>
+      <c r="L7" t="s">
+        <v>435</v>
+      </c>
       <c r="M7" s="29" t="s">
         <v>401</v>
       </c>
@@ -20981,13 +21007,14 @@
       <c r="O7" s="11" t="s">
         <v>387</v>
       </c>
+      <c r="P7"/>
       <c r="Q7" s="20" t="n">
         <v>306</v>
       </c>
       <c r="R7" s="8" t="s">
         <v>403</v>
       </c>
-      <c r="S7" s="30" t="n">
+      <c r="S7" s="30" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -21017,22 +21044,27 @@
       <c r="H8" s="32" t="s">
         <v>414</v>
       </c>
-      <c r="I8" s="33" t="s">
+      <c r="I8" s="31" t="s">
         <v>415</v>
       </c>
-      <c r="J8" s="31" t="s">
+      <c r="J8" s="33" t="s">
         <v>416</v>
       </c>
-      <c r="K8" s="31" t="s">
+      <c r="K8" s="33" t="s">
         <v>417</v>
       </c>
+      <c r="L8"/>
+      <c r="M8"/>
+      <c r="N8"/>
+      <c r="O8"/>
+      <c r="P8"/>
       <c r="Q8" s="1" t="n">
         <v>500</v>
       </c>
       <c r="R8" s="8" t="s">
         <v>403</v>
       </c>
-      <c r="S8" s="30" t="n">
+      <c r="S8" s="30" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -21065,19 +21097,24 @@
       <c r="I9" s="8" t="s">
         <v>419</v>
       </c>
-      <c r="J9" s="31" t="s">
+      <c r="J9" s="33" t="s">
         <v>416</v>
       </c>
       <c r="K9" s="34" t="s">
         <v>417</v>
       </c>
+      <c r="L9"/>
+      <c r="M9"/>
+      <c r="N9"/>
+      <c r="O9"/>
+      <c r="P9"/>
       <c r="Q9" s="1" t="n">
         <v>501</v>
       </c>
       <c r="R9" s="8" t="s">
         <v>403</v>
       </c>
-      <c r="S9" s="30" t="n">
+      <c r="S9" s="30" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -21124,7 +21161,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="9.14"/>
+    <col min="1" max="1025" customWidth="true" hidden="false" style="0" width="9.14" collapsed="true" outlineLevel="0"/>
   </cols>
   <sheetData>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -21134,27 +21171,27 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="35" t="s">
-        <v>411</v>
+        <v>420</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="35" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="35" t="s">
-        <v>411</v>
+        <v>420</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="35" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="35" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -21164,27 +21201,27 @@
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="35" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="35" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="0" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="0" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="0" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -21193,15 +21230,15 @@
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="0" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="0" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -21209,17 +21246,17 @@
         <v>415</v>
       </c>
       <c r="F25" s="36" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="0" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="0" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -21229,7 +21266,7 @@
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="0" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
android device finding utility class updation
</commit_message>
<xml_diff>
--- a/src/test/resources/DataSet/NMCO_ONB.xlsx
+++ b/src/test/resources/DataSet/NMCO_ONB.xlsx
@@ -20651,11 +20651,11 @@
   <dimension ref="A1:U9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="F1" activeCellId="0" sqref="F1"/>
-      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I5" activeCellId="0" sqref="I5"/>
+      <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="H4" activeCellId="0" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
made changes in pcloudy class
</commit_message>
<xml_diff>
--- a/src/test/resources/DataSet/NMCO_ONB.xlsx
+++ b/src/test/resources/DataSet/NMCO_ONB.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2739" uniqueCount="436">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2745" uniqueCount="437">
   <si>
     <t xml:space="preserve">TestCaseName</t>
   </si>
@@ -1349,6 +1349,9 @@
   </si>
   <si>
     <t>null</t>
+  </si>
+  <si>
+    <t>https://readuser:Re@d@1234@artifactory.appzillon.com/artifactory/android-apk/ao/manual/qaRelease-1.0.7-21-12-2021-15:37.apk</t>
   </si>
 </sst>
 </file>
@@ -20831,7 +20834,7 @@
         <v>399</v>
       </c>
       <c r="L4" s="17" t="s">
-        <v>400</v>
+        <v>436</v>
       </c>
       <c r="M4" s="11" t="s">
         <v>401</v>

</xml_diff>

<commit_message>
updating pcloudy dependency jar to local maven
</commit_message>
<xml_diff>
--- a/src/test/resources/DataSet/NMCO_ONB.xlsx
+++ b/src/test/resources/DataSet/NMCO_ONB.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2745" uniqueCount="437">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2748" uniqueCount="438">
   <si>
     <t xml:space="preserve">TestCaseName</t>
   </si>
@@ -1352,6 +1352,9 @@
   </si>
   <si>
     <t>https://readuser:Re@d@1234@artifactory.appzillon.com/artifactory/android-apk/ao/manual/qaRelease-1.0.7-21-12-2021-15:37.apk</t>
+  </si>
+  <si>
+    <t>https://artifactory.appzillon.com/artifactory/android-apk/ao/manual/qaRelease-1.0.7-21-12-2021-15:37.apk</t>
   </si>
 </sst>
 </file>
@@ -20834,7 +20837,7 @@
         <v>399</v>
       </c>
       <c r="L4" s="17" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="M4" s="11" t="s">
         <v>401</v>

</xml_diff>

<commit_message>
updating ios connection utility
</commit_message>
<xml_diff>
--- a/src/test/resources/DataSet/NMCO_ONB.xlsx
+++ b/src/test/resources/DataSet/NMCO_ONB.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="TestData" sheetId="1" state="visible" r:id="rId2"/>
@@ -25996,12 +25996,12 @@
   </sheetPr>
   <dimension ref="A1:U13"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B6" activePane="bottomRight" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="F6" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="topRight" activeCell="F1" activeCellId="0" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="I8" activeCellId="0" sqref="I8"/>
+      <selection pane="bottomRight" activeCell="J7" activeCellId="0" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -26533,7 +26533,7 @@
   </sheetPr>
   <dimension ref="B4:G46"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D37" activeCellId="0" sqref="D37"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
commended home feature file for CD job trigger
</commit_message>
<xml_diff>
--- a/src/test/resources/DataSet/NMCO_ONB.xlsx
+++ b/src/test/resources/DataSet/NMCO_ONB.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="TestData" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2144" uniqueCount="482">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2144" uniqueCount="481">
   <si>
     <t xml:space="preserve">TestCaseName</t>
   </si>
@@ -1359,26 +1359,7 @@
     <t xml:space="preserve">https://readuser:Re@d@1234@artifactory.appzillon.com/artifactory/android-apk/ao/manual/qaRelease-1.0.7-21-12-2021-15:37.apk</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF067D17"/>
-        <rFont val="JetBrains Mono"/>
-        <family val="3"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Automation-1-0-13-18-01-2022</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF067D17"/>
-        <rFont val="JetBrains Mono"/>
-        <family val="3"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">.apk</t>
-    </r>
+    <t xml:space="preserve">Automation-1-0-15-21-01-2022.apk</t>
   </si>
   <si>
     <t xml:space="preserve">com.iexceed.assistedonboardingapp.assistedonboarding.AssistedOnboardingActivity</t>
@@ -1403,28 +1384,6 @@
   </si>
   <si>
     <t xml:space="preserve">Android_0003</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF067D17"/>
-        <rFont val="JetBrains Mono"/>
-        <family val="3"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Automation-1-0-12-18-01-2022</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF067D17"/>
-        <rFont val="JetBrains Mono"/>
-        <family val="3"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">.apk</t>
-    </r>
   </si>
   <si>
     <t xml:space="preserve">IOS_001</t>
@@ -1693,7 +1652,7 @@
     <numFmt numFmtId="168" formatCode="&quot;+91&quot;"/>
     <numFmt numFmtId="169" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
-  <fonts count="17">
+  <fonts count="16">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1778,13 +1737,6 @@
     <font>
       <sz val="13.5"/>
       <color rgb="FF6A8759"/>
-      <name val="JetBrains Mono"/>
-      <family val="3"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF067D17"/>
       <name val="JetBrains Mono"/>
       <family val="3"/>
       <charset val="1"/>
@@ -2029,7 +1981,7 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2045,11 +1997,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2132,7 +2084,7 @@
   </sheetPr>
   <dimension ref="A1:AMJ1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A157" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A157" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="0" topLeftCell="B157" activePane="topRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A157" activeCellId="0" sqref="A157"/>
       <selection pane="topRight" activeCell="A162" activeCellId="0" sqref="A162"/>
@@ -16446,12 +16398,12 @@
   </sheetPr>
   <dimension ref="A1:U13"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="M6" activePane="bottomRight" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="F5" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="M1" activeCellId="0" sqref="M1"/>
-      <selection pane="bottomLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="R8" activeCellId="0" sqref="R8"/>
+      <selection pane="topRight" activeCell="F1" activeCellId="0" sqref="F1"/>
+      <selection pane="bottomLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+      <selection pane="bottomRight" activeCell="L7" activeCellId="0" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -16611,7 +16563,7 @@
       </c>
       <c r="U3" s="28"/>
     </row>
-    <row r="4" customFormat="false" ht="109.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="108.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="8" t="s">
         <v>417</v>
       </c>
@@ -16668,7 +16620,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="136.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="8" t="s">
         <v>430</v>
       </c>
@@ -16725,7 +16677,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="46.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="8" t="s">
         <v>433</v>
       </c>
@@ -16811,7 +16763,7 @@
         <v>424</v>
       </c>
       <c r="M7" s="11" t="s">
-        <v>436</v>
+        <v>427</v>
       </c>
       <c r="N7" s="24" t="s">
         <v>412</v>
@@ -16832,7 +16784,7 @@
     </row>
     <row r="8" customFormat="false" ht="106.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="8" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="B8" s="8" t="s">
         <v>30</v>
@@ -16841,7 +16793,7 @@
         <v>418</v>
       </c>
       <c r="D8" s="32" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="E8" s="29" t="s">
         <v>420</v>
@@ -16850,26 +16802,26 @@
         <v>421</v>
       </c>
       <c r="G8" s="8" t="s">
+        <v>438</v>
+      </c>
+      <c r="H8" s="33" t="s">
         <v>439</v>
       </c>
-      <c r="H8" s="33" t="s">
+      <c r="I8" s="34" t="s">
         <v>440</v>
       </c>
-      <c r="I8" s="34" t="s">
+      <c r="J8" s="30" t="s">
         <v>441</v>
       </c>
-      <c r="J8" s="30" t="s">
+      <c r="K8" s="30" t="s">
         <v>442</v>
-      </c>
-      <c r="K8" s="30" t="s">
-        <v>443</v>
       </c>
       <c r="M8" s="11"/>
       <c r="Q8" s="23" t="n">
         <v>506</v>
       </c>
       <c r="R8" s="8" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="S8" s="31" t="n">
         <f aca="false">FALSE()</f>
@@ -16878,7 +16830,7 @@
     </row>
     <row r="9" customFormat="false" ht="82.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="18" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="B9" s="18" t="s">
         <v>30</v>
@@ -16887,7 +16839,7 @@
         <v>418</v>
       </c>
       <c r="D9" s="18" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="E9" s="29" t="s">
         <v>420</v>
@@ -16896,26 +16848,26 @@
         <v>421</v>
       </c>
       <c r="G9" s="32" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="H9" s="33" t="s">
+        <v>445</v>
+      </c>
+      <c r="I9" s="8" t="s">
         <v>446</v>
       </c>
-      <c r="I9" s="8" t="s">
-        <v>447</v>
-      </c>
       <c r="J9" s="30" t="s">
+        <v>441</v>
+      </c>
+      <c r="K9" s="35" t="s">
         <v>442</v>
-      </c>
-      <c r="K9" s="35" t="s">
-        <v>443</v>
       </c>
       <c r="M9" s="11"/>
       <c r="Q9" s="23" t="n">
         <v>507</v>
       </c>
       <c r="R9" s="8" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="S9" s="31" t="n">
         <f aca="false">FALSE()</f>
@@ -16924,13 +16876,13 @@
     </row>
     <row r="10" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H10" s="33" t="s">
+        <v>447</v>
+      </c>
+      <c r="I10" s="8" t="s">
         <v>448</v>
       </c>
-      <c r="I10" s="8" t="s">
-        <v>449</v>
-      </c>
       <c r="J10" s="30" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="M10" s="11"/>
       <c r="Q10" s="23"/>
@@ -16996,7 +16948,7 @@
   <sheetData>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="0" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17006,7 +16958,7 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="36" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17016,12 +16968,12 @@
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="36" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="36" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17031,27 +16983,27 @@
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="36" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="36" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="0" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="0" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="0" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -17060,139 +17012,139 @@
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="0" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="0" t="s">
+        <v>458</v>
+      </c>
+      <c r="F24" s="0" t="s">
         <v>459</v>
-      </c>
-      <c r="F24" s="0" t="s">
-        <v>460</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="37" t="s">
+        <v>460</v>
+      </c>
+      <c r="F25" s="37" t="s">
         <v>461</v>
-      </c>
-      <c r="F25" s="37" t="s">
-        <v>462</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="0" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="0" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="0" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="0" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="9" t="s">
+        <v>466</v>
+      </c>
+      <c r="E31" s="0" t="s">
         <v>467</v>
-      </c>
-      <c r="E31" s="0" t="s">
-        <v>468</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B32" s="37" t="s">
+        <v>468</v>
+      </c>
+      <c r="E32" s="0" t="s">
         <v>469</v>
-      </c>
-      <c r="E32" s="0" t="s">
-        <v>470</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B33" s="0" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="E33" s="0" t="s">
+        <v>469</v>
+      </c>
+      <c r="F33" s="0" t="s">
         <v>470</v>
-      </c>
-      <c r="F33" s="0" t="s">
-        <v>471</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B34" s="0" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="E34" s="0" t="s">
+        <v>469</v>
+      </c>
+      <c r="F34" s="0" t="s">
         <v>470</v>
-      </c>
-      <c r="F34" s="0" t="s">
-        <v>471</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="0" t="s">
+        <v>472</v>
+      </c>
+      <c r="E35" s="0" t="s">
+        <v>469</v>
+      </c>
+      <c r="F35" s="0" t="s">
+        <v>470</v>
+      </c>
+      <c r="G35" s="0" t="s">
         <v>473</v>
-      </c>
-      <c r="E35" s="0" t="s">
-        <v>470</v>
-      </c>
-      <c r="F35" s="0" t="s">
-        <v>471</v>
-      </c>
-      <c r="G35" s="0" t="s">
-        <v>474</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="0" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="E36" s="0" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B37" s="0" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="E37" s="0" t="s">
+        <v>469</v>
+      </c>
+      <c r="F37" s="0" t="s">
         <v>470</v>
       </c>
-      <c r="F37" s="0" t="s">
-        <v>471</v>
-      </c>
       <c r="G37" s="0" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B44" s="37" t="s">
+        <v>476</v>
+      </c>
+      <c r="E44" s="0" t="s">
         <v>477</v>
-      </c>
-      <c r="E44" s="0" t="s">
-        <v>478</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B45" s="38" t="s">
+        <v>478</v>
+      </c>
+      <c r="F45" s="0" t="s">
         <v>479</v>
-      </c>
-      <c r="F45" s="0" t="s">
-        <v>480</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B46" s="39" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
made chages in business location features
</commit_message>
<xml_diff>
--- a/src/test/resources/DataSet/NMCO_ONB.xlsx
+++ b/src/test/resources/DataSet/NMCO_ONB.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="TestData" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2387" uniqueCount="520">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2458" uniqueCount="528">
   <si>
     <t xml:space="preserve">TestCaseName</t>
   </si>
@@ -1303,6 +1303,30 @@
   </si>
   <si>
     <t xml:space="preserve">TestCase_172</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TestCase_173</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#$#%$%^%^%^&amp;^        %^&amp;^&amp;*&amp;^*&amp;*(*(*)*()(</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Business Logic screen-countrycode and type of operation,with invalid input</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TestCase_174</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TestCase_175</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TestCase_176</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TestCase_177</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TestCase_178</t>
   </si>
   <si>
     <t xml:space="preserve">mode</t>
@@ -2171,12 +2195,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMJ1048576"/>
+  <dimension ref="A1:AMJ182"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A105" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="0" topLeftCell="I105" activePane="topRight" state="frozen"/>
-      <selection pane="topLeft" activeCell="A105" activeCellId="0" sqref="A105"/>
-      <selection pane="topRight" activeCell="I107" activeCellId="0" sqref="I107"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A180" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="0" topLeftCell="Z180" activePane="topRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A180" activeCellId="0" sqref="A180"/>
+      <selection pane="topRight" activeCell="AB182" activeCellId="0" sqref="AB182"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -17253,7 +17277,344 @@
         <v>424</v>
       </c>
     </row>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="177" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A177" s="8" t="s">
+        <v>385</v>
+      </c>
+      <c r="B177" s="8" t="s">
+        <v>427</v>
+      </c>
+      <c r="C177" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="E177" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="F177" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G177" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="H177" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="I177" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="J177" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="K177" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="M177" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="N177" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="W177" s="8"/>
+      <c r="X177" s="8"/>
+      <c r="Y177" s="8"/>
+      <c r="Z177" s="8"/>
+      <c r="AA177" s="8" t="s">
+        <v>428</v>
+      </c>
+      <c r="AB177" s="16" t="n">
+        <v>189</v>
+      </c>
+      <c r="AC177" s="8"/>
+      <c r="AD177" s="8"/>
+      <c r="AE177" s="8"/>
+      <c r="AF177" s="8"/>
+      <c r="AG177" s="8"/>
+      <c r="AH177" s="16"/>
+      <c r="AI177" s="8"/>
+      <c r="AJ177" s="8"/>
+    </row>
+    <row r="178" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A178" s="8" t="s">
+        <v>429</v>
+      </c>
+      <c r="B178" s="8" t="s">
+        <v>430</v>
+      </c>
+      <c r="C178" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="E178" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="F178" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G178" s="1" t="n">
+        <v>101</v>
+      </c>
+      <c r="H178" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="I178" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="J178" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="K178" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="M178" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="N178" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="W178" s="8"/>
+      <c r="X178" s="8"/>
+      <c r="Y178" s="8"/>
+      <c r="Z178" s="8"/>
+      <c r="AA178" s="8" t="s">
+        <v>398</v>
+      </c>
+      <c r="AB178" s="16" t="n">
+        <v>129</v>
+      </c>
+      <c r="AC178" s="8"/>
+      <c r="AD178" s="8"/>
+      <c r="AE178" s="8"/>
+      <c r="AF178" s="8"/>
+      <c r="AG178" s="8"/>
+      <c r="AH178" s="16"/>
+      <c r="AI178" s="8"/>
+      <c r="AJ178" s="8"/>
+    </row>
+    <row r="179" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A179" s="8" t="s">
+        <v>429</v>
+      </c>
+      <c r="B179" s="8" t="s">
+        <v>431</v>
+      </c>
+      <c r="C179" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="E179" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="F179" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G179" s="1" t="n">
+        <v>101</v>
+      </c>
+      <c r="H179" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="I179" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="J179" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="K179" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="M179" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="N179" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="W179" s="8"/>
+      <c r="X179" s="8"/>
+      <c r="Y179" s="8"/>
+      <c r="Z179" s="8"/>
+      <c r="AA179" s="8"/>
+      <c r="AB179" s="16" t="n">
+        <v>900</v>
+      </c>
+      <c r="AC179" s="8"/>
+      <c r="AD179" s="8"/>
+      <c r="AE179" s="8"/>
+      <c r="AF179" s="8"/>
+      <c r="AG179" s="8"/>
+      <c r="AH179" s="16"/>
+      <c r="AI179" s="8"/>
+      <c r="AJ179" s="8"/>
+    </row>
+    <row r="180" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A180" s="8" t="s">
+        <v>390</v>
+      </c>
+      <c r="B180" s="8" t="s">
+        <v>432</v>
+      </c>
+      <c r="C180" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="E180" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="F180" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G180" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="H180" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="I180" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="J180" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="K180" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="M180" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="N180" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="R180" s="8"/>
+      <c r="T180" s="8"/>
+      <c r="W180" s="8"/>
+      <c r="X180" s="8"/>
+      <c r="Y180" s="8"/>
+      <c r="Z180" s="8"/>
+      <c r="AA180" s="8" t="s">
+        <v>428</v>
+      </c>
+      <c r="AB180" s="16" t="n">
+        <v>555</v>
+      </c>
+      <c r="AC180" s="8"/>
+      <c r="AD180" s="8"/>
+      <c r="AE180" s="8"/>
+      <c r="AF180" s="8"/>
+      <c r="AG180" s="8"/>
+      <c r="AH180" s="16"/>
+      <c r="AI180" s="8"/>
+      <c r="AJ180" s="8"/>
+    </row>
+    <row r="181" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A181" s="8" t="s">
+        <v>392</v>
+      </c>
+      <c r="B181" s="8" t="s">
+        <v>433</v>
+      </c>
+      <c r="C181" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="E181" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="F181" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G181" s="1" t="n">
+        <v>101</v>
+      </c>
+      <c r="H181" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="I181" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="J181" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="K181" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="M181" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="N181" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="R181" s="8"/>
+      <c r="T181" s="8"/>
+      <c r="W181" s="8"/>
+      <c r="X181" s="8"/>
+      <c r="Y181" s="8"/>
+      <c r="Z181" s="8"/>
+      <c r="AA181" s="8" t="s">
+        <v>398</v>
+      </c>
+      <c r="AB181" s="16" t="n">
+        <v>345</v>
+      </c>
+      <c r="AC181" s="8"/>
+      <c r="AD181" s="8"/>
+      <c r="AE181" s="8"/>
+      <c r="AF181" s="8"/>
+      <c r="AG181" s="8"/>
+      <c r="AH181" s="16"/>
+      <c r="AI181" s="8"/>
+      <c r="AJ181" s="8"/>
+    </row>
+    <row r="182" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A182" s="8" t="s">
+        <v>392</v>
+      </c>
+      <c r="B182" s="8" t="s">
+        <v>434</v>
+      </c>
+      <c r="C182" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="E182" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="F182" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G182" s="1" t="n">
+        <v>101</v>
+      </c>
+      <c r="H182" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="I182" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="J182" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="K182" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="M182" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="N182" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="R182" s="8"/>
+      <c r="T182" s="8"/>
+      <c r="W182" s="8"/>
+      <c r="X182" s="8"/>
+      <c r="Y182" s="8"/>
+      <c r="Z182" s="8"/>
+      <c r="AA182" s="8"/>
+      <c r="AB182" s="16" t="n">
+        <v>340</v>
+      </c>
+      <c r="AC182" s="8"/>
+      <c r="AD182" s="8"/>
+      <c r="AE182" s="8"/>
+      <c r="AF182" s="8"/>
+      <c r="AG182" s="8"/>
+      <c r="AH182" s="16"/>
+      <c r="AI182" s="8"/>
+      <c r="AJ182" s="8"/>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="I10" r:id="rId1" display="kimtaehyung@gmail.com"/>
@@ -17316,6 +17677,12 @@
     <hyperlink ref="I174" r:id="rId58" display="parkjimin@gmail.com"/>
     <hyperlink ref="I175" r:id="rId59" display="parkjimin@gmail.com"/>
     <hyperlink ref="I176" r:id="rId60" display="parkjimin@gmail.com"/>
+    <hyperlink ref="I177" r:id="rId61" display="parkjimin@gmail.com"/>
+    <hyperlink ref="I178" r:id="rId62" display="parkjimin@gmail.com"/>
+    <hyperlink ref="I179" r:id="rId63" display="parkjimin@gmail.com"/>
+    <hyperlink ref="I180" r:id="rId64" display="parkjimin@gmail.com"/>
+    <hyperlink ref="I181" r:id="rId65" display="parkjimin@gmail.com"/>
+    <hyperlink ref="I182" r:id="rId66" display="parkjimin@gmail.com"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -17334,12 +17701,12 @@
   </sheetPr>
   <dimension ref="A1:U10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="J4" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="J1" activeCellId="0" sqref="J1"/>
       <selection pane="bottomLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="N5" activeCellId="0" sqref="N5"/>
+      <selection pane="bottomRight" activeCell="J6" activeCellId="0" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -17370,97 +17737,97 @@
         <v>2</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>427</v>
+        <v>435</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>428</v>
+        <v>436</v>
       </c>
       <c r="E1" s="18" t="s">
-        <v>429</v>
+        <v>437</v>
       </c>
       <c r="F1" s="18" t="s">
-        <v>430</v>
+        <v>438</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>431</v>
+        <v>439</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>432</v>
+        <v>440</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>433</v>
+        <v>441</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>434</v>
+        <v>442</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>435</v>
+        <v>443</v>
       </c>
       <c r="L1" s="4" t="s">
-        <v>436</v>
+        <v>444</v>
       </c>
       <c r="M1" s="4" t="s">
-        <v>437</v>
+        <v>445</v>
       </c>
       <c r="N1" s="4" t="s">
-        <v>438</v>
+        <v>446</v>
       </c>
       <c r="O1" s="4" t="s">
-        <v>439</v>
+        <v>447</v>
       </c>
       <c r="P1" s="4" t="s">
-        <v>440</v>
+        <v>448</v>
       </c>
       <c r="Q1" s="4" t="s">
-        <v>441</v>
+        <v>449</v>
       </c>
       <c r="R1" s="19" t="s">
-        <v>442</v>
+        <v>450</v>
       </c>
       <c r="S1" s="4" t="s">
-        <v>443</v>
+        <v>451</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="20" t="s">
-        <v>444</v>
+        <v>452</v>
       </c>
       <c r="B2" s="21" t="s">
         <v>35</v>
       </c>
       <c r="C2" s="21" t="s">
-        <v>445</v>
+        <v>453</v>
       </c>
       <c r="D2" s="21" t="s">
-        <v>446</v>
+        <v>454</v>
       </c>
       <c r="E2"/>
       <c r="F2"/>
       <c r="G2" s="21" t="s">
-        <v>447</v>
+        <v>455</v>
       </c>
       <c r="H2"/>
       <c r="I2" s="21" t="s">
-        <v>448</v>
+        <v>456</v>
       </c>
       <c r="J2" s="22" t="s">
-        <v>449</v>
+        <v>457</v>
       </c>
       <c r="K2"/>
       <c r="L2"/>
       <c r="M2"/>
       <c r="N2" s="23" t="s">
-        <v>450</v>
+        <v>458</v>
       </c>
       <c r="O2" s="11" t="s">
-        <v>451</v>
+        <v>459</v>
       </c>
       <c r="P2"/>
       <c r="Q2" s="22" t="n">
         <v>500</v>
       </c>
       <c r="R2" s="24" t="s">
-        <v>452</v>
+        <v>460</v>
       </c>
       <c r="S2" s="22" t="n">
         <v>0</v>
@@ -17468,44 +17835,44 @@
     </row>
     <row r="3" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="20" t="s">
+        <v>461</v>
+      </c>
+      <c r="B3" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="C3" s="20" t="s">
         <v>453</v>
       </c>
-      <c r="B3" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="C3" s="20" t="s">
-        <v>445</v>
-      </c>
       <c r="D3" s="20" t="s">
-        <v>446</v>
+        <v>454</v>
       </c>
       <c r="E3"/>
       <c r="F3"/>
       <c r="G3" s="20" t="s">
-        <v>447</v>
+        <v>455</v>
       </c>
       <c r="H3"/>
       <c r="I3" s="25" t="s">
-        <v>454</v>
+        <v>462</v>
       </c>
       <c r="J3" s="25" t="s">
-        <v>449</v>
+        <v>457</v>
       </c>
       <c r="K3"/>
       <c r="L3"/>
       <c r="M3"/>
       <c r="N3" s="23" t="s">
-        <v>450</v>
+        <v>458</v>
       </c>
       <c r="O3" s="11" t="s">
-        <v>451</v>
+        <v>459</v>
       </c>
       <c r="P3"/>
       <c r="Q3" s="22" t="n">
         <v>501</v>
       </c>
       <c r="R3" s="25" t="s">
-        <v>452</v>
+        <v>460</v>
       </c>
       <c r="S3" s="26" t="b">
         <f aca="false">FALSE()</f>
@@ -17515,56 +17882,56 @@
     </row>
     <row r="4" customFormat="false" ht="109.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="8" t="s">
+        <v>463</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>464</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>465</v>
+      </c>
+      <c r="E4" s="28" t="s">
+        <v>466</v>
+      </c>
+      <c r="F4" s="28" t="s">
+        <v>467</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>455</v>
       </c>
-      <c r="B4" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>456</v>
-      </c>
-      <c r="D4" s="8" t="s">
-        <v>457</v>
-      </c>
-      <c r="E4" s="28" t="s">
-        <v>458</v>
-      </c>
-      <c r="F4" s="28" t="s">
+      <c r="H4" s="8" t="s">
+        <v>468</v>
+      </c>
+      <c r="I4" s="29" t="s">
+        <v>469</v>
+      </c>
+      <c r="J4" s="8" t="s">
+        <v>470</v>
+      </c>
+      <c r="K4" s="8" t="s">
+        <v>471</v>
+      </c>
+      <c r="L4" s="30" t="s">
+        <v>527</v>
+      </c>
+      <c r="M4" s="31" t="s">
+        <v>473</v>
+      </c>
+      <c r="N4" s="23" t="s">
+        <v>474</v>
+      </c>
+      <c r="O4" s="11" t="s">
         <v>459</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>447</v>
-      </c>
-      <c r="H4" s="8" t="s">
-        <v>460</v>
-      </c>
-      <c r="I4" s="29" t="s">
-        <v>461</v>
-      </c>
-      <c r="J4" s="8" t="s">
-        <v>462</v>
-      </c>
-      <c r="K4" s="8" t="s">
-        <v>463</v>
-      </c>
-      <c r="L4" s="30" t="s">
-        <v>519</v>
-      </c>
-      <c r="M4" s="31" t="s">
-        <v>465</v>
-      </c>
-      <c r="N4" s="23" t="s">
-        <v>466</v>
-      </c>
-      <c r="O4" s="11" t="s">
-        <v>451</v>
       </c>
       <c r="P4"/>
       <c r="Q4" s="22" t="n">
         <v>502</v>
       </c>
       <c r="R4" s="8" t="s">
-        <v>467</v>
+        <v>475</v>
       </c>
       <c r="S4" s="32" t="b">
         <f aca="false">FALSE()</f>
@@ -17573,56 +17940,56 @@
     </row>
     <row r="5" customFormat="false" ht="109.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="8" t="s">
-        <v>468</v>
+        <v>476</v>
       </c>
       <c r="B5" s="8" t="s">
         <v>35</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>456</v>
+        <v>464</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>457</v>
+        <v>465</v>
       </c>
       <c r="E5" s="28" t="s">
-        <v>458</v>
+        <v>466</v>
       </c>
       <c r="F5" s="28" t="s">
+        <v>467</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>455</v>
+      </c>
+      <c r="H5" s="8" t="s">
+        <v>477</v>
+      </c>
+      <c r="I5" s="8" t="s">
+        <v>478</v>
+      </c>
+      <c r="J5" s="8" t="s">
+        <v>470</v>
+      </c>
+      <c r="K5" s="8" t="s">
+        <v>471</v>
+      </c>
+      <c r="L5" s="17" t="s">
+        <v>472</v>
+      </c>
+      <c r="M5" s="31" t="s">
+        <v>473</v>
+      </c>
+      <c r="N5" s="23" t="s">
+        <v>474</v>
+      </c>
+      <c r="O5" s="11" t="s">
         <v>459</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>447</v>
-      </c>
-      <c r="H5" s="8" t="s">
-        <v>469</v>
-      </c>
-      <c r="I5" s="8" t="s">
-        <v>470</v>
-      </c>
-      <c r="J5" s="8" t="s">
-        <v>462</v>
-      </c>
-      <c r="K5" s="8" t="s">
-        <v>463</v>
-      </c>
-      <c r="L5" s="17" t="s">
-        <v>464</v>
-      </c>
-      <c r="M5" s="31" t="s">
-        <v>465</v>
-      </c>
-      <c r="N5" s="23" t="s">
-        <v>466</v>
-      </c>
-      <c r="O5" s="11" t="s">
-        <v>451</v>
       </c>
       <c r="P5"/>
       <c r="Q5" s="22" t="n">
         <v>503</v>
       </c>
       <c r="R5" s="8" t="s">
-        <v>467</v>
+        <v>475</v>
       </c>
       <c r="S5" s="32" t="b">
         <f aca="false">FALSE()</f>
@@ -17631,54 +17998,54 @@
     </row>
     <row r="6" customFormat="false" ht="46.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="8" t="s">
-        <v>471</v>
+        <v>479</v>
       </c>
       <c r="B6" s="8" t="s">
         <v>35</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>456</v>
+        <v>464</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>457</v>
+        <v>465</v>
       </c>
       <c r="E6" s="28" t="s">
-        <v>458</v>
+        <v>466</v>
       </c>
       <c r="F6" s="28" t="s">
-        <v>459</v>
+        <v>467</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>447</v>
+        <v>455</v>
       </c>
       <c r="H6" s="8" t="s">
-        <v>460</v>
+        <v>468</v>
       </c>
       <c r="I6" s="29" t="s">
-        <v>461</v>
+        <v>469</v>
       </c>
       <c r="J6" s="8" t="s">
-        <v>462</v>
+        <v>470</v>
       </c>
       <c r="K6"/>
       <c r="L6" s="11" t="s">
-        <v>472</v>
+        <v>480</v>
       </c>
       <c r="M6" s="31" t="s">
-        <v>465</v>
+        <v>473</v>
       </c>
       <c r="N6" s="23" t="s">
-        <v>466</v>
+        <v>474</v>
       </c>
       <c r="O6" s="11" t="s">
-        <v>451</v>
+        <v>459</v>
       </c>
       <c r="P6"/>
       <c r="Q6" s="22" t="n">
         <v>504</v>
       </c>
       <c r="R6" s="8" t="s">
-        <v>467</v>
+        <v>475</v>
       </c>
       <c r="S6" s="32" t="b">
         <f aca="false">FALSE()</f>
@@ -17687,52 +18054,52 @@
     </row>
     <row r="7" customFormat="false" ht="82.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="8" t="s">
-        <v>473</v>
+        <v>481</v>
       </c>
       <c r="B7" s="8" t="s">
         <v>35</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>456</v>
+        <v>464</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>457</v>
+        <v>465</v>
       </c>
       <c r="E7" s="28" t="s">
-        <v>458</v>
+        <v>466</v>
       </c>
       <c r="F7" s="28" t="s">
-        <v>459</v>
+        <v>467</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>447</v>
+        <v>455</v>
       </c>
       <c r="H7" s="8" t="s">
-        <v>460</v>
+        <v>468</v>
       </c>
       <c r="I7" s="29" t="s">
-        <v>461</v>
+        <v>469</v>
       </c>
       <c r="J7" s="8" t="s">
-        <v>462</v>
+        <v>470</v>
       </c>
       <c r="K7"/>
       <c r="L7"/>
       <c r="M7" s="31" t="s">
-        <v>465</v>
+        <v>473</v>
       </c>
       <c r="N7" s="23" t="s">
-        <v>450</v>
+        <v>458</v>
       </c>
       <c r="O7" s="11" t="s">
-        <v>451</v>
+        <v>459</v>
       </c>
       <c r="P7"/>
       <c r="Q7" s="22" t="n">
         <v>505</v>
       </c>
       <c r="R7" s="8" t="s">
-        <v>467</v>
+        <v>475</v>
       </c>
       <c r="S7" s="32" t="b">
         <f aca="false">FALSE()</f>
@@ -17741,40 +18108,40 @@
     </row>
     <row r="8" customFormat="false" ht="106.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="8" t="s">
-        <v>474</v>
+        <v>482</v>
       </c>
       <c r="B8" s="8" t="s">
         <v>35</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>456</v>
+        <v>464</v>
       </c>
       <c r="D8" s="33" t="s">
-        <v>475</v>
+        <v>483</v>
       </c>
       <c r="E8" s="28" t="s">
-        <v>458</v>
+        <v>466</v>
       </c>
       <c r="F8" s="28" t="s">
-        <v>459</v>
+        <v>467</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>447</v>
+        <v>455</v>
       </c>
       <c r="H8" s="34" t="s">
-        <v>476</v>
+        <v>484</v>
       </c>
       <c r="I8" s="11" t="s">
-        <v>477</v>
+        <v>485</v>
       </c>
       <c r="J8" s="29" t="s">
-        <v>478</v>
+        <v>486</v>
       </c>
       <c r="K8" s="29" t="s">
-        <v>479</v>
+        <v>487</v>
       </c>
       <c r="L8" s="17" t="s">
-        <v>480</v>
+        <v>488</v>
       </c>
       <c r="M8"/>
       <c r="N8"/>
@@ -17784,7 +18151,7 @@
         <v>506</v>
       </c>
       <c r="R8" s="8" t="s">
-        <v>481</v>
+        <v>489</v>
       </c>
       <c r="S8" s="32" t="b">
         <f aca="false">FALSE()</f>
@@ -17793,37 +18160,37 @@
     </row>
     <row r="9" customFormat="false" ht="82.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="17" t="s">
-        <v>482</v>
+        <v>490</v>
       </c>
       <c r="B9" s="17" t="s">
         <v>35</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>456</v>
+        <v>464</v>
       </c>
       <c r="D9" s="17" t="s">
-        <v>475</v>
+        <v>483</v>
       </c>
       <c r="E9" s="28" t="s">
-        <v>458</v>
+        <v>466</v>
       </c>
       <c r="F9" s="28" t="s">
-        <v>459</v>
+        <v>467</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>447</v>
+        <v>455</v>
       </c>
       <c r="H9" s="34" t="s">
-        <v>483</v>
+        <v>491</v>
       </c>
       <c r="I9" s="8" t="s">
-        <v>484</v>
+        <v>492</v>
       </c>
       <c r="J9" s="29" t="s">
-        <v>478</v>
+        <v>486</v>
       </c>
       <c r="K9" s="35" t="s">
-        <v>479</v>
+        <v>487</v>
       </c>
       <c r="L9"/>
       <c r="M9"/>
@@ -17834,7 +18201,7 @@
         <v>507</v>
       </c>
       <c r="R9" s="8" t="s">
-        <v>481</v>
+        <v>489</v>
       </c>
       <c r="S9" s="32" t="b">
         <f aca="false">FALSE()</f>
@@ -17850,13 +18217,13 @@
       <c r="F10"/>
       <c r="G10"/>
       <c r="H10" s="34" t="s">
-        <v>485</v>
+        <v>493</v>
       </c>
       <c r="I10" s="8" t="s">
+        <v>494</v>
+      </c>
+      <c r="J10" s="29" t="s">
         <v>486</v>
-      </c>
-      <c r="J10" s="29" t="s">
-        <v>478</v>
       </c>
       <c r="K10"/>
       <c r="L10"/>
@@ -17918,62 +18285,62 @@
   <sheetData>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="0" t="s">
-        <v>487</v>
+        <v>495</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="36" t="s">
-        <v>461</v>
+        <v>469</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="36" t="s">
-        <v>488</v>
+        <v>496</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="36" t="s">
-        <v>461</v>
+        <v>469</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="36" t="s">
-        <v>489</v>
+        <v>497</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="36" t="s">
-        <v>490</v>
+        <v>498</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="0" t="s">
-        <v>470</v>
+        <v>478</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="36" t="s">
-        <v>489</v>
+        <v>497</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="36" t="s">
-        <v>491</v>
+        <v>499</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="0" t="s">
-        <v>492</v>
+        <v>500</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="0" t="s">
-        <v>493</v>
+        <v>501</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="0" t="s">
-        <v>494</v>
+        <v>502</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -17982,139 +18349,139 @@
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="0" t="s">
-        <v>495</v>
+        <v>503</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="0" t="s">
-        <v>496</v>
+        <v>504</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>497</v>
+        <v>505</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="37" t="s">
-        <v>498</v>
+        <v>506</v>
       </c>
       <c r="F25" s="37" t="s">
-        <v>499</v>
+        <v>507</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="0" t="s">
-        <v>500</v>
+        <v>508</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="0" t="s">
-        <v>501</v>
+        <v>509</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="0" t="s">
-        <v>502</v>
+        <v>510</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="0" t="s">
-        <v>503</v>
+        <v>511</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="9" t="s">
-        <v>504</v>
+        <v>512</v>
       </c>
       <c r="E31" s="0" t="s">
-        <v>505</v>
+        <v>513</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B32" s="37" t="s">
-        <v>506</v>
+        <v>514</v>
       </c>
       <c r="E32" s="0" t="s">
-        <v>507</v>
+        <v>515</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B33" s="0" t="s">
-        <v>477</v>
+        <v>485</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>507</v>
+        <v>515</v>
       </c>
       <c r="F33" s="0" t="s">
-        <v>508</v>
+        <v>516</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B34" s="0" t="s">
-        <v>509</v>
+        <v>517</v>
       </c>
       <c r="E34" s="0" t="s">
-        <v>507</v>
+        <v>515</v>
       </c>
       <c r="F34" s="0" t="s">
-        <v>508</v>
+        <v>516</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="0" t="s">
-        <v>510</v>
+        <v>518</v>
       </c>
       <c r="E35" s="0" t="s">
-        <v>507</v>
+        <v>515</v>
       </c>
       <c r="F35" s="0" t="s">
-        <v>508</v>
+        <v>516</v>
       </c>
       <c r="G35" s="0" t="s">
-        <v>511</v>
+        <v>519</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="0" t="s">
-        <v>512</v>
+        <v>520</v>
       </c>
       <c r="E36" s="0" t="s">
-        <v>507</v>
+        <v>515</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B37" s="0" t="s">
-        <v>486</v>
+        <v>494</v>
       </c>
       <c r="E37" s="0" t="s">
-        <v>507</v>
+        <v>515</v>
       </c>
       <c r="F37" s="0" t="s">
-        <v>508</v>
+        <v>516</v>
       </c>
       <c r="G37" s="0" t="s">
-        <v>513</v>
+        <v>521</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B44" s="37" t="s">
-        <v>514</v>
+        <v>522</v>
       </c>
       <c r="E44" s="0" t="s">
-        <v>515</v>
+        <v>523</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B45" s="38" t="s">
-        <v>516</v>
+        <v>524</v>
       </c>
       <c r="F45" s="0" t="s">
-        <v>517</v>
+        <v>525</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B46" s="39" t="s">
-        <v>518</v>
+        <v>526</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
made changes in Industry page objects
</commit_message>
<xml_diff>
--- a/src/test/resources/DataSet/NMCO_ONB.xlsx
+++ b/src/test/resources/DataSet/NMCO_ONB.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2471" uniqueCount="538">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2457" uniqueCount="537">
   <si>
     <t xml:space="preserve">TestCaseName</t>
   </si>
@@ -1771,9 +1771,6 @@
       </rPr>
       <t xml:space="preserve">);</t>
     </r>
-  </si>
-  <si>
-    <t>https://artifactory.appzillon.com/artifactory/android-apk/ao/automation/qaDebug-1.0.20-09-02-2022-19:04.apk</t>
   </si>
 </sst>
 </file>
@@ -2230,61 +2227,61 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A169" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="0" topLeftCell="Z169" activePane="topRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A169" activeCellId="0" sqref="A169"/>
-      <selection pane="topRight" activeCell="AD175" activeCellId="0" sqref="AD175"/>
+      <selection pane="topRight" activeCell="AC175" activeCellId="0" sqref="AC175"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" customWidth="true" hidden="false" style="1" width="32.3" collapsed="true" outlineLevel="0"/>
-    <col min="2" max="2" customWidth="true" hidden="false" style="1" width="14.33" collapsed="true" outlineLevel="0"/>
-    <col min="3" max="3" customWidth="true" hidden="false" style="1" width="4.43" collapsed="true" outlineLevel="0"/>
-    <col min="4" max="4" customWidth="true" hidden="false" style="1" width="7.83" collapsed="true" outlineLevel="0"/>
-    <col min="5" max="6" customWidth="true" hidden="false" style="1" width="11.9" collapsed="true" outlineLevel="0"/>
-    <col min="7" max="8" customWidth="true" hidden="false" style="1" width="15.54" collapsed="true" outlineLevel="0"/>
-    <col min="9" max="9" customWidth="true" hidden="false" style="1" width="17.31" collapsed="true" outlineLevel="0"/>
-    <col min="10" max="10" customWidth="true" hidden="false" style="1" width="16.2" collapsed="true" outlineLevel="0"/>
-    <col min="11" max="11" customWidth="true" hidden="false" style="2" width="22.49" collapsed="true" outlineLevel="0"/>
-    <col min="12" max="12" customWidth="true" hidden="false" style="1" width="22.49" collapsed="true" outlineLevel="0"/>
-    <col min="13" max="13" customWidth="true" hidden="false" style="1" width="17.86" collapsed="true" outlineLevel="0"/>
-    <col min="14" max="14" customWidth="true" hidden="false" style="1" width="16.2" collapsed="true" outlineLevel="0"/>
-    <col min="15" max="15" customWidth="true" hidden="false" style="1" width="15.21" collapsed="true" outlineLevel="0"/>
-    <col min="16" max="16" customWidth="true" hidden="false" style="1" width="13.78" collapsed="true" outlineLevel="0"/>
-    <col min="17" max="17" customWidth="true" hidden="false" style="1" width="13.56" collapsed="true" outlineLevel="0"/>
-    <col min="18" max="18" customWidth="true" hidden="false" style="1" width="24.43" collapsed="true" outlineLevel="0"/>
-    <col min="19" max="19" customWidth="true" hidden="false" style="1" width="20.28" collapsed="true" outlineLevel="0"/>
-    <col min="20" max="20" customWidth="true" hidden="false" style="1" width="14.11" collapsed="true" outlineLevel="0"/>
-    <col min="21" max="21" customWidth="true" hidden="false" style="2" width="19.51" collapsed="true" outlineLevel="0"/>
-    <col min="22" max="22" customWidth="true" hidden="false" style="2" width="21.17" collapsed="true" outlineLevel="0"/>
-    <col min="23" max="23" customWidth="true" hidden="false" style="1" width="14.99" collapsed="true" outlineLevel="0"/>
-    <col min="24" max="25" customWidth="true" hidden="false" style="1" width="19.51" collapsed="true" outlineLevel="0"/>
-    <col min="26" max="26" customWidth="true" hidden="false" style="1" width="24.36" collapsed="true" outlineLevel="0"/>
-    <col min="27" max="27" customWidth="true" hidden="false" style="1" width="13.0" collapsed="true" outlineLevel="0"/>
-    <col min="28" max="28" customWidth="true" hidden="false" style="1" width="18.85" collapsed="true" outlineLevel="0"/>
-    <col min="29" max="29" customWidth="true" hidden="false" style="1" width="19.95" collapsed="true" outlineLevel="0"/>
-    <col min="30" max="31" customWidth="true" hidden="false" style="1" width="21.04" collapsed="true" outlineLevel="0"/>
-    <col min="32" max="32" customWidth="true" hidden="false" style="1" width="22.49" collapsed="true" outlineLevel="0"/>
-    <col min="33" max="33" customWidth="true" hidden="false" style="1" width="20.94" collapsed="true" outlineLevel="0"/>
-    <col min="34" max="34" customWidth="true" hidden="false" style="1" width="20.28" collapsed="true" outlineLevel="0"/>
-    <col min="35" max="35" customWidth="true" hidden="false" style="1" width="21.04" collapsed="true" outlineLevel="0"/>
-    <col min="36" max="37" customWidth="true" hidden="false" style="1" width="19.4" collapsed="true" outlineLevel="0"/>
-    <col min="38" max="38" customWidth="true" hidden="false" style="1" width="18.3" collapsed="true" outlineLevel="0"/>
-    <col min="39" max="39" customWidth="true" hidden="false" style="1" width="19.95" collapsed="true" outlineLevel="0"/>
-    <col min="40" max="40" customWidth="true" hidden="false" style="2" width="20.84" collapsed="true" outlineLevel="0"/>
-    <col min="41" max="41" customWidth="true" hidden="false" style="3" width="32.74" collapsed="true" outlineLevel="0"/>
-    <col min="42" max="42" customWidth="true" hidden="false" style="1" width="22.04" collapsed="true" outlineLevel="0"/>
-    <col min="43" max="43" customWidth="true" hidden="false" style="1" width="8.57" collapsed="true" outlineLevel="0"/>
-    <col min="44" max="44" customWidth="true" hidden="false" style="1" width="20.94" collapsed="true" outlineLevel="0"/>
-    <col min="45" max="45" customWidth="true" hidden="false" style="1" width="15.11" collapsed="true" outlineLevel="0"/>
-    <col min="46" max="46" customWidth="true" hidden="false" style="1" width="19.18" collapsed="true" outlineLevel="0"/>
-    <col min="47" max="47" customWidth="true" hidden="false" style="1" width="16.74" collapsed="true" outlineLevel="0"/>
-    <col min="48" max="48" customWidth="true" hidden="false" style="3" width="14.0" collapsed="true" outlineLevel="0"/>
-    <col min="49" max="49" customWidth="true" hidden="false" style="3" width="16.11" collapsed="true" outlineLevel="0"/>
-    <col min="50" max="50" customWidth="true" hidden="false" style="1" width="12.35" collapsed="true" outlineLevel="0"/>
-    <col min="51" max="52" customWidth="true" hidden="false" style="1" width="17.64" collapsed="true" outlineLevel="0"/>
-    <col min="53" max="53" customWidth="true" hidden="false" style="1" width="18.08" collapsed="true" outlineLevel="0"/>
-    <col min="54" max="54" customWidth="true" hidden="false" style="2" width="18.08" collapsed="true" outlineLevel="0"/>
-    <col min="55" max="990" customWidth="true" hidden="false" style="1" width="8.57" collapsed="true" outlineLevel="0"/>
-    <col min="991" max="1025" customWidth="true" hidden="false" style="4" width="9.14" collapsed="true" outlineLevel="0"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="32.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="14.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="4.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="7.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="1" width="11.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="1" width="15.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="17.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="16.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="2" width="22.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="22.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="17.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="16.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="15.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="13.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="13.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="24.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="1" width="20.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="1" width="14.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="2" width="19.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="2" width="21.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="1" width="14.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="24" style="1" width="19.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="1" width="24.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="1" width="13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="1" width="18.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="1" width="19.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="30" style="1" width="21.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="32" style="1" width="22.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="33" style="1" width="20.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="34" min="34" style="1" width="20.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="35" min="35" style="1" width="21.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="37" min="36" style="1" width="19.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="38" min="38" style="1" width="18.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="39" min="39" style="1" width="19.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="40" min="40" style="2" width="20.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="41" min="41" style="3" width="32.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="42" min="42" style="1" width="22.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="43" min="43" style="1" width="8.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="44" min="44" style="1" width="20.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="45" min="45" style="1" width="15.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="46" min="46" style="1" width="19.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="47" min="47" style="1" width="16.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="48" min="48" style="3" width="14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="49" min="49" style="3" width="16.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="50" min="50" style="1" width="12.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="52" min="51" style="1" width="17.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="53" min="53" style="1" width="18.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="54" min="54" style="2" width="18.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="990" min="55" style="1" width="8.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="991" style="4" width="9.14"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -16680,7 +16677,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="175" customFormat="false" ht="55.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="175" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A175" s="1" t="s">
         <v>403</v>
       </c>
@@ -16754,16 +16751,16 @@
         <v>405</v>
       </c>
       <c r="AD175" s="1" t="s">
-        <v>406</v>
+        <v>411</v>
       </c>
       <c r="AE175" s="1" t="s">
-        <v>407</v>
+        <v>412</v>
       </c>
       <c r="AF175" s="1" t="s">
-        <v>408</v>
+        <v>413</v>
       </c>
       <c r="AG175" s="1" t="s">
-        <v>409</v>
+        <v>414</v>
       </c>
     </row>
     <row r="176" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17911,22 +17908,22 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" customWidth="true" hidden="false" style="11" width="12.57" collapsed="true" outlineLevel="0"/>
-    <col min="2" max="2" customWidth="true" hidden="false" style="11" width="5.18" collapsed="true" outlineLevel="0"/>
-    <col min="3" max="4" customWidth="true" hidden="false" style="11" width="9.17" collapsed="true" outlineLevel="0"/>
-    <col min="5" max="5" customWidth="true" hidden="false" style="11" width="19.4" collapsed="true" outlineLevel="0"/>
-    <col min="6" max="6" customWidth="true" hidden="false" style="11" width="20.5" collapsed="true" outlineLevel="0"/>
-    <col min="7" max="7" customWidth="true" hidden="false" style="11" width="15.11" collapsed="true" outlineLevel="0"/>
-    <col min="8" max="8" customWidth="true" hidden="false" style="11" width="9.17" collapsed="true" outlineLevel="0"/>
-    <col min="9" max="9" customWidth="true" hidden="false" style="11" width="18.85" collapsed="true" outlineLevel="0"/>
-    <col min="10" max="10" customWidth="true" hidden="false" style="11" width="9.17" collapsed="true" outlineLevel="0"/>
-    <col min="11" max="11" customWidth="true" hidden="false" style="11" width="17.86" collapsed="true" outlineLevel="0"/>
-    <col min="12" max="13" customWidth="true" hidden="false" style="11" width="14.87" collapsed="true" outlineLevel="0"/>
-    <col min="14" max="14" customWidth="true" hidden="false" style="11" width="19.18" collapsed="true" outlineLevel="0"/>
-    <col min="15" max="15" customWidth="true" hidden="false" style="11" width="26.35" collapsed="true" outlineLevel="0"/>
-    <col min="16" max="17" customWidth="true" hidden="false" style="11" width="9.17" collapsed="true" outlineLevel="0"/>
-    <col min="18" max="18" customWidth="true" hidden="false" style="11" width="29.45" collapsed="true" outlineLevel="0"/>
-    <col min="19" max="1025" customWidth="true" hidden="false" style="11" width="9.17" collapsed="true" outlineLevel="0"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="11" width="12.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="11" width="5.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="11" width="9.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="11" width="19.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="11" width="20.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="11" width="15.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="11" width="9.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="11" width="18.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="11" width="9.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="11" width="17.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="12" style="11" width="14.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="11" width="19.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="11" width="26.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="16" style="11" width="9.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="11" width="29.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="19" style="11" width="9.17"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18001,28 +17998,21 @@
       <c r="D2" s="23" t="s">
         <v>463</v>
       </c>
-      <c r="E2"/>
-      <c r="F2"/>
       <c r="G2" s="23" t="s">
         <v>464</v>
       </c>
-      <c r="H2"/>
       <c r="I2" s="23" t="s">
         <v>465</v>
       </c>
       <c r="J2" s="24" t="s">
         <v>466</v>
       </c>
-      <c r="K2"/>
-      <c r="L2"/>
-      <c r="M2"/>
       <c r="N2" s="25" t="s">
         <v>467</v>
       </c>
       <c r="O2" s="12" t="s">
         <v>468</v>
       </c>
-      <c r="P2"/>
       <c r="Q2" s="24" t="n">
         <v>500</v>
       </c>
@@ -18046,35 +18036,28 @@
       <c r="D3" s="22" t="s">
         <v>463</v>
       </c>
-      <c r="E3"/>
-      <c r="F3"/>
       <c r="G3" s="22" t="s">
         <v>464</v>
       </c>
-      <c r="H3"/>
       <c r="I3" s="27" t="s">
         <v>471</v>
       </c>
       <c r="J3" s="27" t="s">
         <v>466</v>
       </c>
-      <c r="K3"/>
-      <c r="L3"/>
-      <c r="M3"/>
       <c r="N3" s="25" t="s">
         <v>467</v>
       </c>
       <c r="O3" s="12" t="s">
         <v>468</v>
       </c>
-      <c r="P3"/>
       <c r="Q3" s="24" t="n">
         <v>501</v>
       </c>
       <c r="R3" s="27" t="s">
         <v>469</v>
       </c>
-      <c r="S3" s="28" t="b">
+      <c r="S3" s="28" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -18115,7 +18098,7 @@
         <v>480</v>
       </c>
       <c r="L4" s="32" t="s">
-        <v>537</v>
+        <v>481</v>
       </c>
       <c r="M4" s="12" t="s">
         <v>482</v>
@@ -18126,14 +18109,13 @@
       <c r="O4" s="12" t="s">
         <v>468</v>
       </c>
-      <c r="P4"/>
       <c r="Q4" s="24" t="n">
         <v>502</v>
       </c>
       <c r="R4" s="9" t="s">
         <v>484</v>
       </c>
-      <c r="S4" s="33" t="b">
+      <c r="S4" s="33" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -18184,14 +18166,13 @@
       <c r="O5" s="12" t="s">
         <v>468</v>
       </c>
-      <c r="P5"/>
       <c r="Q5" s="24" t="n">
         <v>503</v>
       </c>
       <c r="R5" s="9" t="s">
         <v>484</v>
       </c>
-      <c r="S5" s="33" t="b">
+      <c r="S5" s="33" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -18227,7 +18208,6 @@
       <c r="J6" s="9" t="s">
         <v>479</v>
       </c>
-      <c r="K6"/>
       <c r="L6" s="12" t="s">
         <v>490</v>
       </c>
@@ -18240,14 +18220,13 @@
       <c r="O6" s="12" t="s">
         <v>468</v>
       </c>
-      <c r="P6"/>
       <c r="Q6" s="24" t="n">
         <v>504</v>
       </c>
       <c r="R6" s="9" t="s">
         <v>484</v>
       </c>
-      <c r="S6" s="33" t="b">
+      <c r="S6" s="33" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -18283,8 +18262,6 @@
       <c r="J7" s="9" t="s">
         <v>479</v>
       </c>
-      <c r="K7"/>
-      <c r="L7"/>
       <c r="M7" s="12" t="s">
         <v>482</v>
       </c>
@@ -18294,14 +18271,13 @@
       <c r="O7" s="12" t="s">
         <v>468</v>
       </c>
-      <c r="P7"/>
       <c r="Q7" s="24" t="n">
         <v>505</v>
       </c>
       <c r="R7" s="9" t="s">
         <v>484</v>
       </c>
-      <c r="S7" s="33" t="b">
+      <c r="S7" s="33" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -18343,17 +18319,13 @@
       <c r="L8" s="11" t="s">
         <v>498</v>
       </c>
-      <c r="M8"/>
-      <c r="N8"/>
-      <c r="O8"/>
-      <c r="P8"/>
       <c r="Q8" s="24" t="n">
         <v>506</v>
       </c>
       <c r="R8" s="9" t="s">
         <v>499</v>
       </c>
-      <c r="S8" s="33" t="b">
+      <c r="S8" s="33" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -18392,30 +18364,18 @@
       <c r="K9" s="35" t="s">
         <v>497</v>
       </c>
-      <c r="L9"/>
-      <c r="M9"/>
-      <c r="N9"/>
-      <c r="O9"/>
-      <c r="P9"/>
       <c r="Q9" s="24" t="n">
         <v>507</v>
       </c>
       <c r="R9" s="9" t="s">
         <v>499</v>
       </c>
-      <c r="S9" s="33" t="b">
+      <c r="S9" s="33" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10"/>
-      <c r="B10"/>
-      <c r="C10"/>
-      <c r="D10"/>
-      <c r="E10"/>
-      <c r="F10"/>
-      <c r="G10"/>
       <c r="H10" s="34" t="s">
         <v>503</v>
       </c>
@@ -18425,15 +18385,6 @@
       <c r="J10" s="31" t="s">
         <v>496</v>
       </c>
-      <c r="K10"/>
-      <c r="L10"/>
-      <c r="M10"/>
-      <c r="N10"/>
-      <c r="O10"/>
-      <c r="P10"/>
-      <c r="Q10"/>
-      <c r="R10"/>
-      <c r="S10"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -18478,9 +18429,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" customWidth="true" hidden="false" style="0" width="9.14" collapsed="true" outlineLevel="0"/>
-    <col min="2" max="2" customWidth="true" hidden="false" style="0" width="13.93" collapsed="true" outlineLevel="0"/>
-    <col min="3" max="1025" customWidth="true" hidden="false" style="0" width="9.14" collapsed="true" outlineLevel="0"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="9.14"/>
   </cols>
   <sheetData>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
made changes in jenkins file
</commit_message>
<xml_diff>
--- a/src/test/resources/DataSet/NMCO_ONB.xlsx
+++ b/src/test/resources/DataSet/NMCO_ONB.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2553" uniqueCount="551">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2554" uniqueCount="552">
   <si>
     <t xml:space="preserve">TestCaseName</t>
   </si>
@@ -1813,6 +1813,9 @@
       </rPr>
       <t xml:space="preserve">);</t>
     </r>
+  </si>
+  <si>
+    <t>https://artifactory.appzillon.com/artifactory/android-apk/ao/automation/qaDebug-1.0.21-24-02-2022-13:09.apk</t>
   </si>
 </sst>
 </file>
@@ -2272,56 +2275,56 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="32.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="14.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="4.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="7.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="1" width="11.9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="1" width="15.54"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="17.31"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="16.2"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="2" width="22.49"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="22.49"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="17.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="16.2"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="15.21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="13.78"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="13.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="24.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="1" width="20.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="1" width="14.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="2" width="19.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="2" width="21.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="1" width="14.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="24" style="1" width="19.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="1" width="24.36"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="1" width="13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="1" width="18.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="1" width="19.95"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="30" style="1" width="21.04"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="32" style="1" width="22.49"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="33" style="1" width="20.94"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="34" min="34" style="1" width="20.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="35" min="35" style="1" width="21.04"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="37" min="36" style="1" width="19.4"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="38" min="38" style="1" width="18.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="39" min="39" style="1" width="19.95"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="40" min="40" style="2" width="20.84"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="41" min="41" style="3" width="32.74"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="42" min="42" style="1" width="22.04"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="43" min="43" style="1" width="8.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="44" min="44" style="1" width="20.94"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="45" min="45" style="1" width="15.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="46" min="46" style="1" width="19.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="47" min="47" style="1" width="16.74"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="48" min="48" style="3" width="14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="49" min="49" style="3" width="16.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="50" min="50" style="1" width="12.35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="52" min="51" style="1" width="17.64"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="53" min="53" style="1" width="18.08"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="54" min="54" style="2" width="18.08"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="990" min="55" style="1" width="8.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="991" style="4" width="9.14"/>
+    <col min="1" max="1" customWidth="true" hidden="false" style="1" width="32.3" collapsed="true" outlineLevel="0"/>
+    <col min="2" max="2" customWidth="true" hidden="false" style="1" width="14.33" collapsed="true" outlineLevel="0"/>
+    <col min="3" max="3" customWidth="true" hidden="false" style="1" width="4.43" collapsed="true" outlineLevel="0"/>
+    <col min="4" max="4" customWidth="true" hidden="false" style="1" width="7.83" collapsed="true" outlineLevel="0"/>
+    <col min="5" max="6" customWidth="true" hidden="false" style="1" width="11.9" collapsed="true" outlineLevel="0"/>
+    <col min="7" max="8" customWidth="true" hidden="false" style="1" width="15.54" collapsed="true" outlineLevel="0"/>
+    <col min="9" max="9" customWidth="true" hidden="false" style="1" width="17.31" collapsed="true" outlineLevel="0"/>
+    <col min="10" max="10" customWidth="true" hidden="false" style="1" width="16.2" collapsed="true" outlineLevel="0"/>
+    <col min="11" max="11" customWidth="true" hidden="false" style="2" width="22.49" collapsed="true" outlineLevel="0"/>
+    <col min="12" max="12" customWidth="true" hidden="false" style="1" width="22.49" collapsed="true" outlineLevel="0"/>
+    <col min="13" max="13" customWidth="true" hidden="false" style="1" width="17.86" collapsed="true" outlineLevel="0"/>
+    <col min="14" max="14" customWidth="true" hidden="false" style="1" width="16.2" collapsed="true" outlineLevel="0"/>
+    <col min="15" max="15" customWidth="true" hidden="false" style="1" width="15.21" collapsed="true" outlineLevel="0"/>
+    <col min="16" max="16" customWidth="true" hidden="false" style="1" width="13.78" collapsed="true" outlineLevel="0"/>
+    <col min="17" max="17" customWidth="true" hidden="false" style="1" width="13.56" collapsed="true" outlineLevel="0"/>
+    <col min="18" max="18" customWidth="true" hidden="false" style="1" width="24.43" collapsed="true" outlineLevel="0"/>
+    <col min="19" max="19" customWidth="true" hidden="false" style="1" width="20.28" collapsed="true" outlineLevel="0"/>
+    <col min="20" max="20" customWidth="true" hidden="false" style="1" width="14.11" collapsed="true" outlineLevel="0"/>
+    <col min="21" max="21" customWidth="true" hidden="false" style="2" width="19.51" collapsed="true" outlineLevel="0"/>
+    <col min="22" max="22" customWidth="true" hidden="false" style="2" width="21.17" collapsed="true" outlineLevel="0"/>
+    <col min="23" max="23" customWidth="true" hidden="false" style="1" width="14.99" collapsed="true" outlineLevel="0"/>
+    <col min="24" max="25" customWidth="true" hidden="false" style="1" width="19.51" collapsed="true" outlineLevel="0"/>
+    <col min="26" max="26" customWidth="true" hidden="false" style="1" width="24.36" collapsed="true" outlineLevel="0"/>
+    <col min="27" max="27" customWidth="true" hidden="false" style="1" width="13.0" collapsed="true" outlineLevel="0"/>
+    <col min="28" max="28" customWidth="true" hidden="false" style="1" width="18.85" collapsed="true" outlineLevel="0"/>
+    <col min="29" max="29" customWidth="true" hidden="false" style="1" width="19.95" collapsed="true" outlineLevel="0"/>
+    <col min="30" max="31" customWidth="true" hidden="false" style="1" width="21.04" collapsed="true" outlineLevel="0"/>
+    <col min="32" max="32" customWidth="true" hidden="false" style="1" width="22.49" collapsed="true" outlineLevel="0"/>
+    <col min="33" max="33" customWidth="true" hidden="false" style="1" width="20.94" collapsed="true" outlineLevel="0"/>
+    <col min="34" max="34" customWidth="true" hidden="false" style="1" width="20.28" collapsed="true" outlineLevel="0"/>
+    <col min="35" max="35" customWidth="true" hidden="false" style="1" width="21.04" collapsed="true" outlineLevel="0"/>
+    <col min="36" max="37" customWidth="true" hidden="false" style="1" width="19.4" collapsed="true" outlineLevel="0"/>
+    <col min="38" max="38" customWidth="true" hidden="false" style="1" width="18.3" collapsed="true" outlineLevel="0"/>
+    <col min="39" max="39" customWidth="true" hidden="false" style="1" width="19.95" collapsed="true" outlineLevel="0"/>
+    <col min="40" max="40" customWidth="true" hidden="false" style="2" width="20.84" collapsed="true" outlineLevel="0"/>
+    <col min="41" max="41" customWidth="true" hidden="false" style="3" width="32.74" collapsed="true" outlineLevel="0"/>
+    <col min="42" max="42" customWidth="true" hidden="false" style="1" width="22.04" collapsed="true" outlineLevel="0"/>
+    <col min="43" max="43" customWidth="true" hidden="false" style="1" width="8.57" collapsed="true" outlineLevel="0"/>
+    <col min="44" max="44" customWidth="true" hidden="false" style="1" width="20.94" collapsed="true" outlineLevel="0"/>
+    <col min="45" max="45" customWidth="true" hidden="false" style="1" width="15.11" collapsed="true" outlineLevel="0"/>
+    <col min="46" max="46" customWidth="true" hidden="false" style="1" width="19.18" collapsed="true" outlineLevel="0"/>
+    <col min="47" max="47" customWidth="true" hidden="false" style="1" width="16.74" collapsed="true" outlineLevel="0"/>
+    <col min="48" max="48" customWidth="true" hidden="false" style="3" width="14.0" collapsed="true" outlineLevel="0"/>
+    <col min="49" max="49" customWidth="true" hidden="false" style="3" width="16.11" collapsed="true" outlineLevel="0"/>
+    <col min="50" max="50" customWidth="true" hidden="false" style="1" width="12.35" collapsed="true" outlineLevel="0"/>
+    <col min="51" max="52" customWidth="true" hidden="false" style="1" width="17.64" collapsed="true" outlineLevel="0"/>
+    <col min="53" max="53" customWidth="true" hidden="false" style="1" width="18.08" collapsed="true" outlineLevel="0"/>
+    <col min="54" max="54" customWidth="true" hidden="false" style="2" width="18.08" collapsed="true" outlineLevel="0"/>
+    <col min="55" max="990" customWidth="true" hidden="false" style="1" width="8.57" collapsed="true" outlineLevel="0"/>
+    <col min="991" max="1025" customWidth="true" hidden="false" style="4" width="9.14" collapsed="true" outlineLevel="0"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18366,22 +18369,22 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="11" width="12.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="11" width="5.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="11" width="9.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="11" width="19.4"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="11" width="20.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="11" width="15.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="11" width="9.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="11" width="18.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="11" width="9.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="11" width="17.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="12" style="11" width="14.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="11" width="19.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="11" width="26.35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="16" style="11" width="9.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="11" width="29.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="19" style="11" width="9.17"/>
+    <col min="1" max="1" customWidth="true" hidden="false" style="11" width="12.57" collapsed="true" outlineLevel="0"/>
+    <col min="2" max="2" customWidth="true" hidden="false" style="11" width="5.18" collapsed="true" outlineLevel="0"/>
+    <col min="3" max="4" customWidth="true" hidden="false" style="11" width="9.17" collapsed="true" outlineLevel="0"/>
+    <col min="5" max="5" customWidth="true" hidden="false" style="11" width="19.4" collapsed="true" outlineLevel="0"/>
+    <col min="6" max="6" customWidth="true" hidden="false" style="11" width="20.5" collapsed="true" outlineLevel="0"/>
+    <col min="7" max="7" customWidth="true" hidden="false" style="11" width="15.11" collapsed="true" outlineLevel="0"/>
+    <col min="8" max="8" customWidth="true" hidden="false" style="11" width="9.17" collapsed="true" outlineLevel="0"/>
+    <col min="9" max="9" customWidth="true" hidden="false" style="11" width="18.85" collapsed="true" outlineLevel="0"/>
+    <col min="10" max="10" customWidth="true" hidden="false" style="11" width="9.17" collapsed="true" outlineLevel="0"/>
+    <col min="11" max="11" customWidth="true" hidden="false" style="11" width="17.86" collapsed="true" outlineLevel="0"/>
+    <col min="12" max="13" customWidth="true" hidden="false" style="11" width="14.87" collapsed="true" outlineLevel="0"/>
+    <col min="14" max="14" customWidth="true" hidden="false" style="11" width="19.18" collapsed="true" outlineLevel="0"/>
+    <col min="15" max="15" customWidth="true" hidden="false" style="11" width="26.35" collapsed="true" outlineLevel="0"/>
+    <col min="16" max="17" customWidth="true" hidden="false" style="11" width="9.17" collapsed="true" outlineLevel="0"/>
+    <col min="18" max="18" customWidth="true" hidden="false" style="11" width="29.45" collapsed="true" outlineLevel="0"/>
+    <col min="19" max="1025" customWidth="true" hidden="false" style="11" width="9.17" collapsed="true" outlineLevel="0"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18456,21 +18459,28 @@
       <c r="D2" s="23" t="s">
         <v>477</v>
       </c>
+      <c r="E2"/>
+      <c r="F2"/>
       <c r="G2" s="23" t="s">
         <v>478</v>
       </c>
+      <c r="H2"/>
       <c r="I2" s="23" t="s">
         <v>479</v>
       </c>
       <c r="J2" s="24" t="s">
         <v>480</v>
       </c>
+      <c r="K2"/>
+      <c r="L2"/>
+      <c r="M2"/>
       <c r="N2" s="25" t="s">
         <v>481</v>
       </c>
       <c r="O2" s="12" t="s">
         <v>482</v>
       </c>
+      <c r="P2"/>
       <c r="Q2" s="24" t="n">
         <v>500</v>
       </c>
@@ -18494,28 +18504,35 @@
       <c r="D3" s="22" t="s">
         <v>477</v>
       </c>
+      <c r="E3"/>
+      <c r="F3"/>
       <c r="G3" s="22" t="s">
         <v>478</v>
       </c>
+      <c r="H3"/>
       <c r="I3" s="27" t="s">
         <v>485</v>
       </c>
       <c r="J3" s="27" t="s">
         <v>480</v>
       </c>
+      <c r="K3"/>
+      <c r="L3"/>
+      <c r="M3"/>
       <c r="N3" s="25" t="s">
         <v>481</v>
       </c>
       <c r="O3" s="12" t="s">
         <v>482</v>
       </c>
+      <c r="P3"/>
       <c r="Q3" s="24" t="n">
         <v>501</v>
       </c>
       <c r="R3" s="27" t="s">
         <v>483</v>
       </c>
-      <c r="S3" s="28" t="n">
+      <c r="S3" s="28" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -18556,7 +18573,7 @@
         <v>494</v>
       </c>
       <c r="L4" s="32" t="s">
-        <v>495</v>
+        <v>551</v>
       </c>
       <c r="M4" s="12" t="s">
         <v>496</v>
@@ -18567,13 +18584,14 @@
       <c r="O4" s="12" t="s">
         <v>482</v>
       </c>
+      <c r="P4"/>
       <c r="Q4" s="24" t="n">
         <v>502</v>
       </c>
       <c r="R4" s="9" t="s">
         <v>498</v>
       </c>
-      <c r="S4" s="33" t="n">
+      <c r="S4" s="33" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -18624,13 +18642,14 @@
       <c r="O5" s="12" t="s">
         <v>482</v>
       </c>
+      <c r="P5"/>
       <c r="Q5" s="24" t="n">
         <v>503</v>
       </c>
       <c r="R5" s="9" t="s">
         <v>498</v>
       </c>
-      <c r="S5" s="33" t="n">
+      <c r="S5" s="33" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -18666,6 +18685,7 @@
       <c r="J6" s="9" t="s">
         <v>493</v>
       </c>
+      <c r="K6"/>
       <c r="L6" s="12" t="s">
         <v>504</v>
       </c>
@@ -18678,13 +18698,14 @@
       <c r="O6" s="12" t="s">
         <v>482</v>
       </c>
+      <c r="P6"/>
       <c r="Q6" s="24" t="n">
         <v>504</v>
       </c>
       <c r="R6" s="9" t="s">
         <v>498</v>
       </c>
-      <c r="S6" s="33" t="n">
+      <c r="S6" s="33" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -18720,6 +18741,8 @@
       <c r="J7" s="9" t="s">
         <v>493</v>
       </c>
+      <c r="K7"/>
+      <c r="L7"/>
       <c r="M7" s="12" t="s">
         <v>496</v>
       </c>
@@ -18729,13 +18752,14 @@
       <c r="O7" s="12" t="s">
         <v>482</v>
       </c>
+      <c r="P7"/>
       <c r="Q7" s="24" t="n">
         <v>505</v>
       </c>
       <c r="R7" s="9" t="s">
         <v>498</v>
       </c>
-      <c r="S7" s="33" t="n">
+      <c r="S7" s="33" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -18777,13 +18801,17 @@
       <c r="L8" s="11" t="s">
         <v>512</v>
       </c>
+      <c r="M8"/>
+      <c r="N8"/>
+      <c r="O8"/>
+      <c r="P8"/>
       <c r="Q8" s="24" t="n">
         <v>506</v>
       </c>
       <c r="R8" s="9" t="s">
         <v>513</v>
       </c>
-      <c r="S8" s="33" t="n">
+      <c r="S8" s="33" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -18822,18 +18850,30 @@
       <c r="K9" s="35" t="s">
         <v>511</v>
       </c>
+      <c r="L9"/>
+      <c r="M9"/>
+      <c r="N9"/>
+      <c r="O9"/>
+      <c r="P9"/>
       <c r="Q9" s="24" t="n">
         <v>507</v>
       </c>
       <c r="R9" s="9" t="s">
         <v>513</v>
       </c>
-      <c r="S9" s="33" t="n">
+      <c r="S9" s="33" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10"/>
+      <c r="B10"/>
+      <c r="C10"/>
+      <c r="D10"/>
+      <c r="E10"/>
+      <c r="F10"/>
+      <c r="G10"/>
       <c r="H10" s="34" t="s">
         <v>517</v>
       </c>
@@ -18843,6 +18883,15 @@
       <c r="J10" s="31" t="s">
         <v>510</v>
       </c>
+      <c r="K10"/>
+      <c r="L10"/>
+      <c r="M10"/>
+      <c r="N10"/>
+      <c r="O10"/>
+      <c r="P10"/>
+      <c r="Q10"/>
+      <c r="R10"/>
+      <c r="S10"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -18887,9 +18936,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.93"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="9.14"/>
+    <col min="1" max="1" customWidth="true" hidden="false" style="0" width="9.14" collapsed="true" outlineLevel="0"/>
+    <col min="2" max="2" customWidth="true" hidden="false" style="0" width="13.93" collapsed="true" outlineLevel="0"/>
+    <col min="3" max="1025" customWidth="true" hidden="false" style="0" width="9.14" collapsed="true" outlineLevel="0"/>
   </cols>
   <sheetData>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
made changes in IOS entity contact info features
</commit_message>
<xml_diff>
--- a/src/test/resources/DataSet/NMCO_ONB.xlsx
+++ b/src/test/resources/DataSet/NMCO_ONB.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2664" uniqueCount="565">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2660" uniqueCount="564">
   <si>
     <t xml:space="preserve">TestCaseName</t>
   </si>
@@ -1852,9 +1852,6 @@
   </si>
   <si>
     <t xml:space="preserve">e2e testdata</t>
-  </si>
-  <si>
-    <t>null</t>
   </si>
 </sst>
 </file>
@@ -2309,61 +2306,61 @@
   <dimension ref="A1:AMJ202"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A196" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E202" activeCellId="0" sqref="E202"/>
+      <selection pane="topLeft" activeCell="D201" activeCellId="0" sqref="D201"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" customWidth="true" hidden="false" style="1" width="32.3" collapsed="true" outlineLevel="0"/>
-    <col min="2" max="2" customWidth="true" hidden="false" style="1" width="14.33" collapsed="true" outlineLevel="0"/>
-    <col min="3" max="3" customWidth="true" hidden="false" style="1" width="4.43" collapsed="true" outlineLevel="0"/>
-    <col min="4" max="4" customWidth="true" hidden="false" style="1" width="7.83" collapsed="true" outlineLevel="0"/>
-    <col min="5" max="6" customWidth="true" hidden="false" style="1" width="11.9" collapsed="true" outlineLevel="0"/>
-    <col min="7" max="8" customWidth="true" hidden="false" style="1" width="15.54" collapsed="true" outlineLevel="0"/>
-    <col min="9" max="9" customWidth="true" hidden="false" style="1" width="17.31" collapsed="true" outlineLevel="0"/>
-    <col min="10" max="10" customWidth="true" hidden="false" style="1" width="16.2" collapsed="true" outlineLevel="0"/>
-    <col min="11" max="11" customWidth="true" hidden="false" style="2" width="22.49" collapsed="true" outlineLevel="0"/>
-    <col min="12" max="12" customWidth="true" hidden="false" style="1" width="22.49" collapsed="true" outlineLevel="0"/>
-    <col min="13" max="13" customWidth="true" hidden="false" style="1" width="17.86" collapsed="true" outlineLevel="0"/>
-    <col min="14" max="14" customWidth="true" hidden="false" style="1" width="16.2" collapsed="true" outlineLevel="0"/>
-    <col min="15" max="15" customWidth="true" hidden="false" style="1" width="15.21" collapsed="true" outlineLevel="0"/>
-    <col min="16" max="16" customWidth="true" hidden="false" style="1" width="13.78" collapsed="true" outlineLevel="0"/>
-    <col min="17" max="17" customWidth="true" hidden="false" style="1" width="13.56" collapsed="true" outlineLevel="0"/>
-    <col min="18" max="18" customWidth="true" hidden="false" style="1" width="24.43" collapsed="true" outlineLevel="0"/>
-    <col min="19" max="19" customWidth="true" hidden="false" style="1" width="20.28" collapsed="true" outlineLevel="0"/>
-    <col min="20" max="20" customWidth="true" hidden="false" style="1" width="14.11" collapsed="true" outlineLevel="0"/>
-    <col min="21" max="21" customWidth="true" hidden="false" style="2" width="19.51" collapsed="true" outlineLevel="0"/>
-    <col min="22" max="22" customWidth="true" hidden="false" style="2" width="21.17" collapsed="true" outlineLevel="0"/>
-    <col min="23" max="23" customWidth="true" hidden="false" style="1" width="14.99" collapsed="true" outlineLevel="0"/>
-    <col min="24" max="25" customWidth="true" hidden="false" style="1" width="19.51" collapsed="true" outlineLevel="0"/>
-    <col min="26" max="26" customWidth="true" hidden="false" style="1" width="24.36" collapsed="true" outlineLevel="0"/>
-    <col min="27" max="27" customWidth="true" hidden="false" style="1" width="13.0" collapsed="true" outlineLevel="0"/>
-    <col min="28" max="28" customWidth="true" hidden="false" style="1" width="18.85" collapsed="true" outlineLevel="0"/>
-    <col min="29" max="29" customWidth="true" hidden="false" style="1" width="19.95" collapsed="true" outlineLevel="0"/>
-    <col min="30" max="31" customWidth="true" hidden="false" style="1" width="21.04" collapsed="true" outlineLevel="0"/>
-    <col min="32" max="32" customWidth="true" hidden="false" style="1" width="22.49" collapsed="true" outlineLevel="0"/>
-    <col min="33" max="33" customWidth="true" hidden="false" style="1" width="20.94" collapsed="true" outlineLevel="0"/>
-    <col min="34" max="34" customWidth="true" hidden="false" style="1" width="20.28" collapsed="true" outlineLevel="0"/>
-    <col min="35" max="35" customWidth="true" hidden="false" style="1" width="21.04" collapsed="true" outlineLevel="0"/>
-    <col min="36" max="37" customWidth="true" hidden="false" style="1" width="19.4" collapsed="true" outlineLevel="0"/>
-    <col min="38" max="38" customWidth="true" hidden="false" style="1" width="18.3" collapsed="true" outlineLevel="0"/>
-    <col min="39" max="39" customWidth="true" hidden="false" style="1" width="19.95" collapsed="true" outlineLevel="0"/>
-    <col min="40" max="40" customWidth="true" hidden="false" style="2" width="20.84" collapsed="true" outlineLevel="0"/>
-    <col min="41" max="41" customWidth="true" hidden="false" style="3" width="32.74" collapsed="true" outlineLevel="0"/>
-    <col min="42" max="42" customWidth="true" hidden="false" style="1" width="22.04" collapsed="true" outlineLevel="0"/>
-    <col min="43" max="43" customWidth="true" hidden="false" style="1" width="8.57" collapsed="true" outlineLevel="0"/>
-    <col min="44" max="44" customWidth="true" hidden="false" style="1" width="20.94" collapsed="true" outlineLevel="0"/>
-    <col min="45" max="45" customWidth="true" hidden="false" style="1" width="15.11" collapsed="true" outlineLevel="0"/>
-    <col min="46" max="46" customWidth="true" hidden="false" style="1" width="19.18" collapsed="true" outlineLevel="0"/>
-    <col min="47" max="47" customWidth="true" hidden="false" style="1" width="16.74" collapsed="true" outlineLevel="0"/>
-    <col min="48" max="48" customWidth="true" hidden="false" style="3" width="14.0" collapsed="true" outlineLevel="0"/>
-    <col min="49" max="49" customWidth="true" hidden="false" style="3" width="16.11" collapsed="true" outlineLevel="0"/>
-    <col min="50" max="50" customWidth="true" hidden="false" style="1" width="12.35" collapsed="true" outlineLevel="0"/>
-    <col min="51" max="52" customWidth="true" hidden="false" style="1" width="17.64" collapsed="true" outlineLevel="0"/>
-    <col min="53" max="53" customWidth="true" hidden="false" style="1" width="18.08" collapsed="true" outlineLevel="0"/>
-    <col min="54" max="54" customWidth="true" hidden="false" style="2" width="18.08" collapsed="true" outlineLevel="0"/>
-    <col min="55" max="990" customWidth="true" hidden="false" style="1" width="8.57" collapsed="true" outlineLevel="0"/>
-    <col min="991" max="1025" customWidth="true" hidden="false" style="4" width="9.14" collapsed="true" outlineLevel="0"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="32.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="14.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="4.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="7.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="1" width="11.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="1" width="15.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="17.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="16.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="2" width="22.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="22.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="17.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="16.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="15.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="13.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="13.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="24.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="1" width="20.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="1" width="14.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="2" width="19.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="2" width="21.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="1" width="14.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="24" style="1" width="19.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="1" width="24.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="1" width="13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="1" width="18.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="1" width="19.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="30" style="1" width="21.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="32" style="1" width="22.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="33" style="1" width="20.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="34" min="34" style="1" width="20.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="35" min="35" style="1" width="21.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="37" min="36" style="1" width="19.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="38" min="38" style="1" width="18.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="39" min="39" style="1" width="19.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="40" min="40" style="2" width="20.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="41" min="41" style="3" width="32.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="42" min="42" style="1" width="22.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="43" min="43" style="1" width="8.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="44" min="44" style="1" width="20.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="45" min="45" style="1" width="15.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="46" min="46" style="1" width="19.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="47" min="47" style="1" width="16.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="48" min="48" style="3" width="14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="49" min="49" style="3" width="16.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="50" min="50" style="1" width="12.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="52" min="51" style="1" width="17.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="53" min="53" style="1" width="18.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="54" min="54" style="2" width="18.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="990" min="55" style="1" width="8.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="991" style="4" width="9.14"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18839,27 +18836,27 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A44" activeCellId="0" sqref="A44"/>
-      <selection pane="bottomRight" activeCell="F1" activeCellId="1" sqref="E202 F1"/>
+      <selection pane="bottomRight" activeCell="F1" activeCellId="0" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" customWidth="true" hidden="false" style="11" width="12.57" collapsed="true" outlineLevel="0"/>
-    <col min="2" max="2" customWidth="true" hidden="false" style="11" width="5.18" collapsed="true" outlineLevel="0"/>
-    <col min="3" max="4" customWidth="true" hidden="false" style="11" width="9.17" collapsed="true" outlineLevel="0"/>
-    <col min="5" max="5" customWidth="true" hidden="false" style="11" width="19.4" collapsed="true" outlineLevel="0"/>
-    <col min="6" max="6" customWidth="true" hidden="false" style="11" width="20.5" collapsed="true" outlineLevel="0"/>
-    <col min="7" max="7" customWidth="true" hidden="false" style="11" width="15.11" collapsed="true" outlineLevel="0"/>
-    <col min="8" max="8" customWidth="true" hidden="false" style="11" width="9.17" collapsed="true" outlineLevel="0"/>
-    <col min="9" max="9" customWidth="true" hidden="false" style="11" width="18.85" collapsed="true" outlineLevel="0"/>
-    <col min="10" max="10" customWidth="true" hidden="false" style="11" width="9.17" collapsed="true" outlineLevel="0"/>
-    <col min="11" max="11" customWidth="true" hidden="false" style="11" width="17.86" collapsed="true" outlineLevel="0"/>
-    <col min="12" max="13" customWidth="true" hidden="false" style="11" width="14.87" collapsed="true" outlineLevel="0"/>
-    <col min="14" max="14" customWidth="true" hidden="false" style="11" width="19.18" collapsed="true" outlineLevel="0"/>
-    <col min="15" max="15" customWidth="true" hidden="false" style="11" width="26.35" collapsed="true" outlineLevel="0"/>
-    <col min="16" max="17" customWidth="true" hidden="false" style="11" width="9.17" collapsed="true" outlineLevel="0"/>
-    <col min="18" max="18" customWidth="true" hidden="false" style="11" width="29.45" collapsed="true" outlineLevel="0"/>
-    <col min="19" max="1025" customWidth="true" hidden="false" style="11" width="9.17" collapsed="true" outlineLevel="0"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="11" width="12.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="11" width="5.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="11" width="9.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="11" width="19.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="11" width="20.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="11" width="15.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="11" width="9.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="11" width="18.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="11" width="9.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="11" width="17.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="12" style="11" width="14.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="11" width="19.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="11" width="26.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="16" style="11" width="9.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="11" width="29.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="19" style="11" width="9.17"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18934,28 +18931,21 @@
       <c r="D2" s="23" t="s">
         <v>488</v>
       </c>
-      <c r="E2"/>
-      <c r="F2"/>
       <c r="G2" s="23" t="s">
         <v>489</v>
       </c>
-      <c r="H2"/>
       <c r="I2" s="23" t="s">
         <v>490</v>
       </c>
       <c r="J2" s="24" t="s">
         <v>491</v>
       </c>
-      <c r="K2"/>
-      <c r="L2"/>
-      <c r="M2"/>
       <c r="N2" s="25" t="s">
         <v>492</v>
       </c>
       <c r="O2" s="12" t="s">
         <v>493</v>
       </c>
-      <c r="P2"/>
       <c r="Q2" s="24" t="n">
         <v>500</v>
       </c>
@@ -18979,35 +18969,28 @@
       <c r="D3" s="22" t="s">
         <v>488</v>
       </c>
-      <c r="E3"/>
-      <c r="F3"/>
       <c r="G3" s="22" t="s">
         <v>489</v>
       </c>
-      <c r="H3"/>
       <c r="I3" s="27" t="s">
         <v>496</v>
       </c>
       <c r="J3" s="27" t="s">
         <v>491</v>
       </c>
-      <c r="K3"/>
-      <c r="L3"/>
-      <c r="M3"/>
       <c r="N3" s="25" t="s">
         <v>492</v>
       </c>
       <c r="O3" s="12" t="s">
         <v>493</v>
       </c>
-      <c r="P3"/>
       <c r="Q3" s="24" t="n">
         <v>501</v>
       </c>
       <c r="R3" s="27" t="s">
         <v>494</v>
       </c>
-      <c r="S3" s="28" t="b">
+      <c r="S3" s="28" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -19059,14 +19042,13 @@
       <c r="O4" s="12" t="s">
         <v>493</v>
       </c>
-      <c r="P4"/>
       <c r="Q4" s="24" t="n">
         <v>502</v>
       </c>
       <c r="R4" s="9" t="s">
         <v>509</v>
       </c>
-      <c r="S4" s="33" t="b">
+      <c r="S4" s="33" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -19117,14 +19099,13 @@
       <c r="O5" s="12" t="s">
         <v>493</v>
       </c>
-      <c r="P5"/>
       <c r="Q5" s="24" t="n">
         <v>503</v>
       </c>
       <c r="R5" s="9" t="s">
         <v>509</v>
       </c>
-      <c r="S5" s="33" t="b">
+      <c r="S5" s="33" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -19160,7 +19141,6 @@
       <c r="J6" s="9" t="s">
         <v>504</v>
       </c>
-      <c r="K6"/>
       <c r="L6" s="12" t="s">
         <v>516</v>
       </c>
@@ -19173,14 +19153,13 @@
       <c r="O6" s="12" t="s">
         <v>493</v>
       </c>
-      <c r="P6"/>
       <c r="Q6" s="24" t="n">
         <v>504</v>
       </c>
       <c r="R6" s="9" t="s">
         <v>509</v>
       </c>
-      <c r="S6" s="33" t="b">
+      <c r="S6" s="33" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -19216,8 +19195,6 @@
       <c r="J7" s="9" t="s">
         <v>504</v>
       </c>
-      <c r="K7"/>
-      <c r="L7"/>
       <c r="M7" s="12" t="s">
         <v>518</v>
       </c>
@@ -19227,14 +19204,13 @@
       <c r="O7" s="12" t="s">
         <v>493</v>
       </c>
-      <c r="P7"/>
       <c r="Q7" s="24" t="n">
         <v>505</v>
       </c>
       <c r="R7" s="9" t="s">
         <v>509</v>
       </c>
-      <c r="S7" s="33" t="b">
+      <c r="S7" s="33" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -19274,19 +19250,15 @@
         <v>524</v>
       </c>
       <c r="L8" s="11" t="s">
-        <v>564</v>
-      </c>
-      <c r="M8"/>
-      <c r="N8"/>
-      <c r="O8"/>
-      <c r="P8"/>
+        <v>525</v>
+      </c>
       <c r="Q8" s="24" t="n">
         <v>506</v>
       </c>
       <c r="R8" s="9" t="s">
         <v>526</v>
       </c>
-      <c r="S8" s="33" t="b">
+      <c r="S8" s="33" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -19325,30 +19297,18 @@
       <c r="K9" s="35" t="s">
         <v>524</v>
       </c>
-      <c r="L9"/>
-      <c r="M9"/>
-      <c r="N9"/>
-      <c r="O9"/>
-      <c r="P9"/>
       <c r="Q9" s="24" t="n">
         <v>507</v>
       </c>
       <c r="R9" s="9" t="s">
         <v>526</v>
       </c>
-      <c r="S9" s="33" t="b">
+      <c r="S9" s="33" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10"/>
-      <c r="B10"/>
-      <c r="C10"/>
-      <c r="D10"/>
-      <c r="E10"/>
-      <c r="F10"/>
-      <c r="G10"/>
       <c r="H10" s="34" t="s">
         <v>530</v>
       </c>
@@ -19358,15 +19318,6 @@
       <c r="J10" s="31" t="s">
         <v>523</v>
       </c>
-      <c r="K10"/>
-      <c r="L10"/>
-      <c r="M10"/>
-      <c r="N10"/>
-      <c r="O10"/>
-      <c r="P10"/>
-      <c r="Q10"/>
-      <c r="R10"/>
-      <c r="S10"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -19406,14 +19357,14 @@
   <dimension ref="A4:G50"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A37" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A50" activeCellId="1" sqref="E202 A50"/>
+      <selection pane="topLeft" activeCell="A50" activeCellId="0" sqref="A50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" customWidth="true" hidden="false" style="0" width="9.14" collapsed="true" outlineLevel="0"/>
-    <col min="2" max="2" customWidth="true" hidden="false" style="0" width="13.93" collapsed="true" outlineLevel="0"/>
-    <col min="3" max="1025" customWidth="true" hidden="false" style="0" width="9.14" collapsed="true" outlineLevel="0"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="9.14"/>
   </cols>
   <sheetData>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
made changes in entity user objects
</commit_message>
<xml_diff>
--- a/src/test/resources/DataSet/NMCO_ONB.xlsx
+++ b/src/test/resources/DataSet/NMCO_ONB.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="TestData" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3040" uniqueCount="593">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3037" uniqueCount="593">
   <si>
     <t xml:space="preserve">TestCaseName</t>
   </si>
@@ -2376,8 +2376,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A83" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A85" activeCellId="0" sqref="A85"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A200" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A203" activeCellId="0" sqref="A203"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -20187,12 +20187,12 @@
   </sheetPr>
   <dimension ref="A1:U10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="F4" activePane="bottomRight" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="F1" activeCellId="0" sqref="F1"/>
-      <selection pane="bottomLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="F6" activeCellId="0" sqref="F6"/>
+      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="F5" activeCellId="1" sqref="A203 F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -20759,7 +20759,7 @@
   <dimension ref="A4:G50"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A37" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A50" activeCellId="0" sqref="A50"/>
+      <selection pane="topLeft" activeCell="A50" activeCellId="1" sqref="A203 A50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
made chages in product selection feature
</commit_message>
<xml_diff>
--- a/src/test/resources/DataSet/NMCO_ONB.xlsx
+++ b/src/test/resources/DataSet/NMCO_ONB.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="TestData" sheetId="1" state="visible" r:id="rId2"/>
@@ -1938,7 +1938,7 @@
     <numFmt numFmtId="169" formatCode="YYYY\-MM\-DD"/>
     <numFmt numFmtId="170" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
-  <fonts count="17">
+  <fonts count="15">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -2022,23 +2022,11 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color rgb="FF6A8759"/>
-      <name val="JetBrains Mono"/>
-      <family val="3"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF067D17"/>
       <name val="JetBrains Mono"/>
       <family val="3"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF067D17"/>
-      <name val="JetBrains Mono"/>
-      <family val="3"/>
     </font>
     <font>
       <sz val="10"/>
@@ -2137,7 +2125,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="41">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2262,23 +2250,15 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2302,11 +2282,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2389,8 +2369,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J199" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="T201" activeCellId="0" sqref="T201"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J199" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L203" activeCellId="0" sqref="L203"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -20200,7 +20180,7 @@
   </sheetPr>
   <dimension ref="A1:U10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="F4" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="F1" activeCellId="0" sqref="F1"/>
@@ -20402,7 +20382,7 @@
       <c r="L4" s="32" t="s">
         <v>536</v>
       </c>
-      <c r="M4" s="33" t="s">
+      <c r="M4" s="12" t="s">
         <v>537</v>
       </c>
       <c r="N4" s="25" t="s">
@@ -20417,7 +20397,7 @@
       <c r="R4" s="9" t="s">
         <v>539</v>
       </c>
-      <c r="S4" s="34" t="n">
+      <c r="S4" s="33" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -20459,7 +20439,7 @@
       <c r="L5" s="11" t="s">
         <v>543</v>
       </c>
-      <c r="M5" s="33" t="s">
+      <c r="M5" s="12" t="s">
         <v>537</v>
       </c>
       <c r="N5" s="25" t="s">
@@ -20474,7 +20454,7 @@
       <c r="R5" s="9" t="s">
         <v>539</v>
       </c>
-      <c r="S5" s="34" t="n">
+      <c r="S5" s="33" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -20504,7 +20484,7 @@
       <c r="H6" s="9" t="s">
         <v>532</v>
       </c>
-      <c r="I6" s="35" t="s">
+      <c r="I6" s="31" t="s">
         <v>533</v>
       </c>
       <c r="J6" s="9" t="s">
@@ -20513,7 +20493,7 @@
       <c r="L6" s="12" t="s">
         <v>545</v>
       </c>
-      <c r="M6" s="33" t="s">
+      <c r="M6" s="12" t="s">
         <v>537</v>
       </c>
       <c r="N6" s="25" t="s">
@@ -20528,7 +20508,7 @@
       <c r="R6" s="9" t="s">
         <v>539</v>
       </c>
-      <c r="S6" s="34" t="n">
+      <c r="S6" s="33" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -20558,13 +20538,13 @@
       <c r="H7" s="9" t="s">
         <v>532</v>
       </c>
-      <c r="I7" s="35" t="s">
+      <c r="I7" s="31" t="s">
         <v>533</v>
       </c>
       <c r="J7" s="9" t="s">
         <v>534</v>
       </c>
-      <c r="M7" s="33" t="s">
+      <c r="M7" s="12" t="s">
         <v>537</v>
       </c>
       <c r="N7" s="25" t="s">
@@ -20579,7 +20559,7 @@
       <c r="R7" s="9" t="s">
         <v>539</v>
       </c>
-      <c r="S7" s="34" t="n">
+      <c r="S7" s="33" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -20606,16 +20586,16 @@
       <c r="G8" s="1" t="s">
         <v>519</v>
       </c>
-      <c r="H8" s="36" t="s">
+      <c r="H8" s="34" t="s">
         <v>549</v>
       </c>
       <c r="I8" s="12" t="s">
         <v>550</v>
       </c>
-      <c r="J8" s="35" t="s">
+      <c r="J8" s="31" t="s">
         <v>551</v>
       </c>
-      <c r="K8" s="35" t="s">
+      <c r="K8" s="31" t="s">
         <v>552</v>
       </c>
       <c r="L8" s="11" t="s">
@@ -20627,7 +20607,7 @@
       <c r="R8" s="9" t="s">
         <v>554</v>
       </c>
-      <c r="S8" s="34" t="n">
+      <c r="S8" s="33" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -20654,16 +20634,16 @@
       <c r="G9" s="1" t="s">
         <v>519</v>
       </c>
-      <c r="H9" s="36" t="s">
+      <c r="H9" s="34" t="s">
         <v>556</v>
       </c>
       <c r="I9" s="9" t="s">
         <v>557</v>
       </c>
-      <c r="J9" s="35" t="s">
+      <c r="J9" s="31" t="s">
         <v>551</v>
       </c>
-      <c r="K9" s="37" t="s">
+      <c r="K9" s="35" t="s">
         <v>552</v>
       </c>
       <c r="Q9" s="24" t="n">
@@ -20672,19 +20652,19 @@
       <c r="R9" s="9" t="s">
         <v>554</v>
       </c>
-      <c r="S9" s="34" t="n">
+      <c r="S9" s="33" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H10" s="36" t="s">
+      <c r="H10" s="34" t="s">
         <v>558</v>
       </c>
       <c r="I10" s="9" t="s">
         <v>559</v>
       </c>
-      <c r="J10" s="35" t="s">
+      <c r="J10" s="31" t="s">
         <v>551</v>
       </c>
     </row>
@@ -20742,27 +20722,27 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="38" t="s">
+      <c r="B5" s="36" t="s">
         <v>533</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="38" t="s">
+      <c r="B6" s="36" t="s">
         <v>561</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="38" t="s">
+      <c r="B7" s="36" t="s">
         <v>533</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="38" t="s">
+      <c r="B8" s="36" t="s">
         <v>562</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="38" t="s">
+      <c r="B9" s="36" t="s">
         <v>563</v>
       </c>
     </row>
@@ -20772,12 +20752,12 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="38" t="s">
+      <c r="B11" s="36" t="s">
         <v>562</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="38" t="s">
+      <c r="B13" s="36" t="s">
         <v>564</v>
       </c>
     </row>
@@ -20814,10 +20794,10 @@
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="39" t="s">
+      <c r="B25" s="37" t="s">
         <v>571</v>
       </c>
-      <c r="F25" s="39" t="s">
+      <c r="F25" s="37" t="s">
         <v>572</v>
       </c>
     </row>
@@ -20842,7 +20822,7 @@
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B31" s="40" t="s">
+      <c r="B31" s="38" t="s">
         <v>577</v>
       </c>
       <c r="E31" s="0" t="s">
@@ -20850,7 +20830,7 @@
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B32" s="39" t="s">
+      <c r="B32" s="37" t="s">
         <v>579</v>
       </c>
       <c r="E32" s="0" t="s">
@@ -20917,7 +20897,7 @@
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B44" s="39" t="s">
+      <c r="B44" s="37" t="s">
         <v>588</v>
       </c>
       <c r="E44" s="0" t="s">
@@ -20925,7 +20905,7 @@
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B45" s="41" t="s">
+      <c r="B45" s="39" t="s">
         <v>590</v>
       </c>
       <c r="F45" s="0" t="s">
@@ -20933,7 +20913,7 @@
       </c>
     </row>
     <row r="46" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B46" s="42" t="s">
+      <c r="B46" s="40" t="s">
         <v>592</v>
       </c>
     </row>

</xml_diff>

<commit_message>
made hnages in product object class
</commit_message>
<xml_diff>
--- a/src/test/resources/DataSet/NMCO_ONB.xlsx
+++ b/src/test/resources/DataSet/NMCO_ONB.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="TestData" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3053" uniqueCount="597">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3041" uniqueCount="596">
   <si>
     <t xml:space="preserve">TestCaseName</t>
   </si>
@@ -1929,9 +1929,6 @@
   </si>
   <si>
     <t xml:space="preserve">e2e testdata</t>
-  </si>
-  <si>
-    <t>https://artifactory.appzillon.com/artifactory/android-apk/ao/automation/qaDebug-1.0.22-10-03-2022-16:52.apk</t>
   </si>
 </sst>
 </file>
@@ -2388,62 +2385,62 @@
   </sheetPr>
   <dimension ref="A1:AMJ1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A169" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D203" activeCellId="0" sqref="D203"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A203" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E205" activeCellId="0" sqref="E205"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" customWidth="true" hidden="false" style="1" width="32.3" collapsed="true" outlineLevel="0"/>
-    <col min="2" max="2" customWidth="true" hidden="false" style="1" width="14.33" collapsed="true" outlineLevel="0"/>
-    <col min="3" max="3" customWidth="true" hidden="false" style="1" width="4.43" collapsed="true" outlineLevel="0"/>
-    <col min="4" max="4" customWidth="true" hidden="false" style="1" width="7.83" collapsed="true" outlineLevel="0"/>
-    <col min="5" max="6" customWidth="true" hidden="false" style="1" width="11.9" collapsed="true" outlineLevel="0"/>
-    <col min="7" max="8" customWidth="true" hidden="false" style="1" width="15.54" collapsed="true" outlineLevel="0"/>
-    <col min="9" max="9" customWidth="true" hidden="false" style="1" width="17.31" collapsed="true" outlineLevel="0"/>
-    <col min="10" max="10" customWidth="true" hidden="false" style="1" width="16.2" collapsed="true" outlineLevel="0"/>
-    <col min="11" max="11" customWidth="true" hidden="false" style="2" width="22.49" collapsed="true" outlineLevel="0"/>
-    <col min="12" max="12" customWidth="true" hidden="false" style="1" width="22.49" collapsed="true" outlineLevel="0"/>
-    <col min="13" max="13" customWidth="true" hidden="false" style="1" width="17.86" collapsed="true" outlineLevel="0"/>
-    <col min="14" max="14" customWidth="true" hidden="false" style="1" width="16.2" collapsed="true" outlineLevel="0"/>
-    <col min="15" max="15" customWidth="true" hidden="false" style="1" width="15.21" collapsed="true" outlineLevel="0"/>
-    <col min="16" max="16" customWidth="true" hidden="false" style="1" width="13.78" collapsed="true" outlineLevel="0"/>
-    <col min="17" max="17" customWidth="true" hidden="false" style="1" width="13.56" collapsed="true" outlineLevel="0"/>
-    <col min="18" max="18" customWidth="true" hidden="false" style="1" width="24.43" collapsed="true" outlineLevel="0"/>
-    <col min="19" max="19" customWidth="true" hidden="false" style="1" width="20.28" collapsed="true" outlineLevel="0"/>
-    <col min="20" max="20" customWidth="true" hidden="false" style="1" width="14.11" collapsed="true" outlineLevel="0"/>
-    <col min="21" max="21" customWidth="true" hidden="false" style="2" width="19.51" collapsed="true" outlineLevel="0"/>
-    <col min="22" max="22" customWidth="true" hidden="false" style="2" width="21.17" collapsed="true" outlineLevel="0"/>
-    <col min="23" max="23" customWidth="true" hidden="false" style="1" width="14.99" collapsed="true" outlineLevel="0"/>
-    <col min="24" max="25" customWidth="true" hidden="false" style="1" width="19.51" collapsed="true" outlineLevel="0"/>
-    <col min="26" max="26" customWidth="true" hidden="false" style="1" width="24.36" collapsed="true" outlineLevel="0"/>
-    <col min="27" max="27" customWidth="true" hidden="false" style="1" width="13.0" collapsed="true" outlineLevel="0"/>
-    <col min="28" max="28" customWidth="true" hidden="false" style="1" width="18.85" collapsed="true" outlineLevel="0"/>
-    <col min="29" max="29" customWidth="true" hidden="false" style="1" width="19.95" collapsed="true" outlineLevel="0"/>
-    <col min="30" max="31" customWidth="true" hidden="false" style="1" width="21.04" collapsed="true" outlineLevel="0"/>
-    <col min="32" max="32" customWidth="true" hidden="false" style="1" width="22.49" collapsed="true" outlineLevel="0"/>
-    <col min="33" max="33" customWidth="true" hidden="false" style="1" width="20.94" collapsed="true" outlineLevel="0"/>
-    <col min="34" max="34" customWidth="true" hidden="false" style="1" width="20.28" collapsed="true" outlineLevel="0"/>
-    <col min="35" max="35" customWidth="true" hidden="false" style="1" width="21.04" collapsed="true" outlineLevel="0"/>
-    <col min="36" max="37" customWidth="true" hidden="false" style="1" width="19.4" collapsed="true" outlineLevel="0"/>
-    <col min="38" max="38" customWidth="true" hidden="false" style="1" width="18.3" collapsed="true" outlineLevel="0"/>
-    <col min="39" max="39" customWidth="true" hidden="false" style="1" width="19.95" collapsed="true" outlineLevel="0"/>
-    <col min="40" max="40" customWidth="true" hidden="false" style="2" width="20.84" collapsed="true" outlineLevel="0"/>
-    <col min="41" max="41" customWidth="true" hidden="false" style="3" width="32.74" collapsed="true" outlineLevel="0"/>
-    <col min="42" max="42" customWidth="true" hidden="false" style="1" width="22.04" collapsed="true" outlineLevel="0"/>
-    <col min="43" max="43" customWidth="true" hidden="false" style="1" width="8.57" collapsed="true" outlineLevel="0"/>
-    <col min="44" max="44" customWidth="true" hidden="false" style="1" width="20.94" collapsed="true" outlineLevel="0"/>
-    <col min="45" max="45" customWidth="true" hidden="false" style="1" width="15.11" collapsed="true" outlineLevel="0"/>
-    <col min="46" max="46" customWidth="true" hidden="false" style="1" width="19.18" collapsed="true" outlineLevel="0"/>
-    <col min="47" max="47" customWidth="true" hidden="false" style="1" width="16.74" collapsed="true" outlineLevel="0"/>
-    <col min="48" max="48" customWidth="true" hidden="false" style="3" width="14.0" collapsed="true" outlineLevel="0"/>
-    <col min="49" max="49" customWidth="true" hidden="false" style="3" width="16.11" collapsed="true" outlineLevel="0"/>
-    <col min="50" max="50" customWidth="true" hidden="false" style="1" width="12.35" collapsed="true" outlineLevel="0"/>
-    <col min="51" max="52" customWidth="true" hidden="false" style="1" width="17.64" collapsed="true" outlineLevel="0"/>
-    <col min="53" max="53" customWidth="true" hidden="false" style="1" width="18.08" collapsed="true" outlineLevel="0"/>
-    <col min="54" max="54" customWidth="true" hidden="false" style="2" width="18.08" collapsed="true" outlineLevel="0"/>
-    <col min="55" max="990" customWidth="true" hidden="false" style="1" width="8.57" collapsed="true" outlineLevel="0"/>
-    <col min="991" max="1025" customWidth="true" hidden="false" style="4" width="9.14" collapsed="true" outlineLevel="0"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="32.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="14.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="4.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="7.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="1" width="11.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="1" width="15.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="17.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="16.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="2" width="22.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="22.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="17.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="16.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="15.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="13.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="13.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="24.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="1" width="20.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="1" width="14.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="2" width="19.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="2" width="21.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="1" width="14.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="24" style="1" width="19.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="1" width="24.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="1" width="13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="1" width="18.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="1" width="19.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="30" style="1" width="21.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="32" style="1" width="22.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="33" style="1" width="20.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="34" min="34" style="1" width="20.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="35" min="35" style="1" width="21.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="37" min="36" style="1" width="19.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="38" min="38" style="1" width="18.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="39" min="39" style="1" width="19.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="40" min="40" style="2" width="20.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="41" min="41" style="3" width="32.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="42" min="42" style="1" width="22.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="43" min="43" style="1" width="8.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="44" min="44" style="1" width="20.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="45" min="45" style="1" width="15.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="46" min="46" style="1" width="19.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="47" min="47" style="1" width="16.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="48" min="48" style="3" width="14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="49" min="49" style="3" width="16.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="50" min="50" style="1" width="12.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="52" min="51" style="1" width="17.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="53" min="53" style="1" width="18.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="54" min="54" style="2" width="18.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="990" min="55" style="1" width="8.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="991" style="4" width="9.14"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19096,7 +19093,7 @@
         <v>99910</v>
       </c>
     </row>
-    <row r="204" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="204" customFormat="false" ht="96" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A204" s="9" t="s">
         <v>481</v>
       </c>
@@ -19218,8 +19215,11 @@
       <c r="AQ204" s="1" t="s">
         <v>478</v>
       </c>
-    </row>
-    <row r="205" customFormat="false" ht="216.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AR204" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="205" customFormat="false" ht="231" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A205" s="9" t="s">
         <v>481</v>
       </c>
@@ -19342,7 +19342,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="206" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="206" customFormat="false" ht="55.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A206" s="9" t="s">
         <v>481</v>
       </c>
@@ -19464,6 +19464,9 @@
       <c r="AQ206" s="1" t="s">
         <v>73</v>
       </c>
+      <c r="AR206" s="1" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="207" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A207" s="9" t="s">
@@ -19585,7 +19588,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="208" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="208" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A208" s="9" t="s">
         <v>481</v>
       </c>
@@ -19707,7 +19710,9 @@
       <c r="AQ208" s="1" t="s">
         <v>495</v>
       </c>
-      <c r="AR208" s="9"/>
+      <c r="AR208" s="1" t="s">
+        <v>73</v>
+      </c>
       <c r="AS208" s="9"/>
     </row>
     <row r="209" customFormat="false" ht="231" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19832,7 +19837,9 @@
       <c r="AQ209" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="AR209" s="9"/>
+      <c r="AR209" s="1" t="s">
+        <v>70</v>
+      </c>
       <c r="AS209" s="9"/>
     </row>
     <row r="210" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -20199,32 +20206,32 @@
   </sheetPr>
   <dimension ref="A1:U10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="F11" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="F1" activeCellId="0" sqref="F1"/>
-      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
       <selection pane="bottomRight" activeCell="I4" activeCellId="0" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" customWidth="true" hidden="false" style="11" width="12.57" collapsed="true" outlineLevel="0"/>
-    <col min="2" max="2" customWidth="true" hidden="false" style="11" width="5.18" collapsed="true" outlineLevel="0"/>
-    <col min="3" max="4" customWidth="true" hidden="false" style="11" width="9.17" collapsed="true" outlineLevel="0"/>
-    <col min="5" max="5" customWidth="true" hidden="false" style="11" width="19.4" collapsed="true" outlineLevel="0"/>
-    <col min="6" max="6" customWidth="true" hidden="false" style="11" width="20.5" collapsed="true" outlineLevel="0"/>
-    <col min="7" max="7" customWidth="true" hidden="false" style="11" width="15.11" collapsed="true" outlineLevel="0"/>
-    <col min="8" max="8" customWidth="true" hidden="false" style="11" width="9.17" collapsed="true" outlineLevel="0"/>
-    <col min="9" max="9" customWidth="true" hidden="false" style="11" width="18.85" collapsed="true" outlineLevel="0"/>
-    <col min="10" max="10" customWidth="true" hidden="false" style="11" width="9.17" collapsed="true" outlineLevel="0"/>
-    <col min="11" max="11" customWidth="true" hidden="false" style="11" width="17.86" collapsed="true" outlineLevel="0"/>
-    <col min="12" max="13" customWidth="true" hidden="false" style="11" width="14.87" collapsed="true" outlineLevel="0"/>
-    <col min="14" max="14" customWidth="true" hidden="false" style="11" width="19.18" collapsed="true" outlineLevel="0"/>
-    <col min="15" max="15" customWidth="true" hidden="false" style="11" width="26.35" collapsed="true" outlineLevel="0"/>
-    <col min="16" max="17" customWidth="true" hidden="false" style="11" width="9.17" collapsed="true" outlineLevel="0"/>
-    <col min="18" max="18" customWidth="true" hidden="false" style="11" width="29.45" collapsed="true" outlineLevel="0"/>
-    <col min="19" max="1025" customWidth="true" hidden="false" style="11" width="9.17" collapsed="true" outlineLevel="0"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="11" width="12.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="11" width="5.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="11" width="9.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="11" width="19.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="11" width="20.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="11" width="15.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="11" width="9.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="11" width="18.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="11" width="9.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="11" width="17.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="12" style="11" width="14.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="11" width="19.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="11" width="26.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="16" style="11" width="9.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="11" width="29.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="19" style="11" width="9.17"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -20299,28 +20306,21 @@
       <c r="D2" s="24" t="s">
         <v>518</v>
       </c>
-      <c r="E2"/>
-      <c r="F2"/>
       <c r="G2" s="24" t="s">
         <v>519</v>
       </c>
-      <c r="H2"/>
       <c r="I2" s="24" t="s">
         <v>520</v>
       </c>
       <c r="J2" s="25" t="s">
         <v>521</v>
       </c>
-      <c r="K2"/>
-      <c r="L2"/>
-      <c r="M2"/>
       <c r="N2" s="26" t="s">
         <v>522</v>
       </c>
       <c r="O2" s="12" t="s">
         <v>523</v>
       </c>
-      <c r="P2"/>
       <c r="Q2" s="25" t="n">
         <v>500</v>
       </c>
@@ -20344,35 +20344,28 @@
       <c r="D3" s="23" t="s">
         <v>518</v>
       </c>
-      <c r="E3"/>
-      <c r="F3"/>
       <c r="G3" s="23" t="s">
         <v>519</v>
       </c>
-      <c r="H3"/>
       <c r="I3" s="28" t="s">
         <v>526</v>
       </c>
       <c r="J3" s="28" t="s">
         <v>521</v>
       </c>
-      <c r="K3"/>
-      <c r="L3"/>
-      <c r="M3"/>
       <c r="N3" s="26" t="s">
         <v>522</v>
       </c>
       <c r="O3" s="12" t="s">
         <v>523</v>
       </c>
-      <c r="P3"/>
       <c r="Q3" s="25" t="n">
         <v>501</v>
       </c>
       <c r="R3" s="28" t="s">
         <v>524</v>
       </c>
-      <c r="S3" s="29" t="b">
+      <c r="S3" s="29" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -20413,7 +20406,7 @@
         <v>535</v>
       </c>
       <c r="L4" s="33" t="s">
-        <v>596</v>
+        <v>536</v>
       </c>
       <c r="M4" s="12" t="s">
         <v>537</v>
@@ -20424,14 +20417,13 @@
       <c r="O4" s="12" t="s">
         <v>523</v>
       </c>
-      <c r="P4"/>
       <c r="Q4" s="25" t="n">
         <v>502</v>
       </c>
       <c r="R4" s="9" t="s">
         <v>539</v>
       </c>
-      <c r="S4" s="34" t="b">
+      <c r="S4" s="34" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -20482,14 +20474,13 @@
       <c r="O5" s="12" t="s">
         <v>523</v>
       </c>
-      <c r="P5"/>
       <c r="Q5" s="25" t="n">
         <v>503</v>
       </c>
       <c r="R5" s="9" t="s">
         <v>539</v>
       </c>
-      <c r="S5" s="34" t="b">
+      <c r="S5" s="34" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -20525,7 +20516,6 @@
       <c r="J6" s="9" t="s">
         <v>534</v>
       </c>
-      <c r="K6"/>
       <c r="L6" s="12" t="s">
         <v>544</v>
       </c>
@@ -20538,14 +20528,13 @@
       <c r="O6" s="12" t="s">
         <v>523</v>
       </c>
-      <c r="P6"/>
       <c r="Q6" s="25" t="n">
         <v>504</v>
       </c>
       <c r="R6" s="9" t="s">
         <v>539</v>
       </c>
-      <c r="S6" s="34" t="b">
+      <c r="S6" s="34" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -20581,8 +20570,6 @@
       <c r="J7" s="9" t="s">
         <v>534</v>
       </c>
-      <c r="K7"/>
-      <c r="L7"/>
       <c r="M7" s="12" t="s">
         <v>537</v>
       </c>
@@ -20592,14 +20579,13 @@
       <c r="O7" s="12" t="s">
         <v>523</v>
       </c>
-      <c r="P7"/>
       <c r="Q7" s="25" t="n">
         <v>505</v>
       </c>
       <c r="R7" s="9" t="s">
         <v>539</v>
       </c>
-      <c r="S7" s="34" t="b">
+      <c r="S7" s="34" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -20641,17 +20627,13 @@
       <c r="L8" s="11" t="s">
         <v>552</v>
       </c>
-      <c r="M8"/>
-      <c r="N8"/>
-      <c r="O8"/>
-      <c r="P8"/>
       <c r="Q8" s="25" t="n">
         <v>506</v>
       </c>
       <c r="R8" s="9" t="s">
         <v>553</v>
       </c>
-      <c r="S8" s="34" t="b">
+      <c r="S8" s="34" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -20690,30 +20672,18 @@
       <c r="K9" s="36" t="s">
         <v>551</v>
       </c>
-      <c r="L9"/>
-      <c r="M9"/>
-      <c r="N9"/>
-      <c r="O9"/>
-      <c r="P9"/>
       <c r="Q9" s="25" t="n">
         <v>507</v>
       </c>
       <c r="R9" s="9" t="s">
         <v>553</v>
       </c>
-      <c r="S9" s="34" t="b">
+      <c r="S9" s="34" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10"/>
-      <c r="B10"/>
-      <c r="C10"/>
-      <c r="D10"/>
-      <c r="E10"/>
-      <c r="F10"/>
-      <c r="G10"/>
       <c r="H10" s="35" t="s">
         <v>557</v>
       </c>
@@ -20723,15 +20693,6 @@
       <c r="J10" s="32" t="s">
         <v>550</v>
       </c>
-      <c r="K10"/>
-      <c r="L10"/>
-      <c r="M10"/>
-      <c r="N10"/>
-      <c r="O10"/>
-      <c r="P10"/>
-      <c r="Q10"/>
-      <c r="R10"/>
-      <c r="S10"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -20776,9 +20737,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" customWidth="true" hidden="false" style="0" width="9.14" collapsed="true" outlineLevel="0"/>
-    <col min="2" max="2" customWidth="true" hidden="false" style="0" width="13.93" collapsed="true" outlineLevel="0"/>
-    <col min="3" max="1025" customWidth="true" hidden="false" style="0" width="9.14" collapsed="true" outlineLevel="0"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="9.14"/>
   </cols>
   <sheetData>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>